<commit_message>
sensitivity experiments generated (both cases) -> now integrate into main tool! Stability constraint: Added shortage
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="218">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -165,9 +165,15 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
     <t xml:space="preserve">restore_blackouts_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
     <t xml:space="preserve">base_case_with_min_loading</t>
   </si>
   <si>
@@ -264,6 +270,9 @@
     <t xml:space="preserve">display_graphs_solar</t>
   </si>
   <si>
+    <t xml:space="preserve">todo: change names from”display”, as inaccurate</t>
+  </si>
+  <si>
     <t xml:space="preserve">display_graphs_demand</t>
   </si>
   <si>
@@ -558,6 +567,9 @@
     <t xml:space="preserve">pv_file</t>
   </si>
   <si>
+    <t xml:space="preserve">Z_low</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -567,12 +579,18 @@
     <t xml:space="preserve">./inputs/pv_gen_zambia.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">Z_median</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/demand_zambia_median.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">Z_high</t>
+  </si>
+  <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
@@ -658,17 +676,21 @@
   </si>
   <si>
     <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -780,7 +802,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -829,7 +851,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,7 +859,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -845,7 +871,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -859,14 +885,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -952,19 +970,19 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B2:C2 D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.02551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.42857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.29591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1184,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1181,16 +1199,16 @@
   </sheetPr>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="B2:C2 B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,74 +1324,67 @@
       <c r="B13" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C13" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="7" t="n">
         <v>365</v>
@@ -1381,7 +1392,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C21" s="13" t="n">
         <v>43101</v>
@@ -1389,22 +1400,21 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="14" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1418,44 +1428,42 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>69</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,174 +1473,165 @@
       <c r="A32" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
       <c r="B33" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="C33" s="14"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
       <c r="B34" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11"/>
       <c r="B35" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="12"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C37" s="0"/>
-      <c r="D37" s="14"/>
-      <c r="G37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="G37" s="15"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="12"/>
+      <c r="C42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="14"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="12"/>
+      <c r="C48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
+      <c r="C49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>86</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>88</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="12"/>
+      <c r="C54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
@@ -1642,44 +1641,40 @@
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>90</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>91</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="12" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1694,741 +1689,741 @@
   </sheetPr>
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="B2:C2 B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="D1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>94</v>
+      <c r="C2" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="D2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>96</v>
+      <c r="C3" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>98</v>
+      <c r="C4" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="D4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>96</v>
+      <c r="C5" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>101</v>
+      <c r="C6" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>103</v>
+      <c r="C7" s="16" t="s">
+        <v>106</v>
       </c>
       <c r="D7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>105</v>
+      <c r="C8" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="D8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>107</v>
+      <c r="C9" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>109</v>
+      <c r="C10" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>111</v>
+      <c r="C11" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="D11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>113</v>
+      <c r="C12" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>25</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>115</v>
+      <c r="C13" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="D13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>0.023</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>103</v>
+      <c r="C14" s="16" t="s">
+        <v>106</v>
       </c>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>0.33</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>96</v>
+      <c r="C15" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>109</v>
+      <c r="C16" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>96</v>
+      <c r="C17" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>96</v>
+      <c r="C18" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>122</v>
+      <c r="C19" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>113</v>
+      <c r="C20" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>125</v>
+      <c r="C21" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>127</v>
+      <c r="C22" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>127</v>
+      <c r="C23" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="D23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>0.12</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>113</v>
+      <c r="C24" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>96</v>
+      <c r="C25" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>96</v>
+      <c r="C26" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B27" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>96</v>
+      <c r="C27" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>111</v>
+      <c r="C28" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="D28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>600</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>113</v>
+      <c r="C29" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>115</v>
+      <c r="C30" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>103</v>
+      <c r="C31" s="16" t="s">
+        <v>106</v>
       </c>
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>0.98</v>
       </c>
-      <c r="C32" s="15" t="s">
-        <v>96</v>
+      <c r="C32" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>109</v>
+      <c r="C33" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>113</v>
+      <c r="C34" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>107</v>
+      <c r="C36" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="D36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="C37" s="15" t="s">
-        <v>109</v>
+      <c r="C37" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="15" t="s">
-        <v>144</v>
+      <c r="C38" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="D38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>950</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>113</v>
+      <c r="C39" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C40" s="15" t="s">
-        <v>115</v>
+      <c r="C40" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>103</v>
+      <c r="C41" s="16" t="s">
+        <v>106</v>
       </c>
       <c r="D41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>109</v>
+      <c r="C42" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>96</v>
+      <c r="C43" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>151</v>
+      <c r="C44" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>96</v>
+      <c r="C45" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>96</v>
+      <c r="C46" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>800</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>113</v>
+      <c r="C47" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>115</v>
+      <c r="C48" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="D48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>109</v>
+      <c r="C49" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C50" s="15" t="s">
-        <v>96</v>
+      <c r="C50" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B51" s="16" t="n">
+        <v>161</v>
+      </c>
+      <c r="B51" s="17" t="n">
         <v>0.2</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>96</v>
+      <c r="C51" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="C52" s="15" t="s">
-        <v>96</v>
+      <c r="C52" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="D53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B54" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>109</v>
+      <c r="C54" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="D54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>96</v>
+      <c r="C55" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B56" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="C56" s="15" t="s">
-        <v>96</v>
+      <c r="C56" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C57" s="15" t="s">
-        <v>96</v>
+      <c r="C57" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B58" s="7" t="n">
         <v>0.12</v>
       </c>
-      <c r="C58" s="15" t="s">
-        <v>96</v>
+      <c r="C58" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C59" s="15" t="s">
-        <v>96</v>
+      <c r="C59" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="C60" s="15" t="s">
-        <v>96</v>
+      <c r="C60" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D60" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2443,32 +2438,32 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="B2:C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>171</v>
+        <v>173</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>174</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>2</v>
@@ -2482,7 +2477,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>20</v>
@@ -2497,7 +2492,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2512,78 +2507,80 @@
   </sheetPr>
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B2:C2 C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="17" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
-        <v>1</v>
+      <c r="A3" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
-        <v>2</v>
+      <c r="A4" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
-        <v>3</v>
+      <c r="A5" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>183</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2598,16 +2595,16 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="B2:C2 F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="18" min="9" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="9" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,416 +2613,399 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>184</v>
+      <c r="A2" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="B23" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16" s="19" t="s">
+      <c r="B25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B17" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C17" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F17" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G17" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="B19" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D19" s="22" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G19" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="22" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G20" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="B21" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="E21" s="22" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G21" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="20" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="H24" s="20" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="H25" s="21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18" t="s">
-        <v>199</v>
-      </c>
       <c r="B26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Working on stability constraint including dod Working on renewable constraint
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="210">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -558,43 +558,19 @@
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demand_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z_low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/demand_zambia_low.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/pv_gen_zambia.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z_median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/demand_zambia_median.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z_high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/demand_zambia_high.csv</t>
+    <t xml:space="preserve">timeseries_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masbate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/local/RL-INSTITUT/martha.hoffmann/Nextcloud/Masterthesis/ASEP_Test/Example1_Masbate.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atulayan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/local/RL-INSTITUT/martha.hoffmann/Nextcloud/Masterthesis/ASEP_Test/Example2_Atulayan.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -977,11 +953,11 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
@@ -1199,7 +1175,7 @@
   </sheetPr>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2505,20 +2481,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="32.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="19" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,53 +2505,21 @@
       <c r="B2" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2614,66 +2559,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,70 +2626,70 @@
         <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>46</v>
@@ -2770,22 +2715,22 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>164</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>164</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>164</v>
@@ -2796,13 +2741,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>48</v>
@@ -2811,7 +2756,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>48</v>
@@ -2822,13 +2767,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>48</v>
@@ -2837,7 +2782,7 @@
         <v>46</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>48</v>
@@ -2848,22 +2793,22 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>48</v>
@@ -2874,7 +2819,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>164</v>
@@ -2886,21 +2831,21 @@
         <v>164</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>164</v>
@@ -2915,10 +2860,10 @@
         <v>48</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>164</v>
@@ -2929,22 +2874,22 @@
         <v>51</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>46</v>
@@ -2952,54 +2897,54 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renewable constraint not working, new features still completely closed off
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="216">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -561,16 +561,34 @@
     <t xml:space="preserve">timeseries_file</t>
   </si>
   <si>
+    <t xml:space="preserve">title_demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_pv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_wind</t>
+  </si>
+  <si>
     <t xml:space="preserve">Masbate</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/local/RL-INSTITUT/martha.hoffmann/Nextcloud/Masterthesis/ASEP_Test/Example1_Masbate.csv</t>
+    <t xml:space="preserve">./inputs/Example1_Masbate.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SolarPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
   </si>
   <si>
     <t xml:space="preserve">Atulayan</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/local/RL-INSTITUT/martha.hoffmann/Nextcloud/Masterthesis/ASEP_Test/Example2_Atulayan.csv</t>
+    <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -946,19 +964,19 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.02551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="1.88775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.1836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,7 +1178,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1175,16 +1193,16 @@
   </sheetPr>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1668,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1665,17 +1683,17 @@
   </sheetPr>
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2417,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2414,13 +2432,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,7 +2486,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2481,21 +2499,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="32.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="19" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1023" min="19" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,27 +2523,54 @@
       <c r="B2" s="0" t="s">
         <v>177</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2540,16 +2585,16 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="9" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="9" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2559,66 +2604,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,70 +2671,70 @@
         <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>46</v>
@@ -2715,22 +2760,22 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>164</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>164</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>164</v>
@@ -2741,13 +2786,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>48</v>
@@ -2756,7 +2801,7 @@
         <v>46</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>48</v>
@@ -2767,13 +2812,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>48</v>
@@ -2782,7 +2827,7 @@
         <v>46</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>48</v>
@@ -2793,22 +2838,22 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="E21" s="21" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>48</v>
@@ -2819,7 +2864,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>164</v>
@@ -2831,21 +2876,21 @@
         <v>164</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>164</v>
@@ -2860,10 +2905,10 @@
         <v>48</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>164</v>
@@ -2874,22 +2919,22 @@
         <v>51</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>46</v>
@@ -2897,60 +2942,60 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Integrating new experiment structure (simulation parameters, settings and dict) Deleted internal demand profile estimation Deleted internal pv profile estimation
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="217">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -543,7 +543,7 @@
     <t xml:space="preserve">white_noise_demand</t>
   </si>
   <si>
-    <t xml:space="preserve">white_noise_irradiation</t>
+    <t xml:space="preserve">white_noise_pv</t>
   </si>
   <si>
     <t xml:space="preserve">Min</t>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t xml:space="preserve">timeseries_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_time</t>
   </si>
   <si>
     <t xml:space="preserve">title_demand</t>
@@ -964,19 +967,19 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.02551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="1.88775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="2.29591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.1836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,7 +1181,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1193,16 +1196,16 @@
   </sheetPr>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,7 +1671,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1683,17 +1686,17 @@
   </sheetPr>
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,7 +2114,9 @@
       <c r="B35" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="C35" s="16"/>
+      <c r="C35" s="16" t="s">
+        <v>108</v>
+      </c>
       <c r="D35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2417,7 +2422,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2432,13 +2437,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2486,7 +2491,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2499,21 +2504,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1023" min="19" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="32.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,16 +2536,19 @@
       <c r="E2" s="0" t="s">
         <v>180</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>184</v>
@@ -2549,28 +2556,34 @@
       <c r="E3" s="0" t="s">
         <v>185</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>184</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>185</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2585,16 +2598,16 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="18" min="9" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="9" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,66 +2617,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>196</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,70 +2684,70 @@
         <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>46</v>
@@ -2760,48 +2773,48 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>206</v>
+        <v>46</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>206</v>
+        <v>46</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>206</v>
+        <v>46</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>164</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>46</v>
+        <v>207</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>48</v>
@@ -2812,22 +2825,22 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>46</v>
+        <v>207</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>48</v>
@@ -2838,22 +2851,22 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>46</v>
+        <v>207</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="G21" s="21" t="s">
         <v>48</v>
@@ -2864,7 +2877,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>164</v>
@@ -2876,21 +2889,21 @@
         <v>164</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>164</v>
@@ -2905,10 +2918,10 @@
         <v>48</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>164</v>
@@ -2919,22 +2932,22 @@
         <v>51</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>46</v>
@@ -2942,60 +2955,60 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Combination complete: - Wind plant optimization - Excel template, csv input per location - sensitivity analysis with/without base case (currently one experiment too much with base case)
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="242">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -165,30 +165,27 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_case_with_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not working currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include_stability_constraint</t>
+  </si>
+  <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_case_with_min_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not working currently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow_shortage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">setting_batch_capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include_stability_constraint</t>
-  </si>
-  <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t xml:space="preserve">cmdline_option_value</t>
   </si>
   <si>
-    <t xml:space="preserve">1*10**(-1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">debug</t>
   </si>
   <si>
@@ -315,6 +309,9 @@
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
+    <t xml:space="preserve">old</t>
+  </si>
+  <si>
     <t xml:space="preserve">blackout_duration</t>
   </si>
   <si>
@@ -339,7 +336,7 @@
     <t xml:space="preserve">combustion_value_fuel</t>
   </si>
   <si>
-    <t xml:space="preserve">kWh/unit</t>
+    <t xml:space="preserve">kWh/l</t>
   </si>
   <si>
     <t xml:space="preserve">costs_var_unsupplied_load</t>
@@ -375,13 +372,19 @@
     <t xml:space="preserve">genset_cost_investment</t>
   </si>
   <si>
-    <t xml:space="preserve">/unit</t>
+    <t xml:space="preserve">/kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using capex of eu islands input parameters</t>
   </si>
   <si>
     <t xml:space="preserve">genset_cost_opex</t>
   </si>
   <si>
-    <t xml:space="preserve">/unit/a</t>
+    <t xml:space="preserve">/kW/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per kW/a, not operating hours</t>
   </si>
   <si>
     <t xml:space="preserve">genset_cost_var</t>
@@ -390,6 +393,9 @@
     <t xml:space="preserve">genset_efficiency</t>
   </si>
   <si>
+    <t xml:space="preserve">not info from sheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">genset_lifetime</t>
   </si>
   <si>
@@ -456,6 +462,15 @@
     <t xml:space="preserve">price_fuel</t>
   </si>
   <si>
+    <t xml:space="preserve">/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We show prices for Philippines from 15-Oct-2018 to 21-Jan-2019. The average value for Philippines during that period was 0.89 Euro with a minimum of 0.77 Euro on 07-Jan-2019 and a maximum of 1.02 Euro on 15-Oct-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.globalpetrolprices.com/Philippines/gasoline_prices/</t>
+  </si>
+  <si>
     <t xml:space="preserve">project_cost_fix</t>
   </si>
   <si>
@@ -474,9 +489,15 @@
     <t xml:space="preserve">pv_cost_investment</t>
   </si>
   <si>
+    <t xml:space="preserve">/kWp</t>
+  </si>
+  <si>
     <t xml:space="preserve">pv_cost_opex</t>
   </si>
   <si>
+    <t xml:space="preserve">/kWp/a</t>
+  </si>
+  <si>
     <t xml:space="preserve">pv_cost_var</t>
   </si>
   <si>
@@ -498,12 +519,18 @@
     <t xml:space="preserve">storage_capacity_min</t>
   </si>
   <si>
+    <t xml:space="preserve">Max DOD 80%</t>
+  </si>
+  <si>
     <t xml:space="preserve">storage_cost_investment</t>
   </si>
   <si>
     <t xml:space="preserve">storage_cost_opex</t>
   </si>
   <si>
+    <t xml:space="preserve">/kWh/a</t>
+  </si>
+  <si>
     <t xml:space="preserve">storage_cost_var</t>
   </si>
   <si>
@@ -546,6 +573,24 @@
     <t xml:space="preserve">white_noise_pv</t>
   </si>
   <si>
+    <t xml:space="preserve">white_noise_wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_lifetime</t>
+  </si>
+  <si>
     <t xml:space="preserve">Min</t>
   </si>
   <si>
@@ -672,10 +717,40 @@
     <t xml:space="preserve">perform_simulation</t>
   </si>
   <si>
+    <t xml:space="preserve">capacity_pv_kWp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_storage_kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_genset_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peak_demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_with_minimal_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do not use for optimization of generator capacities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_pcc_consumption_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimization currently not supported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_pcc_feedin_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_wind_kW</t>
+  </si>
+  <si>
     <t xml:space="preserve">default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
@@ -799,7 +874,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -882,6 +957,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -967,19 +1046,16 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B29 D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="2.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1257,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1194,18 +1270,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="B29 C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,34 +1405,34 @@
         <v>47</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,119 +1440,121 @@
         <v>53</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="0" t="s">
         <v>55</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="7" t="n">
-        <v>365</v>
+      <c r="C20" s="13" t="n">
+        <v>43101</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="13" t="n">
-        <v>43101</v>
+      <c r="C21" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="C22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="C23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="0"/>
+      <c r="C25" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="7" t="s">
         <v>63</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>48</v>
+      <c r="C27" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="7" t="s">
         <v>66</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <f aca="false">10^-3</f>
+        <v>0.001</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="11"/>
+      <c r="B32" s="0" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="C32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11"/>
       <c r="B33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="14"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11"/>
@@ -1489,189 +1566,180 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="11"/>
-      <c r="B35" s="0" t="s">
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="0"/>
+      <c r="D36" s="15"/>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="0"/>
-      <c r="D37" s="15"/>
-      <c r="G37" s="15"/>
+      <c r="C37" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="D43" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>80</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C49" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C52" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="14"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="0"/>
+      <c r="C55" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="C57" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1684,745 +1752,964 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B29 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="14.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="0"/>
+      <c r="D2" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="0"/>
+      <c r="D3" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="0"/>
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="D6" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="D7" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="0"/>
+      <c r="D8" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="D9" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="D10" s="7" t="n">
         <v>40</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>0.5</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="0"/>
+        <v>113</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>650</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="D12" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="E12" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="7" t="n">
-        <v>25</v>
+        <v>0.01</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="7" t="n">
         <v>0.023</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>0.33</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B16" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B18" s="7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>20</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="0"/>
+        <v>132</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="7" t="n">
         <v>0.12</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D25" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B26" s="7" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D26" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B28" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="7" t="n">
         <v>600</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B30" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D30" s="0"/>
+      <c r="D30" s="7" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" s="0"/>
+        <v>105</v>
+      </c>
+      <c r="D31" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="7" t="n">
         <v>0.98</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>20</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="0"/>
+        <v>111</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B34" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="0"/>
+      <c r="E34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="7" t="n">
         <v>200</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>20</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="0"/>
+        <v>111</v>
+      </c>
+      <c r="D37" s="7" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B38" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B39" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="7" t="n">
         <v>950</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B40" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C40" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="0"/>
+        <v>105</v>
+      </c>
+      <c r="D41" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>20</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="0"/>
+        <v>111</v>
+      </c>
+      <c r="D42" s="7" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B43" s="7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="C43" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B44" s="7" t="n">
+        <v>602</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="C44" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D45" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>0.2</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D46" s="7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B47" s="7" t="n">
+        <v>602</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="7" t="n">
         <v>800</v>
       </c>
-      <c r="C47" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B48" s="7" t="n">
-        <v>0</v>
+        <v>17.2</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="0"/>
+        <v>167</v>
+      </c>
+      <c r="D48" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="0"/>
+        <v>111</v>
+      </c>
+      <c r="D49" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D50" s="7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B51" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="17" t="n">
         <v>0.2</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B52" s="7" t="n">
         <v>0.9</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D52" s="7" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="D53" s="0"/>
+        <v>174</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="B54" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="B55" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D55" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B56" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="C56" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B57" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D57" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B58" s="7" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="7" t="n">
         <v>0.12</v>
       </c>
-      <c r="C58" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="B59" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D59" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B60" s="7" t="n">
         <v>0</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="D60" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="7" t="n">
+        <v>1118</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="7" t="n">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="7" t="n">
+        <v>22.36</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D65" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B66" s="7" t="n">
+        <v>20</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D66" s="7" t="n">
+        <v>0.09</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2437,61 +2724,58 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="B29 D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.22"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B2" s="7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7" t="n">
-        <v>4</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="7" t="n">
-        <v>1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>10</v>
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2504,86 +2788,87 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F4"/>
+  <dimension ref="A2:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="1" sqref="B29 G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="32.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.4897959183673"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>181</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>186</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>186</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="G4" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2596,18 +2881,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="9" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2617,398 +2902,485 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>191</v>
-      </c>
       <c r="B16" s="20" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>210</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="H18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="21" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="C22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="H22" s="22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="I22" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="H27" s="21" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="21" t="s">
+      <c r="C29" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="D29" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="E29" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Combination complete: - Wind plant optimization - Excel template, csv input per location - sensitivity analysis with/without base case (currently one experiment too much with base case) - simulation results for base case
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -165,12 +165,15 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
     <t xml:space="preserve">base_case_with_min_loading</t>
   </si>
   <si>
@@ -181,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">include_stability_constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
@@ -1047,15 +1047,16 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B29 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.9795918367347"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,14 +1274,15 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="B29 C20"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,34 +1407,34 @@
         <v>47</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>46</v>
-      </c>
       <c r="D15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1440,7 +1442,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>54</v>
@@ -1475,7 +1477,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>60</v>
@@ -1503,7 +1505,7 @@
         <v>63</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,7 +1530,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,7 +1583,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,7 +1591,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,7 +1599,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,7 +1607,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1625,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>79</v>
@@ -1634,7 +1636,7 @@
         <v>80</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,7 +1644,7 @@
         <v>81</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1652,7 @@
         <v>82</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,7 +1670,7 @@
         <v>83</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,7 +1678,7 @@
         <v>84</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,7 +1686,7 @@
         <v>85</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1694,7 @@
         <v>86</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,7 +1711,7 @@
         <v>87</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1717,7 +1719,7 @@
         <v>88</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1727,7 @@
         <v>89</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,7 +1735,7 @@
         <v>90</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1755,15 +1757,16 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="B29 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,10 +2728,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="B29 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2791,15 +2797,17 @@
   <dimension ref="A2:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="1" sqref="B29 G15"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,15 +2892,16 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +2975,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>216</v>
@@ -3035,25 +3044,25 @@
         <v>229</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,25 +3070,25 @@
         <v>208</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="F18" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,25 +3174,25 @@
         <v>235</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="D22" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H22" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>236</v>
@@ -3275,16 +3284,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>241</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>241</v>
@@ -3296,7 +3305,7 @@
         <v>241</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,13 +3339,13 @@
         <v>219</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>241</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>241</v>
@@ -3356,13 +3365,13 @@
         <v>220</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>241</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>241</v>
@@ -3374,7 +3383,7 @@
         <v>241</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major changes Integrating new experiment structure (simulation parameters, settings and dict) Deleted internal * demand profile estimation * pv profile estimation * input file * config file -> working on: oem with minimal loading, tests, in code documentation
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="242">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -165,27 +165,27 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_case_with_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not working currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include_stability_constraint</t>
+  </si>
+  <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_case_with_min_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not working currently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow_shortage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include_stability_constraint</t>
-  </si>
-  <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
@@ -261,10 +261,10 @@
     <t xml:space="preserve">setting_save_flows_electricity_mg</t>
   </si>
   <si>
+    <t xml:space="preserve">todo: change names from”display”, as inaccurate</t>
+  </si>
+  <si>
     <t xml:space="preserve">display_graphs_solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">todo: change names from”display”, as inaccurate</t>
   </si>
   <si>
     <t xml:space="preserve">display_graphs_demand</t>
@@ -1046,17 +1046,17 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,7 +1258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1273,16 +1273,16 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,34 +1407,34 @@
         <v>47</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,7 +1442,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>54</v>
@@ -1477,7 +1477,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>60</v>
@@ -1505,7 +1505,7 @@
         <v>63</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,8 +1521,7 @@
         <v>66</v>
       </c>
       <c r="C28" s="7" t="n">
-        <f aca="false">10^-3</f>
-        <v>0.001</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,7 +1529,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,7 +1582,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,7 +1590,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,7 +1598,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1607,7 +1606,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,16 +1618,19 @@
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="0"/>
+      <c r="D42" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,7 +1638,10 @@
         <v>80</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1649,7 @@
         <v>81</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1657,7 @@
         <v>82</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1675,7 @@
         <v>83</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1683,7 @@
         <v>84</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1691,7 @@
         <v>85</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,7 +1699,7 @@
         <v>86</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1716,7 @@
         <v>87</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1719,7 +1724,7 @@
         <v>88</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1732,7 @@
         <v>89</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,13 +1740,13 @@
         <v>90</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1756,17 +1761,17 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,7 +1863,7 @@
         <v>104</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>105</v>
@@ -2712,7 +2717,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2727,13 +2732,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,16 +2777,16 @@
         <v>0</v>
       </c>
       <c r="C3" s="7" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2794,20 +2799,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:H4"/>
+  <dimension ref="A2:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,6 +2835,7 @@
         <v>196</v>
       </c>
       <c r="H2" s="7"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
@@ -2876,7 +2882,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2891,17 +2897,17 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2975,7 +2981,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>216</v>
@@ -3044,25 +3050,25 @@
         <v>229</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="D17" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3070,25 +3076,25 @@
         <v>208</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>48</v>
-      </c>
       <c r="E18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="H18" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,25 +3180,25 @@
         <v>235</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="H22" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="22" t="s">
-        <v>48</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>236</v>
@@ -3284,16 +3290,16 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>241</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E26" s="22" t="s">
         <v>241</v>
@@ -3305,7 +3311,7 @@
         <v>241</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,13 +3345,13 @@
         <v>219</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>241</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>241</v>
@@ -3365,13 +3371,13 @@
         <v>220</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>241</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>241</v>
@@ -3383,13 +3389,13 @@
         <v>241</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
oem works (0.03 gap)
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="242">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1046,17 +1046,17 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,7 +1258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1271,18 +1271,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1515,6 +1515,16 @@
       <c r="C27" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">G27*H27</f>
+        <v>150</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
@@ -1523,6 +1533,16 @@
       <c r="C28" s="7" t="n">
         <v>0.03</v>
       </c>
+      <c r="G28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <f aca="false">G28*H28</f>
+        <v>150</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
@@ -1531,9 +1551,23 @@
       <c r="C29" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="G29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <f aca="false">G29*H29</f>
+        <v>180</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0"/>
+      <c r="I30" s="0" t="n">
+        <f aca="false">SUM(I27:I29)</f>
+        <v>480</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
@@ -1724,7 +1758,7 @@
         <v>88</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1766,7 @@
         <v>89</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,13 +1774,13 @@
         <v>90</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1761,17 +1795,17 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="16" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2751,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2730,15 +2764,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,38 +2789,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="D2" s="7" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2801,18 +2807,18 @@
   </sheetPr>
   <dimension ref="A2:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2882,7 +2888,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2897,17 +2903,17 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
New simulation (ratiogap var), cleaning todos
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -548,15 +548,15 @@
     <t xml:space="preserve">setting_value</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">not working currently</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">not implemented</t>
   </si>
   <si>
@@ -686,25 +686,25 @@
     <t xml:space="preserve">Step</t>
   </si>
   <si>
+    <t xml:space="preserve">Atulayan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SolarPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
     <t xml:space="preserve">Masbate</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/Example1_Masbate.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SolarPV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atulayan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -1205,17 +1205,17 @@
   </sheetPr>
   <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A4:F4 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,7 +1417,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1432,16 +1432,16 @@
   </sheetPr>
   <dimension ref="B1:I129"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="1" sqref="A4:F4 K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="6.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5380,7 +5380,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5395,16 +5395,16 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="A4:F4 C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,7 +5529,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5537,10 +5537,10 @@
         <v>39</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5548,7 +5548,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5556,7 +5556,7 @@
         <v>41</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5564,7 +5564,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>176</v>
@@ -5599,7 +5599,7 @@
         <v>46</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>178</v>
@@ -5627,7 +5627,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5651,7 +5651,7 @@
         <v>51</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,7 +5704,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5712,7 +5712,7 @@
         <v>56</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5720,7 +5720,7 @@
         <v>57</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5728,7 +5728,7 @@
         <v>58</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5749,7 +5749,7 @@
         <v>59</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>176</v>
@@ -5760,7 +5760,7 @@
         <v>60</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>176</v>
@@ -5771,7 +5771,7 @@
         <v>61</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5779,7 +5779,7 @@
         <v>62</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5797,7 +5797,7 @@
         <v>63</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5805,7 +5805,7 @@
         <v>64</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5813,7 +5813,7 @@
         <v>65</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5821,7 +5821,7 @@
         <v>66</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5838,7 +5838,7 @@
         <v>67</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5846,7 +5846,7 @@
         <v>68</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5854,7 +5854,7 @@
         <v>69</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5862,13 +5862,13 @@
         <v>70</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5883,17 +5883,17 @@
   </sheetPr>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="1" sqref="A4:F4 A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.6632653061225"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6643,7 +6643,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -6658,13 +6658,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="A4:F4 D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6692,13 +6692,13 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.25</v>
+        <v>0.025</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -6713,18 +6713,18 @@
   </sheetPr>
   <dimension ref="A2:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6789,12 +6789,11 @@
       <c r="F4" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="G4" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -6809,17 +6808,17 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="A4:F4 D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6962,25 +6961,25 @@
         <v>142</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C17" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="E17" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6988,25 +6987,25 @@
         <v>143</v>
       </c>
       <c r="B18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="C18" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="D18" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="E18" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="F18" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G18" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7092,25 +7091,25 @@
         <v>147</v>
       </c>
       <c r="B22" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>175</v>
-      </c>
       <c r="D22" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I22" s="0" t="s">
         <v>249</v>
@@ -7205,13 +7204,13 @@
         <v>40</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" s="37" t="s">
         <v>251</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>251</v>
@@ -7223,7 +7222,7 @@
         <v>251</v>
       </c>
       <c r="H26" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7257,13 +7256,13 @@
         <v>152</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C28" s="37" t="s">
         <v>251</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>251</v>
@@ -7283,13 +7282,13 @@
         <v>153</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>251</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>251</v>
@@ -7301,13 +7300,13 @@
         <v>251</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Ran a couple of simulations
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="252">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -694,7 +694,13 @@
     <t xml:space="preserve">base_oem</t>
   </si>
   <si>
-    <t xml:space="preserve">offgrid_fixed</t>
+    <t xml:space="preserve">fixed_mominload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed_peak_nominload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed_peak_minload</t>
   </si>
   <si>
     <t xml:space="preserve">base_oem_min_loading</t>
@@ -733,13 +739,7 @@
     <t xml:space="preserve">genset_with_minimal_loading</t>
   </si>
   <si>
-    <t xml:space="preserve">do not use for optimization of generator capacities</t>
-  </si>
-  <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optimization currently not supported</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
@@ -1209,17 +1209,17 @@
   </sheetPr>
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,7 +1414,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1429,16 +1429,16 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1908,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1923,17 +1923,17 @@
   </sheetPr>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.98979591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,7 +2170,7 @@
         <v>127</v>
       </c>
       <c r="B21" s="10" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>103</v>
@@ -2214,7 +2214,7 @@
         <v>133</v>
       </c>
       <c r="B25" s="10" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>103</v>
@@ -2440,7 +2440,7 @@
         <v>159</v>
       </c>
       <c r="B45" s="10" t="n">
-        <v>602</v>
+        <v>10</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>160</v>
@@ -2694,7 +2694,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2707,15 +2707,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2732,10 +2732,38 @@
         <v>189</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2750,18 +2778,18 @@
   </sheetPr>
   <dimension ref="A2:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2858,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2843,17 +2871,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,31 +3019,43 @@
       <c r="H16" s="23" t="s">
         <v>227</v>
       </c>
+      <c r="I16" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,111 +3069,135 @@
         <v>43</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="H18" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="J18" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C19" s="25" t="s">
         <v>221</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>221</v>
       </c>
       <c r="F19" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G19" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>230</v>
-      </c>
       <c r="H19" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J19" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>221</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>221</v>
       </c>
       <c r="F20" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G20" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="G20" s="25" t="s">
-        <v>230</v>
-      </c>
       <c r="H20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J20" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>232</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>230</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>221</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E21" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="G21" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="H21" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="G21" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="H21" s="25" t="s">
+      <c r="I21" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J21" s="25" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>43</v>
@@ -3141,18 +3206,21 @@
         <v>43</v>
       </c>
       <c r="G22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="J22" s="25" t="s">
         <v>45</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>172</v>
@@ -3164,19 +3232,22 @@
         <v>172</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>233</v>
+        <v>172</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>233</v>
+        <v>172</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,16 +3267,19 @@
         <v>172</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>233</v>
+        <v>172</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>233</v>
+        <v>172</v>
       </c>
       <c r="H24" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="J24" s="25" t="s">
         <v>172</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3213,24 +3287,30 @@
         <v>239</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>221</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>221</v>
       </c>
       <c r="F25" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G25" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="G25" s="25" t="s">
-        <v>230</v>
-      </c>
       <c r="H25" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J25" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3245,18 +3325,24 @@
         <v>240</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>43</v>
+        <v>240</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>240</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>240</v>
+        <v>43</v>
       </c>
       <c r="G26" s="25" t="s">
         <v>240</v>
       </c>
       <c r="H26" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="J26" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3282,7 +3368,13 @@
       <c r="G27" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="H27" s="24" t="n">
+      <c r="H27" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="J27" s="24" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -3297,18 +3389,24 @@
         <v>240</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>240</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>240</v>
+        <v>45</v>
       </c>
       <c r="G28" s="25" t="s">
         <v>240</v>
       </c>
       <c r="H28" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="J28" s="25" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3322,26 +3420,32 @@
       <c r="C29" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="D29" s="25" t="s">
-        <v>45</v>
+      <c r="D29" s="24" t="s">
+        <v>240</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="F29" s="24" t="s">
-        <v>240</v>
+      <c r="F29" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="G29" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="J29" s="25" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3356,17 +3460,17 @@
   </sheetPr>
   <dimension ref="B1:I130"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6994,7 +7098,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="37" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C118" s="24" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7036,7 +7140,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="37" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C120" s="24" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7057,7 +7161,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="37" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C121" s="24" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7078,7 +7182,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="37" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C122" s="24" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7099,7 +7203,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="37" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C123" s="24" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7120,7 +7224,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="37" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C124" s="24" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7338,7 +7442,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added structure of sarahs evaluation
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="247">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -157,27 +157,27 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_case_with_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not working currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include_stability_constraint</t>
+  </si>
+  <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_case_with_min_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not working currently</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow_shortage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include_stability_constraint</t>
-  </si>
-  <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
@@ -217,426 +217,429 @@
     <t xml:space="preserve">cmdline_option</t>
   </si>
   <si>
+    <t xml:space="preserve">mipgap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmdline_option_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">! this is standardized currently!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./simulation_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output – files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_lp_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_oemofresults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_csv_flows_storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_csv_flows_electricity_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_graphs_solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_graphs_demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_png_flows_storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_png_flows_electricity_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_meta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_invest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_demand_characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_blackout_characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_annuities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blackout_duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrs/mth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blackout_duration_std_deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blackout_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/mth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blackout_frequency_std_deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combustion_value_fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costs_var_unsupplied_load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand_scaling_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distribution_grid_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distribution_grid_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distribution_grid_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">using capex of eu islands input parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kW/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per kW/a, not operating hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not info from sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_max_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genset_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_electricity_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_extension_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_extension_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/km/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_extension_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_feedin_tariff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maingrid_renewable_share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_share_unsupplied_load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_renewable_share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price_fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We show prices for Philippines from 15-Oct-2018 to 21-Jan-2019. The average value for Philippines during that period was 0.89 Euro with a minimum of 0.77 Euro on 07-Jan-2019 and a maximum of 1.02 Euro on 15-Oct-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.globalpetrolprices.com/Philippines/gasoline_prices/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_cost_fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kWp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kWp/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stability_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_capacity_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_capacity_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max DOD 80%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/kWh/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_Crate_charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_Crate_discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_inflow_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_initial_soc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None of factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_loss_timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_outflow_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wacc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white_noise_demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white_noise_pv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white_noise_wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project_site_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeseries_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_pv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atulayan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SolarPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masbate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/Example1_Masbate.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">ratioGap</t>
   </si>
   <si>
-    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmdline_option_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">debug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">! this is standardized currently!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./simulation_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output – files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_lp_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_oemofresults</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_csv_flows_storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_csv_flows_electricity_mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_graphs_solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_graphs_demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_png_flows_storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_png_flows_electricity_mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_invest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_demand_characteristics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_blackout_characteristics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_annuities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_costs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blackout_duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hrs/mth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blackout_duration_std_deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blackout_frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/mth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blackout_frequency_std_deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combustion_value_fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWh/l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costs_var_unsupplied_load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demand_scaling_factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution_grid_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution_grid_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distribution_grid_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">using capex of eu islands input parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kW/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">per kW/a, not operating hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not info from sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_max_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genset_min_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_electricity_price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_extension_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_extension_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/km/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_extension_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_feedin_tariff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maingrid_renewable_share</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max_share_unsupplied_load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_renewable_share</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pcoupling_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price_fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We show prices for Philippines from 15-Oct-2018 to 21-Jan-2019. The average value for Philippines during that period was 0.89 Euro with a minimum of 0.77 Euro on 07-Jan-2019 and a maximum of 1.02 Euro on 15-Oct-2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.globalpetrolprices.com/Philippines/gasoline_prices/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_cost_fix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_life</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kWp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kWp/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stability_limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_capacity_max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_capacity_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max DOD 80%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/kWh/a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_Crate_charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_Crate_discharge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_inflow_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_initial_soc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None of factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_loss_timestep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_outflow_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wacc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">white_noise_demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">white_noise_pv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">white_noise_wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wind_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Step</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project_site_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeseries_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title_demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title_pv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title_wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atulayan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SolarPV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masbate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/Example1_Masbate.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attribute</t>
   </si>
   <si>
@@ -691,40 +694,22 @@
     <t xml:space="preserve">min_renewable share</t>
   </si>
   <si>
-    <t xml:space="preserve">base_oem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed_mominload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed_peak_nominload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed_peak_minload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_oem_min_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interconnected_buy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interconnected_buysell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem_grid_tied_mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sole_maingrid</t>
+    <t xml:space="preserve">oem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oem_nostab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oem_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oem_min_loading_nostab</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pv_kWp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_storage_kWh</t>
@@ -1219,7 +1204,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,15 +1415,15 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,34 +1548,34 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,7 +1583,7 @@
         <v>50</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>51</v>
@@ -1636,7 +1621,7 @@
         <v>57</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>58</v>
@@ -1664,7 +1649,7 @@
         <v>61</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,7 +1668,7 @@
         <v>65</v>
       </c>
       <c r="C28" s="10" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,7 +1676,7 @@
         <v>66</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1747,7 +1732,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,7 +1740,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,7 +1748,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1756,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1774,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>51</v>
@@ -1800,7 +1785,7 @@
         <v>79</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>51</v>
@@ -1811,7 +1796,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1804,7 @@
         <v>81</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,7 +1822,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1845,7 +1830,7 @@
         <v>83</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,7 +1838,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1846,7 @@
         <v>85</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1863,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1886,7 +1871,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1879,7 @@
         <v>88</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1887,7 @@
         <v>89</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1924,7 +1909,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1932,7 +1917,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.99"/>
   </cols>
   <sheetData>
@@ -2710,12 +2695,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,27 +2719,27 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>135</v>
+        <v>65</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.75</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.05</v>
@@ -2776,20 +2761,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I4"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,6 +2796,9 @@
       <c r="F2" s="0" t="s">
         <v>195</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="19"/>
     </row>
@@ -2833,7 +2821,9 @@
       <c r="F3" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="19" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -2853,6 +2843,55 @@
       </c>
       <c r="F4" s="0" t="s">
         <v>200</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2871,18 +2910,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="4" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,178 +2932,148 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="138" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="F16" s="23" t="s">
         <v>225</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="H16" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>43</v>
@@ -3074,153 +3084,78 @@
       <c r="E18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I21" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>172</v>
@@ -3234,25 +3169,10 @@
       <c r="E23" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="J23" s="25" t="s">
-        <v>235</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>172</v>
@@ -3266,180 +3186,90 @@
       <c r="E24" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="J24" s="25" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="H25" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="J25" s="25" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>240</v>
+        <v>49</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>240</v>
+        <v>49</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="H26" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="J26" s="25" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="G27" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="H27" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="J27" s="24" t="n">
-        <v>0.5</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B28" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>240</v>
-      </c>
       <c r="D28" s="25" t="s">
-        <v>240</v>
+        <v>49</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="J28" s="25" t="s">
-        <v>240</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="J29" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3468,15 +3298,15 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="26" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3488,7 +3318,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3511,10 +3341,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3528,7 +3358,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3539,10 +3369,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="30" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3562,16 +3392,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="31" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -3666,7 +3496,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="24" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3699,7 +3529,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="24" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3732,7 +3562,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="24" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -4004,7 +3834,7 @@
       </c>
       <c r="D24" s="35" t="n">
         <f aca="false">SUM(E24:I24)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B24,settings!B:B, 1, 0)), 0)</f>
@@ -4020,7 +3850,7 @@
       </c>
       <c r="H24" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(HLOOKUP(B24,project_sites!$2:$2, 1, 0)), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B24, case_definitions!A$17:A$29,1, 0)), 0)</f>
@@ -7098,7 +6928,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="37" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C118" s="24" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7119,7 +6949,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C119" s="24" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -7140,7 +6970,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="37" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C120" s="24" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7161,7 +6991,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="37" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C121" s="24" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7182,7 +7012,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="37" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C122" s="24" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7203,7 +7033,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="37" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C123" s="24" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7224,7 +7054,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="37" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C124" s="24" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7245,7 +7075,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="37" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C125" s="24" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7266,7 +7096,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="37" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C126" s="24" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7287,7 +7117,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C127" s="24" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>
@@ -7320,7 +7150,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="37" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C128" s="24" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7353,7 +7183,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="37" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C129" s="24" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7386,7 +7216,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="37" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C130" s="24" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
expenditures shortage add to output
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="259">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -157,21 +157,21 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
     <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
     <t xml:space="preserve">include_stability_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
@@ -610,7 +610,7 @@
     <t xml:space="preserve">title_wind</t>
   </si>
   <si>
-    <t xml:space="preserve">Atulayan</t>
+    <t xml:space="preserve">Atulayan_0</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/Example2_Atulayan.csv</t>
@@ -625,12 +625,18 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">Masbate</t>
+    <t xml:space="preserve">Masbate_0</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/Example1_Masbate.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">Atulayan_0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masbate_0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute</t>
   </si>
   <si>
@@ -688,10 +694,22 @@
     <t xml:space="preserve">base_oem</t>
   </si>
   <si>
+    <t xml:space="preserve">base_oem_2Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_oem_no_stability</t>
+  </si>
+  <si>
     <t xml:space="preserve">offgrid_fixed</t>
   </si>
   <si>
-    <t xml:space="preserve">base_oem_min_loading</t>
+    <t xml:space="preserve">base_oem_min_loading_2Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_oem_min_loading_2Gen_no_stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_oem_min_loading_3Gen_no_stability</t>
   </si>
   <si>
     <t xml:space="preserve">interconnected_buy</t>
@@ -727,9 +745,6 @@
     <t xml:space="preserve">genset_with_minimal_loading</t>
   </si>
   <si>
-    <t xml:space="preserve">do not use for optimization of generator capacities</t>
-  </si>
-  <si>
     <t xml:space="preserve">number_of_equal_generators</t>
   </si>
   <si>
@@ -739,10 +754,10 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optimization currently not supported</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
@@ -1222,10 +1237,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.5255102040816"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,16 +1450,16 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,23 +1584,23 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,7 +1608,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>49</v>
@@ -1631,7 +1646,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>56</v>
@@ -1659,7 +1674,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1693,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="10" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1701,7 @@
         <v>64</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1757,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1765,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,7 +1773,7 @@
         <v>74</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,7 +1781,7 @@
         <v>75</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,7 +1799,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>49</v>
@@ -1795,7 +1810,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>49</v>
@@ -1806,7 +1821,7 @@
         <v>78</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,7 +1829,7 @@
         <v>79</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,7 +1847,7 @@
         <v>80</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,7 +1855,7 @@
         <v>81</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,7 +1863,7 @@
         <v>82</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +1871,7 @@
         <v>83</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,7 +1888,7 @@
         <v>84</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1881,7 +1896,7 @@
         <v>85</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1889,7 +1904,7 @@
         <v>86</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,7 +1912,7 @@
         <v>87</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1918,17 +1933,17 @@
   </sheetPr>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,7 +2450,7 @@
         <v>157</v>
       </c>
       <c r="B45" s="10" t="n">
-        <v>602</v>
+        <v>0</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>158</v>
@@ -2702,15 +2717,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2725,6 +2740,20 @@
       </c>
       <c r="D1" s="0" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -2743,20 +2772,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I4"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,6 +2807,9 @@
       <c r="F2" s="0" t="s">
         <v>193</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>100</v>
+      </c>
       <c r="H2" s="10"/>
       <c r="I2" s="19"/>
     </row>
@@ -2800,7 +2832,9 @@
       <c r="F3" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
@@ -2820,6 +2854,55 @@
       </c>
       <c r="F4" s="0" t="s">
         <v>198</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -2838,18 +2921,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,282 +2941,354 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>210</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="185.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>225</v>
+        <v>227</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="F18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="25" t="s">
+      <c r="J18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H18" s="25" t="s">
-        <v>43</v>
+      <c r="K18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="H19" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="L19" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="H20" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="L20" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H21" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="L21" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>47</v>
-      </c>
       <c r="F22" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G22" s="25" t="s">
         <v>43</v>
@@ -3142,39 +3296,60 @@
       <c r="H22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>233</v>
+      <c r="I22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>235</v>
+        <v>242</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>170</v>
@@ -3186,24 +3361,33 @@
         <v>170</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>238</v>
+        <v>170</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="L24" s="25" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>170</v>
@@ -3218,146 +3402,215 @@
         <v>170</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>238</v>
+      <c r="I25" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="L25" s="25" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="H26" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="L26" s="25" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>241</v>
+        <v>43</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>241</v>
+        <v>43</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>241</v>
+        <v>43</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="L27" s="25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="H28" s="24" t="n">
+        <v>246</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="L28" s="24" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>241</v>
+        <v>43</v>
       </c>
       <c r="D29" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="F29" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>241</v>
-      </c>
       <c r="G29" s="25" t="s">
-        <v>241</v>
+        <v>45</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>241</v>
+        <v>45</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>241</v>
+        <v>45</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>241</v>
+        <v>246</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="L30" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3385,16 +3638,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="26" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3406,7 +3659,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3429,10 +3682,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3446,7 +3699,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3457,10 +3710,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="30" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3480,16 +3733,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="31" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -3584,7 +3837,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="34" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="C14" s="24" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3617,7 +3870,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="24" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3650,7 +3903,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="24" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -4813,7 +5066,7 @@
       </c>
       <c r="D51" s="35" t="n">
         <f aca="false">SUM(E51:I51)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B51,settings!B:B, 1, 0)), 0)</f>
@@ -4829,7 +5082,7 @@
       </c>
       <c r="H51" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(HLOOKUP(B51,project_sites!$2:$2, 1, 0)), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B51, case_definitions!A$17:A$30,1, 0)), 0)</f>
@@ -7016,7 +7269,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="37" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C118" s="24" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7037,7 +7290,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="37" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C119" s="24" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -7058,7 +7311,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="37" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C120" s="24" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7079,7 +7332,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="37" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C121" s="24" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7100,7 +7353,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="37" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C122" s="24" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7121,7 +7374,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="37" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C123" s="24" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7142,7 +7395,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="37" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C124" s="24" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7163,7 +7416,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="37" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C125" s="24" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7184,7 +7437,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="37" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C126" s="24" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7205,7 +7458,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C127" s="24" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>
@@ -7238,7 +7491,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="37" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C128" s="24" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7271,7 +7524,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="37" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C129" s="24" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7304,7 +7557,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="37" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C130" s="24" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
changed stability constraint - POSITIVE shortage
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -1218,17 +1218,17 @@
   </sheetPr>
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,7 +1423,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1438,16 +1438,16 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +1909,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1924,17 +1924,17 @@
   </sheetPr>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.79"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,7 +2695,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2710,13 +2710,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,22 +2735,22 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2765,18 +2765,18 @@
   </sheetPr>
   <dimension ref="A2:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2845,7 +2845,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2860,16 +2860,16 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3599,7 +3599,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3614,17 +3614,17 @@
   </sheetPr>
   <dimension ref="B1:I130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.21"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -7581,7 +7581,7 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:I10"/>
   </mergeCells>
-  <conditionalFormatting sqref="C31:C130 C12:C29">
+  <conditionalFormatting sqref="C31:C130,C12:C29">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -7589,7 +7589,7 @@
       <formula>"missing!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D130 D12:D29">
+  <conditionalFormatting sqref="D31:D130,D12:D29">
     <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
@@ -7609,7 +7609,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
changed stability constraint - POSITIVE shortage -> still need to check added networkx diagramm (basics)
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -157,21 +157,21 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
     <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
     <t xml:space="preserve">include_stability_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">blackout_duration</t>
   </si>
   <si>
-    <t xml:space="preserve">hrs/mth</t>
+    <t xml:space="preserve">hrs</t>
   </si>
   <si>
     <t xml:space="preserve">blackout_duration_std_deviation</t>
@@ -1225,10 +1225,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.3112244897959"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,15 +1439,15 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,23 +1572,23 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,7 +1596,7 @@
         <v>48</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>49</v>
@@ -1634,7 +1634,7 @@
         <v>55</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>56</v>
@@ -1662,7 +1662,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,7 +1737,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1745,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>73</v>
@@ -1756,7 +1756,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +1764,7 @@
         <v>75</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1772,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1790,7 @@
         <v>77</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>49</v>
@@ -1801,7 +1801,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>49</v>
@@ -1812,7 +1812,7 @@
         <v>79</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,7 +1820,7 @@
         <v>80</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,7 +1838,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1846,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
         <v>83</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1862,7 @@
         <v>84</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1879,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1887,7 +1887,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1895,7 @@
         <v>87</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1903,7 @@
         <v>88</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1924,17 +1924,17 @@
   </sheetPr>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,7 +1953,7 @@
         <v>92</v>
       </c>
       <c r="B2" s="10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>93</v>
@@ -1975,7 +1975,7 @@
         <v>96</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>97</v>
@@ -2441,7 +2441,7 @@
         <v>158</v>
       </c>
       <c r="B45" s="10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>159</v>
@@ -2710,13 +2710,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.05</v>
@@ -2763,22 +2763,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="10"/>
+      <c r="I1" s="19"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>189</v>
@@ -2860,16 +2864,16 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,7 +2947,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>215</v>
@@ -3027,28 +3031,28 @@
         <v>233</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>43</v>
@@ -3068,40 +3072,40 @@
         <v>207</v>
       </c>
       <c r="B18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="F18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="K18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>47</v>
-      </c>
       <c r="L18" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M18" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,40 +3236,40 @@
         <v>239</v>
       </c>
       <c r="B22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="G22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="H22" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>47</v>
-      </c>
       <c r="I22" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,10 +3301,10 @@
         <v>243</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L23" s="25" t="s">
         <v>241</v>
@@ -3434,43 +3438,43 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>247</v>
+        <v>43</v>
       </c>
       <c r="M27" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,28 +3523,28 @@
         <v>218</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D29" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>247</v>
-      </c>
       <c r="F29" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>247</v>
@@ -3560,28 +3564,28 @@
         <v>219</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>247</v>
+        <v>45</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J30" s="24" t="s">
         <v>247</v>
@@ -3593,7 +3597,7 @@
         <v>247</v>
       </c>
       <c r="M30" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3621,10 +3625,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.69387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3853,7 +3857,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="24" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3886,7 +3890,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="24" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -7441,7 +7445,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C127" s="24" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>
@@ -7581,7 +7585,7 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:I10"/>
   </mergeCells>
-  <conditionalFormatting sqref="C31:C130,C12:C29">
+  <conditionalFormatting sqref="C30">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"OK"</formula>
     </cfRule>
@@ -7589,21 +7593,8 @@
       <formula>"missing!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31:D130,D12:D29">
+  <conditionalFormatting sqref="D30">
     <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>"missing!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="cellIs" priority="7" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added a few debug messages Corrected computation of sole main grid
!changed stability constraint - POSITIVE shortage -> still need to check
added networkx diagramm (basics)
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="261">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -172,94 +172,91 @@
     <t xml:space="preserve">include_stability_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">setting_pcc_utility_owned</t>
+    <t xml:space="preserve">evaluated_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currently only hourly timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity_all_combinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If TRUE: All possible combinations of sensitivity parameters are analysed. Results in a huge number of experiments, but enables indentifyin interdependencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver_verbose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmdline_option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmdline_option_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">! this is standardized currently!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./simulation_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output – files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_lp_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lp_file_for_only_3_timesteps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will perform whole simulation with only 3 timesteps! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_oemofresults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_csv_flows_storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_to_csv_flows_electricity_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display_graphs_solar</t>
   </si>
   <si>
     <t xml:space="preserve">not implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evaluated_days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currently only hourly timestep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensitivity_all_combinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If TRUE: All possible combinations of sensitivity parameters are analysed. Results in a huge number of experiments, but enables indentifyin interdependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solver_verbose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmdline_option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmdline_option_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">! this is standardized currently!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./simulation_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output – files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_lp_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lp_file_for_only_3_timesteps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This will perform whole simulation with only 3 timesteps! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_oemofresults</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_csv_flows_storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_to_csv_flows_electricity_mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display_graphs_solar</t>
   </si>
   <si>
     <t xml:space="preserve">display_graphs_demand</t>
@@ -807,6 +804,9 @@
   </si>
   <si>
     <t xml:space="preserve">base_case_with_min_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setting_pcc_utility_owned</t>
   </si>
   <si>
     <t xml:space="preserve">lp_file_for_only_3_timesteps </t>
@@ -1225,10 +1225,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.234693877551"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,7 +1436,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
@@ -1445,9 +1445,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,111 +1595,109 @@
       <c r="B17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>49</v>
+      <c r="C17" s="10" t="n">
+        <v>365</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="10" t="n">
-        <v>365</v>
+        <v>49</v>
+      </c>
+      <c r="C18" s="16" t="n">
+        <v>43101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="16" t="n">
-        <v>43101</v>
+      <c r="D19" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="10" t="s">
         <v>53</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="C23" s="10" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>58</v>
+      <c r="C24" s="15" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>45</v>
+      <c r="D25" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="C26" s="10" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14"/>
+      <c r="B29" s="0" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C27" s="10" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
       <c r="B30" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1713,31 +1711,33 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
-      <c r="B32" s="0" t="s">
+      <c r="C32" s="17"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="0"/>
+      <c r="D33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="0"/>
-      <c r="D34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>45</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,45 +1745,45 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="17"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
@@ -1793,7 +1793,7 @@
         <v>45</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,10 +1801,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,22 +1813,22 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="17"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="17"/>
+      <c r="C47" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
@@ -1858,31 +1855,31 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="C51" s="17"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="17"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="0"/>
+      <c r="C53" s="15" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
         <v>86</v>
       </c>
@@ -1895,14 +1892,6 @@
         <v>87</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1930,766 +1919,766 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="B3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="10" t="n">
         <v>6</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>8.8</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>0.1</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>104</v>
-      </c>
-      <c r="B9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="B10" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B11" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>650</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="10" t="n">
         <v>0.33</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" s="10" t="n">
         <v>0.3</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="B20" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="B22" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>129</v>
-      </c>
-      <c r="B23" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0.05</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="10" t="n">
         <v>0.95</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="10" t="n">
         <v>0.89</v>
       </c>
       <c r="C35" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B36" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B37" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B38" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B40" s="10" t="n">
         <v>1000</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="19" t="s">
         <v>153</v>
-      </c>
-      <c r="B41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="10" t="n">
         <v>0.4</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B45" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B46" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47" s="10" t="n">
         <v>0.2</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B48" s="10" t="n">
         <v>602</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="B49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B50" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" s="20" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B53" s="10" t="n">
         <v>0.9</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="C54" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="10" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B58" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B59" s="10" t="n">
         <v>0.09</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B61" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B62" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B63" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B64" s="10" t="n">
         <v>1100</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B65" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B66" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B67" s="10" t="n">
         <v>20</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2716,26 +2705,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -2771,12 +2760,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2785,65 +2774,65 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>194</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>199</v>
       </c>
       <c r="G3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>202</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2865,15 +2854,15 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L24" activeCellId="0" sqref="L24"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,66 +2872,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>203</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2950,85 +2939,85 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>216</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="185.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="D16" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="E16" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="F16" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="G16" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="H16" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="I16" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="J16" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="K16" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="L16" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="M16" s="23" t="s">
         <v>231</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>43</v>
@@ -3069,7 +3058,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>45</v>
@@ -3110,130 +3099,130 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>235</v>
-      </c>
       <c r="C19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M19" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M20" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>221</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>238</v>
-      </c>
       <c r="G21" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M21" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>45</v>
@@ -3260,10 +3249,10 @@
         <v>43</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L22" s="25" t="s">
         <v>45</v>
@@ -3274,166 +3263,166 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="D23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="I23" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="J23" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="K23" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="H23" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="J23" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>242</v>
-      </c>
       <c r="L23" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M24" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M25" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M26" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,40 +3468,40 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M28" s="24" t="n">
         <v>0.5</v>
@@ -3520,7 +3509,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>43</v>
@@ -3547,21 +3536,21 @@
         <v>45</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K29" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M29" s="25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>45</v>
@@ -3588,13 +3577,13 @@
         <v>45</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L30" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M30" s="25" t="s">
         <v>45</v>
@@ -3625,16 +3614,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3646,7 +3635,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3669,10 +3658,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="27"/>
       <c r="C5" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3686,7 +3675,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3697,10 +3686,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>254</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3720,16 +3709,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="D10" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="E10" s="31" t="s">
         <v>257</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>258</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
@@ -3824,7 +3813,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" s="24" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3923,19 +3912,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="34" t="s">
-        <v>48</v>
+        <v>259</v>
       </c>
       <c r="C17" s="24" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
-        <v>OK</v>
+        <v>missing!</v>
       </c>
       <c r="D17" s="35" t="n">
         <f aca="false">SUM(E17:I17)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B17,settings!B:B, 1, 0)), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="36" t="n">
         <f aca="false">IFERROR(ISTEXT(VLOOKUP(B17, input_constant!A:A, 1, 0)), 0)</f>
@@ -3956,7 +3945,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="24" t="str">
         <f aca="false">IF(D18&gt;=1, "OK", "missing!")</f>
@@ -3989,7 +3978,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="24" t="str">
         <f aca="false">IF(D19&gt;=1, "OK", "missing!")</f>
@@ -4022,7 +4011,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="24" t="str">
         <f aca="false">IF(D20&gt;=1, "OK", "missing!")</f>
@@ -4055,7 +4044,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="24" t="str">
         <f aca="false">IF(D21&gt;=1, "OK", "missing!")</f>
@@ -4088,7 +4077,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="24" t="str">
         <f aca="false">IF(D22&gt;=1, "OK", "missing!")</f>
@@ -4121,7 +4110,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C23" s="24" t="str">
         <f aca="false">IF(D23&gt;=1, "OK", "missing!")</f>
@@ -4154,7 +4143,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" s="24" t="str">
         <f aca="false">IF(D24&gt;=1, "OK", "missing!")</f>
@@ -4187,7 +4176,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" s="24" t="str">
         <f aca="false">IF(D25&gt;=1, "OK", "missing!")</f>
@@ -4220,7 +4209,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="24" t="str">
         <f aca="false">IF(D26&gt;=1, "OK", "missing!")</f>
@@ -4253,7 +4242,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" s="24" t="str">
         <f aca="false">IF(D27&gt;=1, "OK", "missing!")</f>
@@ -4286,7 +4275,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" s="24" t="str">
         <f aca="false">IF(D28&gt;=1, "OK", "missing!")</f>
@@ -4319,7 +4308,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="24" t="str">
         <f aca="false">IF(D29&gt;=1, "OK", "missing!")</f>
@@ -4385,7 +4374,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="24" t="str">
         <f aca="false">IF(D31&gt;=1, "OK", "missing!")</f>
@@ -4418,7 +4407,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" s="24" t="str">
         <f aca="false">IF(D32&gt;=1, "OK", "missing!")</f>
@@ -4451,7 +4440,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" s="24" t="str">
         <f aca="false">IF(D33&gt;=1, "OK", "missing!")</f>
@@ -4484,7 +4473,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="24" t="str">
         <f aca="false">IF(D34&gt;=1, "OK", "missing!")</f>
@@ -4517,7 +4506,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35" s="24" t="str">
         <f aca="false">IF(D35&gt;=1, "OK", "missing!")</f>
@@ -4550,7 +4539,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="24" t="str">
         <f aca="false">IF(D36&gt;=1, "OK", "missing!")</f>
@@ -4583,7 +4572,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="24" t="str">
         <f aca="false">IF(D37&gt;=1, "OK", "missing!")</f>
@@ -4616,7 +4605,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="24" t="str">
         <f aca="false">IF(D38&gt;=1, "OK", "missing!")</f>
@@ -4649,7 +4638,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="24" t="str">
         <f aca="false">IF(D39&gt;=1, "OK", "missing!")</f>
@@ -4682,7 +4671,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" s="24" t="str">
         <f aca="false">IF(D40&gt;=1, "OK", "missing!")</f>
@@ -4715,7 +4704,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" s="24" t="str">
         <f aca="false">IF(D41&gt;=1, "OK", "missing!")</f>
@@ -4748,7 +4737,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="24" t="str">
         <f aca="false">IF(D42&gt;=1, "OK", "missing!")</f>
@@ -4781,7 +4770,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" s="24" t="str">
         <f aca="false">IF(D43&gt;=1, "OK", "missing!")</f>
@@ -4814,7 +4803,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="24" t="str">
         <f aca="false">IF(D44&gt;=1, "OK", "missing!")</f>
@@ -4847,7 +4836,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="24" t="str">
         <f aca="false">IF(D45&gt;=1, "OK", "missing!")</f>
@@ -4880,7 +4869,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="24" t="str">
         <f aca="false">IF(D46&gt;=1, "OK", "missing!")</f>
@@ -4913,7 +4902,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="24" t="str">
         <f aca="false">IF(D47&gt;=1, "OK", "missing!")</f>
@@ -4946,7 +4935,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" s="24" t="str">
         <f aca="false">IF(D48&gt;=1, "OK", "missing!")</f>
@@ -4979,7 +4968,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C49" s="24" t="str">
         <f aca="false">IF(D49&gt;=1, "OK", "missing!")</f>
@@ -5012,7 +5001,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" s="24" t="str">
         <f aca="false">IF(D50&gt;=1, "OK", "missing!")</f>
@@ -5045,7 +5034,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="24" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5078,7 +5067,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C52" s="24" t="str">
         <f aca="false">IF(D52&gt;=1, "OK", "missing!")</f>
@@ -5111,7 +5100,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="24" t="str">
         <f aca="false">IF(D53&gt;=1, "OK", "missing!")</f>
@@ -5144,7 +5133,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54" s="24" t="str">
         <f aca="false">IF(D54&gt;=1, "OK", "missing!")</f>
@@ -5177,7 +5166,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55" s="24" t="str">
         <f aca="false">IF(D55&gt;=1, "OK", "missing!")</f>
@@ -5210,7 +5199,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C56" s="24" t="str">
         <f aca="false">IF(D56&gt;=1, "OK", "missing!")</f>
@@ -5243,7 +5232,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" s="24" t="str">
         <f aca="false">IF(D57&gt;=1, "OK", "missing!")</f>
@@ -5276,7 +5265,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C58" s="24" t="str">
         <f aca="false">IF(D58&gt;=1, "OK", "missing!")</f>
@@ -5309,7 +5298,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C59" s="24" t="str">
         <f aca="false">IF(D59&gt;=1, "OK", "missing!")</f>
@@ -5342,7 +5331,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C60" s="24" t="str">
         <f aca="false">IF(D60&gt;=1, "OK", "missing!")</f>
@@ -5375,7 +5364,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C61" s="24" t="str">
         <f aca="false">IF(D61&gt;=1, "OK", "missing!")</f>
@@ -5408,7 +5397,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C62" s="24" t="str">
         <f aca="false">IF(D62&gt;=1, "OK", "missing!")</f>
@@ -5441,7 +5430,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C63" s="24" t="str">
         <f aca="false">IF(D63&gt;=1, "OK", "missing!")</f>
@@ -5474,7 +5463,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" s="24" t="str">
         <f aca="false">IF(D64&gt;=1, "OK", "missing!")</f>
@@ -5507,7 +5496,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C65" s="24" t="str">
         <f aca="false">IF(D65&gt;=1, "OK", "missing!")</f>
@@ -5540,7 +5529,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C66" s="24" t="str">
         <f aca="false">IF(D66&gt;=1, "OK", "missing!")</f>
@@ -5573,7 +5562,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C67" s="24" t="str">
         <f aca="false">IF(D67&gt;=1, "OK", "missing!")</f>
@@ -5606,7 +5595,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C68" s="24" t="str">
         <f aca="false">IF(D68&gt;=1, "OK", "missing!")</f>
@@ -5639,7 +5628,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C69" s="24" t="str">
         <f aca="false">IF(D69&gt;=1, "OK", "missing!")</f>
@@ -5672,7 +5661,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C70" s="24" t="str">
         <f aca="false">IF(D70&gt;=1, "OK", "missing!")</f>
@@ -5705,7 +5694,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C71" s="24" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -5738,7 +5727,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C72" s="24" t="str">
         <f aca="false">IF(D72&gt;=1, "OK", "missing!")</f>
@@ -5771,7 +5760,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C73" s="24" t="str">
         <f aca="false">IF(D73&gt;=1, "OK", "missing!")</f>
@@ -5804,7 +5793,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C74" s="24" t="str">
         <f aca="false">IF(D74&gt;=1, "OK", "missing!")</f>
@@ -5837,7 +5826,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C75" s="24" t="str">
         <f aca="false">IF(D75&gt;=1, "OK", "missing!")</f>
@@ -5870,7 +5859,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C76" s="24" t="str">
         <f aca="false">IF(D76&gt;=1, "OK", "missing!")</f>
@@ -5903,7 +5892,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C77" s="24" t="str">
         <f aca="false">IF(D77&gt;=1, "OK", "missing!")</f>
@@ -5936,7 +5925,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C78" s="24" t="str">
         <f aca="false">IF(D78&gt;=1, "OK", "missing!")</f>
@@ -5969,7 +5958,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C79" s="24" t="str">
         <f aca="false">IF(D79&gt;=1, "OK", "missing!")</f>
@@ -6002,7 +5991,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C80" s="24" t="str">
         <f aca="false">IF(D80&gt;=1, "OK", "missing!")</f>
@@ -6035,7 +6024,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C81" s="24" t="str">
         <f aca="false">IF(D81&gt;=1, "OK", "missing!")</f>
@@ -6068,7 +6057,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C82" s="24" t="str">
         <f aca="false">IF(D82&gt;=1, "OK", "missing!")</f>
@@ -6101,7 +6090,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C83" s="24" t="str">
         <f aca="false">IF(D83&gt;=1, "OK", "missing!")</f>
@@ -6134,7 +6123,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C84" s="24" t="str">
         <f aca="false">IF(D84&gt;=1, "OK", "missing!")</f>
@@ -6167,7 +6156,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C85" s="24" t="str">
         <f aca="false">IF(D85&gt;=1, "OK", "missing!")</f>
@@ -6200,7 +6189,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C86" s="24" t="str">
         <f aca="false">IF(D86&gt;=1, "OK", "missing!")</f>
@@ -6233,7 +6222,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C87" s="24" t="str">
         <f aca="false">IF(D87&gt;=1, "OK", "missing!")</f>
@@ -6266,7 +6255,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C88" s="24" t="str">
         <f aca="false">IF(D88&gt;=1, "OK", "missing!")</f>
@@ -6299,7 +6288,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C89" s="24" t="str">
         <f aca="false">IF(D89&gt;=1, "OK", "missing!")</f>
@@ -6332,7 +6321,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C90" s="24" t="str">
         <f aca="false">IF(D90&gt;=1, "OK", "missing!")</f>
@@ -6365,7 +6354,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C91" s="24" t="str">
         <f aca="false">IF(D91&gt;=1, "OK", "missing!")</f>
@@ -6398,7 +6387,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C92" s="24" t="str">
         <f aca="false">IF(D92&gt;=1, "OK", "missing!")</f>
@@ -6431,7 +6420,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C93" s="24" t="str">
         <f aca="false">IF(D93&gt;=1, "OK", "missing!")</f>
@@ -6464,7 +6453,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C94" s="24" t="str">
         <f aca="false">IF(D94&gt;=1, "OK", "missing!")</f>
@@ -6497,7 +6486,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C95" s="24" t="str">
         <f aca="false">IF(D95&gt;=1, "OK", "missing!")</f>
@@ -6530,7 +6519,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C96" s="24" t="str">
         <f aca="false">IF(D96&gt;=1, "OK", "missing!")</f>
@@ -6563,7 +6552,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C97" s="24" t="str">
         <f aca="false">IF(D97&gt;=1, "OK", "missing!")</f>
@@ -6596,7 +6585,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C98" s="24" t="str">
         <f aca="false">IF(D98&gt;=1, "OK", "missing!")</f>
@@ -6629,7 +6618,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C99" s="24" t="str">
         <f aca="false">IF(D99&gt;=1, "OK", "missing!")</f>
@@ -6662,7 +6651,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C100" s="24" t="str">
         <f aca="false">IF(D100&gt;=1, "OK", "missing!")</f>
@@ -6695,7 +6684,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C101" s="24" t="str">
         <f aca="false">IF(D101&gt;=1, "OK", "missing!")</f>
@@ -6728,7 +6717,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C102" s="24" t="str">
         <f aca="false">IF(D102&gt;=1, "OK", "missing!")</f>
@@ -6761,7 +6750,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C103" s="24" t="str">
         <f aca="false">IF(D103&gt;=1, "OK", "missing!")</f>
@@ -6794,7 +6783,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C104" s="24" t="str">
         <f aca="false">IF(D104&gt;=1, "OK", "missing!")</f>
@@ -6827,7 +6816,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C105" s="24" t="str">
         <f aca="false">IF(D105&gt;=1, "OK", "missing!")</f>
@@ -6860,7 +6849,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C106" s="24" t="str">
         <f aca="false">IF(D106&gt;=1, "OK", "missing!")</f>
@@ -6893,7 +6882,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C107" s="24" t="str">
         <f aca="false">IF(D107&gt;=1, "OK", "missing!")</f>
@@ -6926,7 +6915,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C108" s="24" t="str">
         <f aca="false">IF(D108&gt;=1, "OK", "missing!")</f>
@@ -6959,7 +6948,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C109" s="24" t="str">
         <f aca="false">IF(D109&gt;=1, "OK", "missing!")</f>
@@ -6992,7 +6981,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C110" s="24" t="str">
         <f aca="false">IF(D110&gt;=1, "OK", "missing!")</f>
@@ -7025,7 +7014,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C111" s="24" t="str">
         <f aca="false">IF(D111&gt;=1, "OK", "missing!")</f>
@@ -7058,7 +7047,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C112" s="24" t="str">
         <f aca="false">IF(D112&gt;=1, "OK", "missing!")</f>
@@ -7091,7 +7080,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C113" s="24" t="str">
         <f aca="false">IF(D113&gt;=1, "OK", "missing!")</f>
@@ -7124,7 +7113,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C114" s="24" t="str">
         <f aca="false">IF(D114&gt;=1, "OK", "missing!")</f>
@@ -7157,7 +7146,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C115" s="24" t="str">
         <f aca="false">IF(D115&gt;=1, "OK", "missing!")</f>
@@ -7190,7 +7179,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C116" s="24" t="str">
         <f aca="false">IF(D116&gt;=1, "OK", "missing!")</f>
@@ -7223,7 +7212,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C117" s="24" t="str">
         <f aca="false">IF(D117&gt;=1, "OK", "missing!")</f>
@@ -7256,7 +7245,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="37" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C118" s="24" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7277,7 +7266,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C119" s="24" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -7298,7 +7287,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C120" s="24" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7319,7 +7308,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="37" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C121" s="24" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7340,7 +7329,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="37" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C122" s="24" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7361,7 +7350,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C123" s="24" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7382,7 +7371,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C124" s="24" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7403,7 +7392,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C125" s="24" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7424,7 +7413,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C126" s="24" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7478,7 +7467,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="37" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C128" s="24" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7511,7 +7500,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C129" s="24" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7544,7 +7533,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C130" s="24" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Added script to catch renewables ninjas timeseries Includes timeseries of all 10 locations in the philippines Added / edited to stability criterion backup/usage
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="268">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -157,93 +157,93 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evaluated_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time_frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currently only hourly timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sensitivity_all_combinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If TRUE: All possible combinations of sensitivity parameters are analysed. Results in a huge number of experiments, but enables indentifyin interdependencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver_verbose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmdline_option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmdline_option_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">! this is standardized currently!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./simulation_results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output – files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_lp_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lp_file_for_only_3_timesteps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will perform whole simulation with only 3 timesteps! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">save_oemofresults</t>
+  </si>
+  <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow_shortage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evaluated_days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_frequency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currently only hourly timestep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensitivity_all_combinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If TRUE: All possible combinations of sensitivity parameters are analysed. Results in a huge number of experiments, but enables indentifyin interdependencies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solver_verbose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmdline_option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ratioGap, mipgap, AllowedGap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmdline_option_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">! this is standardized currently!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./simulation_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output – files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_lp_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lp_file_for_only_3_timesteps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This will perform whole simulation with only 3 timesteps! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">save_oemofresults</t>
-  </si>
-  <si>
     <t xml:space="preserve">save_to_csv_flows_storage</t>
   </si>
   <si>
@@ -727,19 +727,13 @@
     <t xml:space="preserve">renewable_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">oem_backup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem_usage_wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem_usage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem_min_loading_backup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oem_min_loading_usage</t>
+    <t xml:space="preserve">diesel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solarhybrid_backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solarhybrid_usage</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -766,9 +760,6 @@
     <t xml:space="preserve">number_of_equal_generators</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
@@ -784,10 +775,10 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
+    <t xml:space="preserve">share_usage</t>
+  </si>
+  <si>
     <t xml:space="preserve">share_backup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">share_usage</t>
   </si>
   <si>
     <t xml:space="preserve">Data Sufficiency Check</t>
@@ -1632,20 +1623,20 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>365</v>
@@ -1653,7 +1644,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="16" t="n">
         <v>43101</v>
@@ -1661,24 +1652,24 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,34 +1683,34 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>0.03</v>
@@ -1737,29 +1728,29 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14"/>
       <c r="B28" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
       <c r="B29" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
       <c r="B30" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1767,7 +1758,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" s="0"/>
       <c r="D32" s="18"/>
@@ -1775,29 +1766,29 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>71</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,7 +1796,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1804,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,7 +1822,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>75</v>
@@ -1842,7 +1833,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>75</v>
@@ -1853,7 +1844,7 @@
         <v>77</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +1852,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1870,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,7 +1878,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1886,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1894,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,7 +1911,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1928,7 +1919,7 @@
         <v>84</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,7 +1927,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1935,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1965,8 +1956,8 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1994,7 +1985,7 @@
         <v>90</v>
       </c>
       <c r="B2" s="10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>91</v>
@@ -2016,7 +2007,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>95</v>
@@ -2443,7 +2434,7 @@
         <v>151</v>
       </c>
       <c r="B42" s="10" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>93</v>
@@ -2512,7 +2503,7 @@
         <v>159</v>
       </c>
       <c r="B48" s="10" t="n">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>115</v>
@@ -2746,7 +2737,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3057,10 +3048,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3143,7 +3134,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>227</v>
@@ -3173,7 +3164,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
         <v>217</v>
       </c>
@@ -3186,16 +3177,10 @@
       <c r="D15" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>237</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>43</v>
@@ -3205,12 +3190,6 @@
       </c>
       <c r="D16" s="25" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,124 +3197,88 @@
         <v>219</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>240</v>
+        <v>43</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>240</v>
+        <v>43</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>247</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>167</v>
@@ -3346,16 +3289,10 @@
       <c r="D23" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>167</v>
@@ -3366,51 +3303,33 @@
       <c r="D24" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="E24" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>167</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,39 +3337,27 @@
         <v>228</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>252</v>
+      <c r="B28" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="F28" s="26" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,19 +3365,13 @@
         <v>232</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3507,7 +3408,7 @@
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3519,7 +3420,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3542,10 +3443,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3559,7 +3460,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3570,10 +3471,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3593,16 +3494,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="E10" s="32" t="s">
         <v>261</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>264</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3697,7 +3598,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C14" s="26" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3730,7 +3631,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="26" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3763,7 +3664,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C16" s="26" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3796,7 +3697,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C17" s="26" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3829,7 +3730,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="26" t="str">
         <f aca="false">IF(D18&gt;=1, "OK", "missing!")</f>
@@ -3862,7 +3763,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="26" t="str">
         <f aca="false">IF(D19&gt;=1, "OK", "missing!")</f>
@@ -3895,7 +3796,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="26" t="str">
         <f aca="false">IF(D20&gt;=1, "OK", "missing!")</f>
@@ -3928,7 +3829,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="26" t="str">
         <f aca="false">IF(D21&gt;=1, "OK", "missing!")</f>
@@ -3961,7 +3862,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="26" t="str">
         <f aca="false">IF(D22&gt;=1, "OK", "missing!")</f>
@@ -3994,7 +3895,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="26" t="str">
         <f aca="false">IF(D23&gt;=1, "OK", "missing!")</f>
@@ -4027,7 +3928,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="26" t="str">
         <f aca="false">IF(D24&gt;=1, "OK", "missing!")</f>
@@ -4060,7 +3961,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="26" t="str">
         <f aca="false">IF(D25&gt;=1, "OK", "missing!")</f>
@@ -4093,7 +3994,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="26" t="str">
         <f aca="false">IF(D26&gt;=1, "OK", "missing!")</f>
@@ -4126,7 +4027,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="26" t="str">
         <f aca="false">IF(D27&gt;=1, "OK", "missing!")</f>
@@ -4159,7 +4060,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="26" t="str">
         <f aca="false">IF(D28&gt;=1, "OK", "missing!")</f>
@@ -4192,7 +4093,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="26" t="str">
         <f aca="false">IF(D29&gt;=1, "OK", "missing!")</f>
@@ -4225,7 +4126,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C30" s="26" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4258,7 +4159,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="26" t="str">
         <f aca="false">IF(D31&gt;=1, "OK", "missing!")</f>
@@ -4918,7 +4819,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C51" s="26" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5578,7 +5479,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C71" s="26" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -7129,7 +7030,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="38" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C118" s="26" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7171,7 +7072,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C120" s="26" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7192,7 +7093,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C121" s="26" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7213,7 +7114,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C122" s="26" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7234,7 +7135,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C123" s="26" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7255,7 +7156,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="38" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C124" s="26" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7276,7 +7177,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="38" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C125" s="26" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7297,7 +7198,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="38" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C126" s="26" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7318,7 +7219,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C127" s="26" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Workaround script for local time @ renewables ninjas Most recent input template added script to evaluate results
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="269">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -157,12 +157,15 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
     <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
@@ -241,9 +244,6 @@
     <t xml:space="preserve">save_oemofresults</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">save_to_csv_flows_storage</t>
   </si>
   <si>
@@ -734,6 +734,9 @@
   </si>
   <si>
     <t xml:space="preserve">solarhybrid_usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solarhybrid_usage_no_min_load</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -844,7 +847,7 @@
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -879,11 +882,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1088,11 +1086,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1112,7 +1110,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1124,7 +1122,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1148,11 +1146,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,7 +1158,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1180,7 +1178,6 @@
         <charset val="1"/>
         <family val="2"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1188,7 +1185,6 @@
         <charset val="1"/>
         <family val="2"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
@@ -1196,7 +1192,6 @@
         <charset val="1"/>
         <family val="2"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1269,17 +1264,17 @@
   </sheetPr>
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,7 +1469,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1489,16 +1484,16 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R45" activeCellId="0" sqref="R45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,20 +1618,20 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>365</v>
@@ -1644,7 +1639,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="16" t="n">
         <v>43101</v>
@@ -1652,24 +1647,24 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,34 +1678,34 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>0.03</v>
@@ -1728,29 +1723,29 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14"/>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,7 +1753,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="0"/>
       <c r="D32" s="18"/>
@@ -1766,29 +1761,29 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +1791,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1799,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1817,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>75</v>
@@ -1833,7 +1828,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>75</v>
@@ -1844,7 +1839,7 @@
         <v>77</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1847,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1865,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1873,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +1881,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,7 +1889,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +1906,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1919,7 +1914,7 @@
         <v>84</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +1922,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,13 +1930,13 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1956,17 +1951,17 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,7 +2716,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2736,13 +2731,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2776,7 +2771,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2791,18 +2786,17 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,7 +3029,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3048,19 +3042,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,7 +3128,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>227</v>
@@ -3164,7 +3158,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="139.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
         <v>217</v>
       </c>
@@ -3177,10 +3171,13 @@
       <c r="D15" s="24" t="s">
         <v>235</v>
       </c>
+      <c r="E15" s="24" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>43</v>
@@ -3189,6 +3186,9 @@
         <v>43</v>
       </c>
       <c r="D16" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3197,88 +3197,106 @@
         <v>219</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>238</v>
-      </c>
       <c r="D19" s="25" t="s">
-        <v>238</v>
+        <v>239</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>167</v>
@@ -3289,10 +3307,13 @@
       <c r="D23" s="25" t="s">
         <v>167</v>
       </c>
+      <c r="E23" s="25" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>167</v>
@@ -3303,10 +3324,13 @@
       <c r="D24" s="25" t="s">
         <v>167</v>
       </c>
+      <c r="E24" s="25" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>167</v>
@@ -3317,19 +3341,25 @@
       <c r="D25" s="25" t="s">
         <v>167</v>
       </c>
+      <c r="E25" s="25" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3337,13 +3367,16 @@
         <v>228</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,13 +3384,16 @@
         <v>230</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C28" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="D28" s="26" t="s">
-        <v>249</v>
+      <c r="E28" s="26" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,19 +3401,22 @@
         <v>232</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3392,23 +3431,23 @@
   </sheetPr>
   <dimension ref="B1:I130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3420,7 +3459,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3443,10 +3482,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3460,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3471,10 +3510,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3494,16 +3533,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3598,7 +3637,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C14" s="26" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3631,7 +3670,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="26" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3664,7 +3703,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C16" s="26" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3697,7 +3736,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C17" s="26" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3730,7 +3769,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="26" t="str">
         <f aca="false">IF(D18&gt;=1, "OK", "missing!")</f>
@@ -3763,7 +3802,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="26" t="str">
         <f aca="false">IF(D19&gt;=1, "OK", "missing!")</f>
@@ -3796,7 +3835,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="26" t="str">
         <f aca="false">IF(D20&gt;=1, "OK", "missing!")</f>
@@ -3829,7 +3868,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="26" t="str">
         <f aca="false">IF(D21&gt;=1, "OK", "missing!")</f>
@@ -3862,7 +3901,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="26" t="str">
         <f aca="false">IF(D22&gt;=1, "OK", "missing!")</f>
@@ -3895,7 +3934,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="26" t="str">
         <f aca="false">IF(D23&gt;=1, "OK", "missing!")</f>
@@ -3928,7 +3967,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="26" t="str">
         <f aca="false">IF(D24&gt;=1, "OK", "missing!")</f>
@@ -3961,7 +4000,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="26" t="str">
         <f aca="false">IF(D25&gt;=1, "OK", "missing!")</f>
@@ -3994,7 +4033,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" s="26" t="str">
         <f aca="false">IF(D26&gt;=1, "OK", "missing!")</f>
@@ -4027,7 +4066,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="26" t="str">
         <f aca="false">IF(D27&gt;=1, "OK", "missing!")</f>
@@ -4060,7 +4099,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="26" t="str">
         <f aca="false">IF(D28&gt;=1, "OK", "missing!")</f>
@@ -4093,7 +4132,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C29" s="26" t="str">
         <f aca="false">IF(D29&gt;=1, "OK", "missing!")</f>
@@ -4126,7 +4165,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C30" s="26" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4159,7 +4198,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="26" t="str">
         <f aca="false">IF(D31&gt;=1, "OK", "missing!")</f>
@@ -4819,7 +4858,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C51" s="26" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5479,7 +5518,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C71" s="26" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -7030,7 +7069,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="38" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C118" s="26" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7072,7 +7111,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="38" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C120" s="26" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7093,7 +7132,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="38" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C121" s="26" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7114,7 +7153,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="38" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C122" s="26" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7135,7 +7174,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="38" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C123" s="26" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7156,7 +7195,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="38" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C124" s="26" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7177,7 +7216,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C125" s="26" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7198,7 +7237,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C126" s="26" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7219,7 +7258,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="38" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C127" s="26" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>
@@ -7374,7 +7413,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
get single location from renewables ninjas, potentially implementable in tool included external blackout timeseries from csv -> not saved in blackout.csv file! grid availability displayed in graph
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="251">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -157,12 +157,15 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
     <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
@@ -241,9 +244,6 @@
     <t xml:space="preserve">save_oemofresults</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
     <t xml:space="preserve">save_to_csv_flows_storage</t>
   </si>
   <si>
@@ -604,7 +604,7 @@
     <t xml:space="preserve">title_grid_availability</t>
   </si>
   <si>
-    <t xml:space="preserve">consumer_tier2</t>
+    <t xml:space="preserve">gridavailability_from_file</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/timeseries/intermediate_tier2.csv</t>
@@ -622,7 +622,7 @@
     <t xml:space="preserve">GridAvailability</t>
   </si>
   <si>
-    <t xml:space="preserve">consumer_tier2_b</t>
+    <t xml:space="preserve">gridavailability_internal_randomized</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -679,6 +679,9 @@
     <t xml:space="preserve">renewable_constraint</t>
   </si>
   <si>
+    <t xml:space="preserve">shs_backup</t>
+  </si>
+  <si>
     <t xml:space="preserve">solar_backup</t>
   </si>
   <si>
@@ -719,6 +722,9 @@
   </si>
   <si>
     <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.27</t>
   </si>
   <si>
     <t xml:space="preserve">share_usage</t>
@@ -1222,10 +1228,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4540816326531"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,16 +1441,16 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,20 +1575,20 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>365</v>
@@ -1590,7 +1596,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="16" t="n">
         <v>43101</v>
@@ -1598,24 +1604,24 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1629,34 +1635,34 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="10" t="n">
         <v>0.03</v>
@@ -1674,29 +1680,29 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="14"/>
       <c r="B28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="14"/>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="14"/>
       <c r="B30" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1704,7 +1710,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" s="0"/>
       <c r="D32" s="18"/>
@@ -1712,29 +1718,29 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1748,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1756,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,7 +1774,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>75</v>
@@ -1779,7 +1785,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>75</v>
@@ -1790,7 +1796,7 @@
         <v>77</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,7 +1804,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,7 +1822,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1830,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1832,7 +1838,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,7 +1846,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,7 +1863,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1873,7 +1879,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1881,7 +1887,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1902,17 +1908,17 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,7 +1937,7 @@
         <v>90</v>
       </c>
       <c r="B2" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>91</v>
@@ -1953,7 +1959,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>0</v>
+        <v>191</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>95</v>
@@ -2688,7 +2694,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,17 +2730,16 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,19 +2833,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,7 +2919,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>211</v>
@@ -2951,13 +2956,19 @@
       <c r="B15" s="25" t="s">
         <v>217</v>
       </c>
+      <c r="C15" s="25" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,79 +2976,109 @@
         <v>203</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>220</v>
+      <c r="C19" s="26" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="C20" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>227</v>
+        <v>228</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="C24" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="C25" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3086,10 @@
         <v>212</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,7 +3097,10 @@
         <v>214</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>231</v>
+        <v>233</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,7 +3108,10 @@
         <v>216</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3089,16 +3139,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3110,7 +3160,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3133,10 +3183,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3150,7 +3200,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3161,10 +3211,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3184,16 +3234,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3288,7 +3338,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3321,7 +3371,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="36" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -3354,7 +3404,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3387,7 +3437,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3420,7 +3470,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="36" t="str">
         <f aca="false">IF(D18&gt;=1, "OK", "missing!")</f>
@@ -3453,7 +3503,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="36" t="str">
         <f aca="false">IF(D19&gt;=1, "OK", "missing!")</f>
@@ -3486,7 +3536,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="36" t="str">
         <f aca="false">IF(D20&gt;=1, "OK", "missing!")</f>
@@ -3519,7 +3569,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="36" t="str">
         <f aca="false">IF(D21&gt;=1, "OK", "missing!")</f>
@@ -3552,7 +3602,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="36" t="str">
         <f aca="false">IF(D22&gt;=1, "OK", "missing!")</f>
@@ -3585,7 +3635,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" s="36" t="str">
         <f aca="false">IF(D23&gt;=1, "OK", "missing!")</f>
@@ -3618,7 +3668,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="35" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" s="36" t="str">
         <f aca="false">IF(D24&gt;=1, "OK", "missing!")</f>
@@ -3651,7 +3701,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="36" t="str">
         <f aca="false">IF(D25&gt;=1, "OK", "missing!")</f>
@@ -3684,7 +3734,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" s="36" t="str">
         <f aca="false">IF(D26&gt;=1, "OK", "missing!")</f>
@@ -3717,7 +3767,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="36" t="str">
         <f aca="false">IF(D27&gt;=1, "OK", "missing!")</f>
@@ -3750,7 +3800,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="36" t="str">
         <f aca="false">IF(D28&gt;=1, "OK", "missing!")</f>
@@ -3783,7 +3833,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C29" s="36" t="str">
         <f aca="false">IF(D29&gt;=1, "OK", "missing!")</f>
@@ -3816,7 +3866,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -3849,7 +3899,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" s="36" t="str">
         <f aca="false">IF(D31&gt;=1, "OK", "missing!")</f>
@@ -4509,7 +4559,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5169,7 +5219,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -6720,7 +6770,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -6762,7 +6812,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -6783,7 +6833,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -6804,7 +6854,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -6825,7 +6875,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -6846,7 +6896,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -6867,7 +6917,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -6888,7 +6938,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -6909,7 +6959,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="39" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C127" s="36" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
graphs drawn is steps-mid grid availability displayed in graph included external blackout timeseries from csv -> not saved in blackout.csv file! get single location from renewables ninjas, potentially implementable in tool
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="252">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t xml:space="preserve">solar_backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diesel_solar</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -1228,10 +1231,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0459183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,16 +1444,16 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,11 +1917,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2694,7 +2697,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,11 +2738,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,19 +2837,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,15 +2963,21 @@
       <c r="C15" s="25" t="s">
         <v>218</v>
       </c>
+      <c r="D15" s="25" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2981,32 +2991,41 @@
       <c r="C17" s="26" t="s">
         <v>45</v>
       </c>
+      <c r="D17" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>222</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>221</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="D19" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>167</v>
@@ -3014,10 +3033,13 @@
       <c r="C20" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="D20" s="26" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>45</v>
@@ -3025,32 +3047,41 @@
       <c r="C21" s="26" t="s">
         <v>45</v>
       </c>
+      <c r="D21" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>167</v>
@@ -3058,15 +3089,21 @@
       <c r="C24" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="D24" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>167</v>
       </c>
       <c r="C25" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3080,15 +3117,21 @@
       <c r="C26" s="26" t="s">
         <v>43</v>
       </c>
+      <c r="D26" s="26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
         <v>212</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C27" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3097,10 +3140,13 @@
         <v>214</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>45</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3111,6 +3157,9 @@
         <v>45</v>
       </c>
       <c r="C29" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3139,16 +3188,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3160,7 +3209,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3183,10 +3232,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3200,7 +3249,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3211,10 +3260,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3234,16 +3283,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3338,7 +3387,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3404,7 +3453,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3437,7 +3486,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3866,7 +3915,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4559,7 +4608,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5219,7 +5268,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -6770,7 +6819,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -6812,7 +6861,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -6833,7 +6882,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -6854,7 +6903,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -6875,7 +6924,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -6896,7 +6945,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -6917,7 +6966,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -6938,7 +6987,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Integrating stability constraint, evaluation script
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="272">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -583,6 +583,9 @@
     <t xml:space="preserve">Step</t>
   </si>
   <si>
+    <t xml:space="preserve">shortage_max_share</t>
+  </si>
+  <si>
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
@@ -604,10 +607,13 @@
     <t xml:space="preserve">title_grid_availability</t>
   </si>
   <si>
-    <t xml:space="preserve">gridavailability_from_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/intermediate_tier2.csv</t>
+    <t xml:space="preserve">seperator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17_Polo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/17_Polo.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand</t>
@@ -619,10 +625,61 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">GridAvailability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gridavailability_internal_randomized</t>
+    <t xml:space="preserve">;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20_Mamburao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/20_Mamburao.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32_Taytay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/32_Taytay.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34_Araceli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53_Nabuctot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/53_Nabuctot.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">105_Cinco-Rama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/105_Cinco-Rama.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107_Balut Is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/107_Balut Is..csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">108_Lebak-Kalamansig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/108_Lebak-Kalamansig.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121_Tandubanak.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/121_Tandubanak.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126_Pangutaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/126_Pangutaran.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -679,13 +736,16 @@
     <t xml:space="preserve">renewable_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">shs_backup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solar_backup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diesel_solar</t>
+    <t xml:space="preserve">mg_hybrid_no_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar_battery_mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diesel_mg</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -703,6 +763,9 @@
     <t xml:space="preserve">capacity_genset_kW</t>
   </si>
   <si>
+    <t xml:space="preserve">peak_demand</t>
+  </si>
+  <si>
     <t xml:space="preserve">genset_with_minimal_loading</t>
   </si>
   <si>
@@ -712,12 +775,12 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_demand</t>
-  </si>
-  <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
   </si>
   <si>
@@ -727,10 +790,7 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">0.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">share_usage</t>
+    <t xml:space="preserve">share_hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">Data Sufficiency Check</t>
@@ -1132,27 +1192,9 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-      </font>
-    </dxf>
+    <dxf/>
+    <dxf/>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -1231,10 +1273,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6173469387755"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,15 +1487,15 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,11 +1959,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,7 +1982,7 @@
         <v>90</v>
       </c>
       <c r="B2" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>91</v>
@@ -1962,7 +2004,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="10" t="n">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>95</v>
@@ -2689,15 +2731,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,6 +2754,20 @@
       </c>
       <c r="D1" s="0" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>
@@ -2730,20 +2786,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,73 +2808,289 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" s="10"/>
+        <v>192</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>193</v>
+      </c>
       <c r="I2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>197</v>
+        <v>167</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="F4" s="21" t="s">
+      <c r="D4" s="0" t="s">
         <v>196</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>198</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>167</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2837,19 +3109,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,66 +3131,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>200</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>202</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>207</v>
+        <v>226</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,50 +3198,53 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="58.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>201</v>
+        <v>220</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>219</v>
+        <v>238</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>43</v>
@@ -2980,10 +3255,13 @@
       <c r="D16" s="26" t="s">
         <v>43</v>
       </c>
+      <c r="E16" s="26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>45</v>
@@ -2994,94 +3272,115 @@
       <c r="D17" s="26" t="s">
         <v>45</v>
       </c>
+      <c r="E17" s="26" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>222</v>
+        <v>242</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>167</v>
+        <v>242</v>
       </c>
       <c r="D19" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="B20" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>222</v>
+      <c r="E20" s="26" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>45</v>
       </c>
+      <c r="E21" s="26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>227</v>
+        <v>248</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>227</v>
+        <v>248</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>229</v>
+        <v>167</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>229</v>
+        <v>167</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="E23" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>167</v>
@@ -3092,10 +3391,13 @@
       <c r="D24" s="26" t="s">
         <v>167</v>
       </c>
+      <c r="E24" s="26" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>167</v>
@@ -3104,6 +3406,9 @@
         <v>167</v>
       </c>
       <c r="D25" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3120,38 +3425,47 @@
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
+      <c r="E26" s="26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>232</v>
+        <v>253</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>234</v>
+        <v>254</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>45</v>
@@ -3160,6 +3474,9 @@
         <v>45</v>
       </c>
       <c r="D29" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3188,16 +3505,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3209,7 +3526,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3232,10 +3549,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3249,7 +3566,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3260,10 +3577,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3283,16 +3600,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3387,7 +3704,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3453,7 +3770,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3486,7 +3803,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3915,7 +4232,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4608,7 +4925,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5268,7 +5585,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -6621,7 +6938,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="35" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C112" s="36" t="str">
         <f aca="false">IF(D112&gt;=1, "OK", "missing!")</f>
@@ -6654,7 +6971,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="35" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C113" s="36" t="str">
         <f aca="false">IF(D113&gt;=1, "OK", "missing!")</f>
@@ -6687,7 +7004,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C114" s="36" t="str">
         <f aca="false">IF(D114&gt;=1, "OK", "missing!")</f>
@@ -6720,7 +7037,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="35" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C115" s="36" t="str">
         <f aca="false">IF(D115&gt;=1, "OK", "missing!")</f>
@@ -6753,7 +7070,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="35" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C116" s="36" t="str">
         <f aca="false">IF(D116&gt;=1, "OK", "missing!")</f>
@@ -6786,7 +7103,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="35" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C117" s="36" t="str">
         <f aca="false">IF(D117&gt;=1, "OK", "missing!")</f>
@@ -6819,7 +7136,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -6840,7 +7157,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="39" t="s">
-        <v>203</v>
+        <v>222</v>
       </c>
       <c r="C119" s="36" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -6861,7 +7178,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -6882,7 +7199,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -6903,7 +7220,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -6924,7 +7241,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -6945,7 +7262,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -6966,7 +7283,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -6987,7 +7304,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7041,7 +7358,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="39" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="C128" s="36" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7074,7 +7391,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="39" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="C129" s="36" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7107,7 +7424,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="39" t="s">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="C130" s="36" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
input file for leicester
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="254">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -583,9 +583,6 @@
     <t xml:space="preserve">Step</t>
   </si>
   <si>
-    <t xml:space="preserve">shortage_max_share</t>
-  </si>
-  <si>
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
@@ -610,10 +607,10 @@
     <t xml:space="preserve">seperator</t>
   </si>
   <si>
-    <t xml:space="preserve">17_Polo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/17_Polo.csv</t>
+    <t xml:space="preserve">consumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/intermediate_tier2.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand</t>
@@ -625,61 +622,10 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20_Mamburao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/20_Mamburao.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32_Taytay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/32_Taytay.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34_Araceli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53_Nabuctot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/53_Nabuctot.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105_Cinco-Rama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/105_Cinco-Rama.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">107_Balut Is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/107_Balut Is..csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108_Lebak-Kalamansig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/108_Lebak-Kalamansig.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121_Tandubanak.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/121_Tandubanak.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">126_Pangutaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/126_Pangutaran.csv</t>
+    <t xml:space="preserve">GridAvailability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute</t>
@@ -736,16 +682,16 @@
     <t xml:space="preserve">renewable_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve">mg_hybrid_no_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg_hybrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">solar_battery_mg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diesel_mg</t>
+    <t xml:space="preserve">solar_backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery_backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs_backup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sole_grid</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -763,28 +709,28 @@
     <t xml:space="preserve">capacity_genset_kW</t>
   </si>
   <si>
+    <t xml:space="preserve">genset_with_minimal_loading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_of_equal_generators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_pcc_consumption_kW</t>
+  </si>
+  <si>
     <t xml:space="preserve">peak_demand</t>
   </si>
   <si>
-    <t xml:space="preserve">genset_with_minimal_loading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number_of_equal_generators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacity_pcc_consumption_kW</t>
-  </si>
-  <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_wind_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
   </si>
   <si>
     <t xml:space="preserve">default</t>
@@ -1266,17 +1212,16 @@
   </sheetPr>
   <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,7 +1416,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1486,16 +1431,15 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1882,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1953,17 +1897,16 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.35"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,7 +2132,7 @@
         <v>123</v>
       </c>
       <c r="B20" s="10" t="n">
-        <v>0.15</v>
+        <v>0.0316</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>115</v>
@@ -2387,7 +2330,7 @@
         <v>145</v>
       </c>
       <c r="B38" s="10" t="n">
-        <v>1000</v>
+        <v>1064</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>146</v>
@@ -2398,7 +2341,7 @@
         <v>147</v>
       </c>
       <c r="B39" s="10" t="n">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>148</v>
@@ -2420,7 +2363,7 @@
         <v>150</v>
       </c>
       <c r="B41" s="10" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>105</v>
@@ -2442,7 +2385,7 @@
         <v>152</v>
       </c>
       <c r="B43" s="10" t="n">
-        <v>0.1</v>
+        <v>0.037</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>115</v>
@@ -2500,7 +2443,7 @@
         <v>159</v>
       </c>
       <c r="B48" s="10" t="n">
-        <v>600</v>
+        <v>203</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>115</v>
@@ -2511,7 +2454,7 @@
         <v>160</v>
       </c>
       <c r="B49" s="10" t="n">
-        <v>0</v>
+        <v>15.8</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>161</v>
@@ -2577,7 +2520,7 @@
         <v>169</v>
       </c>
       <c r="B55" s="10" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>105</v>
@@ -2718,7 +2661,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2731,16 +2674,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2756,24 +2696,10 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2786,20 +2712,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,295 +2732,61 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="I2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>195</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>167</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H12" s="0" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3111,17 +2801,15 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,66 +2819,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,53 +2886,53 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="67.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>238</v>
-      </c>
       <c r="E15" s="25" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>43</v>
@@ -3261,7 +2949,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>45</v>
@@ -3278,16 +2966,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>242</v>
+        <v>167</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="E18" s="26" t="s">
         <v>167</v>
@@ -3295,16 +2983,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>242</v>
+        <v>167</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>167</v>
@@ -3312,75 +3000,75 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>242</v>
+        <v>167</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>167</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>167</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>167</v>
@@ -3397,7 +3085,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>167</v>
@@ -3431,41 +3119,41 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>45</v>
@@ -3483,7 +3171,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -3498,23 +3186,21 @@
   </sheetPr>
   <dimension ref="B1:I130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3526,7 +3212,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3549,10 +3235,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3566,7 +3252,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3577,10 +3263,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3600,16 +3286,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3704,7 +3390,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3770,7 +3456,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3803,7 +3489,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -4232,7 +3918,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4925,7 +4611,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5585,7 +5271,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -6938,7 +6624,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C112" s="36" t="str">
         <f aca="false">IF(D112&gt;=1, "OK", "missing!")</f>
@@ -6971,7 +6657,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C113" s="36" t="str">
         <f aca="false">IF(D113&gt;=1, "OK", "missing!")</f>
@@ -7004,7 +6690,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C114" s="36" t="str">
         <f aca="false">IF(D114&gt;=1, "OK", "missing!")</f>
@@ -7037,7 +6723,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C115" s="36" t="str">
         <f aca="false">IF(D115&gt;=1, "OK", "missing!")</f>
@@ -7070,7 +6756,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C116" s="36" t="str">
         <f aca="false">IF(D116&gt;=1, "OK", "missing!")</f>
@@ -7103,7 +6789,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C117" s="36" t="str">
         <f aca="false">IF(D117&gt;=1, "OK", "missing!")</f>
@@ -7136,7 +6822,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7157,7 +6843,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="39" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="C119" s="36" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -7178,7 +6864,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7199,7 +6885,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7220,7 +6906,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7241,7 +6927,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7262,7 +6948,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7283,7 +6969,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7304,7 +6990,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7358,7 +7044,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="39" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="C128" s="36" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7391,7 +7077,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="39" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="C129" s="36" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7424,7 +7110,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="39" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="C130" s="36" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>
@@ -7480,7 +7166,7 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Cleaning for master version
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="259">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -583,9 +583,6 @@
     <t xml:space="preserve">Step</t>
   </si>
   <si>
-    <t xml:space="preserve">shortage_max_share</t>
-  </si>
-  <si>
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
@@ -628,52 +625,16 @@
     <t xml:space="preserve">;</t>
   </si>
   <si>
-    <t xml:space="preserve">20_Mamburao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/20_Mamburao.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32_Taytay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/32_Taytay.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">34_Araceli</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">53_Nabuctot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/53_Nabuctot.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105_Cinco-Rama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/105_Cinco-Rama.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">107_Balut Is.</t>
   </si>
   <si>
     <t xml:space="preserve">./inputs/timeseries/107_Balut Is..csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108_Lebak-Kalamansig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/108_Lebak-Kalamansig.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121_Tandubanak.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/121_Tandubanak.csv</t>
   </si>
   <si>
     <t xml:space="preserve">126_Pangutaran</t>
@@ -1276,7 +1237,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,7 +1456,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,7 +1914,7 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1962,7 +1923,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.35"/>
   </cols>
   <sheetData>
@@ -2731,7 +2692,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -2739,7 +2700,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,20 +2715,6 @@
       </c>
       <c r="D1" s="0" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.03</v>
       </c>
     </row>
   </sheetData>
@@ -2786,20 +2733,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2808,289 +2755,133 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="I2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>195</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>198</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>167</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="B4" s="0" t="s">
         <v>200</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>201</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="G4" s="22" t="s">
         <v>167</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>203</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="G5" s="22" t="s">
         <v>167</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>205</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>167</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>167</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F7" s="0" t="s">
         <v>198</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3112,16 +2903,16 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3131,66 +2922,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,53 +2989,53 @@
         <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>43</v>
@@ -3261,7 +3052,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>45</v>
@@ -3278,16 +3069,16 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="E18" s="26" t="s">
         <v>167</v>
@@ -3295,16 +3086,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>167</v>
@@ -3312,24 +3103,24 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D20" s="26" t="s">
         <v>167</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>45</v>
@@ -3346,24 +3137,24 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>167</v>
@@ -3380,7 +3171,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>167</v>
@@ -3397,7 +3188,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>167</v>
@@ -3431,41 +3222,41 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>45</v>
@@ -3498,7 +3289,7 @@
   </sheetPr>
   <dimension ref="B1:I130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3506,15 +3297,15 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3526,7 +3317,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3549,10 +3340,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3566,7 +3357,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3577,10 +3368,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3600,16 +3391,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3704,7 +3495,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3770,7 +3561,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3803,7 +3594,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -4232,7 +4023,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4925,7 +4716,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5585,7 +5376,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -6938,7 +6729,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C112" s="36" t="str">
         <f aca="false">IF(D112&gt;=1, "OK", "missing!")</f>
@@ -6971,7 +6762,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C113" s="36" t="str">
         <f aca="false">IF(D113&gt;=1, "OK", "missing!")</f>
@@ -7004,7 +6795,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C114" s="36" t="str">
         <f aca="false">IF(D114&gt;=1, "OK", "missing!")</f>
@@ -7037,7 +6828,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C115" s="36" t="str">
         <f aca="false">IF(D115&gt;=1, "OK", "missing!")</f>
@@ -7070,7 +6861,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C116" s="36" t="str">
         <f aca="false">IF(D116&gt;=1, "OK", "missing!")</f>
@@ -7103,7 +6894,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C117" s="36" t="str">
         <f aca="false">IF(D117&gt;=1, "OK", "missing!")</f>
@@ -7136,7 +6927,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -7157,7 +6948,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="39" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C119" s="36" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -7178,7 +6969,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -7199,7 +6990,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7220,7 +7011,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7241,7 +7032,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7262,7 +7053,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7283,7 +7074,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7304,7 +7095,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7358,7 +7149,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="39" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C128" s="36" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7391,7 +7182,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="39" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="C129" s="36" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7424,7 +7215,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="39" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C130" s="36" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Enable "do not save oemof results" -> Save, evaluate, delete
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -157,16 +157,16 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
     <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
     <t xml:space="preserve">evaluated_days</t>
@@ -1447,8 +1447,8 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1581,15 +1581,15 @@
         <v>44</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,7 +1597,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="10" t="n">
-        <v>365</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,7 +1624,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>53</v>
@@ -1652,7 +1652,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1727,7 @@
         <v>68</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1735,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>70</v>
@@ -1754,7 +1754,7 @@
         <v>72</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1762,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1780,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>75</v>
@@ -1791,7 +1791,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>75</v>
@@ -1802,7 +1802,7 @@
         <v>77</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1810,7 @@
         <v>78</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,7 +1828,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1836,7 @@
         <v>80</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,7 +1844,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1852,7 @@
         <v>82</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1869,7 @@
         <v>83</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1877,7 +1877,7 @@
         <v>84</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,7 +1885,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,7 +1893,7 @@
         <v>86</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +1914,7 @@
   </sheetPr>
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2741,8 +2741,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.23"/>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>217</v>
@@ -3038,16 +3038,16 @@
         <v>227</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,16 +3055,16 @@
         <v>209</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,16 +3123,16 @@
         <v>233</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="26" t="s">
-        <v>45</v>
-      </c>
       <c r="E21" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3205,19 +3205,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>43</v>
-      </c>
       <c r="C26" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,16 +3259,16 @@
         <v>222</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="36" t="str">
         <f aca="false">IF(D15&gt;=1, "OK", "missing!")</f>
@@ -7116,7 +7116,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C127" s="36" t="str">
         <f aca="false">IF(D127&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Cleaning for tutorial Cloning inputs capacities == 0 != False -> None in case definition Messages for sum pv/wind gen == 0 Error messages for sum demand == 0 Added colours to generated graph
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="262">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -382,6 +382,12 @@
     <t xml:space="preserve">genset_min_loading</t>
   </si>
   <si>
+    <t xml:space="preserve">genset_oversize_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(only used if estimated through case definition “peak demand”)</t>
+  </si>
+  <si>
     <t xml:space="preserve">maingrid_distance</t>
   </si>
   <si>
@@ -415,6 +421,9 @@
     <t xml:space="preserve">min_renewable_share</t>
   </si>
   <si>
+    <t xml:space="preserve">pcc_oversize_factor</t>
+  </si>
+  <si>
     <t xml:space="preserve">pcoupling_batch</t>
   </si>
   <si>
@@ -523,7 +532,7 @@
     <t xml:space="preserve">None</t>
   </si>
   <si>
-    <t xml:space="preserve">None of factor</t>
+    <t xml:space="preserve">None or factor</t>
   </si>
   <si>
     <t xml:space="preserve">storage_lifetime</t>
@@ -1234,10 +1243,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2704081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,16 +1456,16 @@
   </sheetPr>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1734,7 @@
         <v>66</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>67</v>
@@ -1902,18 +1911,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -2128,10 +2137,13 @@
       <c r="A19" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="10" t="n">
-        <v>0</v>
+      <c r="B19" s="0" t="n">
+        <v>1.2</v>
       </c>
       <c r="C19" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2140,21 +2152,21 @@
         <v>120</v>
       </c>
       <c r="B20" s="10" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B21" s="10" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,37 +2185,37 @@
         <v>125</v>
       </c>
       <c r="B23" s="10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="B24" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B25" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B26" s="10" t="n">
         <v>0</v>
@@ -2214,79 +2226,82 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B28" s="10" t="n">
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1.05</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B29" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B30" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B31" s="10" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B33" s="10" t="n">
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,10 +2309,10 @@
         <v>137</v>
       </c>
       <c r="B34" s="10" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,32 +2320,32 @@
         <v>138</v>
       </c>
       <c r="B35" s="10" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B36" s="10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B37" s="10" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>141</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,32 +2353,32 @@
         <v>142</v>
       </c>
       <c r="B38" s="10" t="n">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="B39" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C40" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="B40" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,40 +2386,40 @@
         <v>147</v>
       </c>
       <c r="B41" s="10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B42" s="10" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B43" s="10" t="n">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B44" s="10" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>90</v>
@@ -2412,13 +2427,13 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B45" s="10" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,7 +2441,7 @@
         <v>153</v>
       </c>
       <c r="B46" s="10" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>90</v>
@@ -2437,12 +2452,9 @@
         <v>154</v>
       </c>
       <c r="B47" s="10" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="0" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2451,10 +2463,10 @@
         <v>156</v>
       </c>
       <c r="B48" s="10" t="n">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,9 +2474,12 @@
         <v>157</v>
       </c>
       <c r="B49" s="10" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C49" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2473,10 +2488,10 @@
         <v>159</v>
       </c>
       <c r="B50" s="10" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,29 +2499,29 @@
         <v>160</v>
       </c>
       <c r="B51" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B52" s="20" t="n">
-        <v>1</v>
+        <v>162</v>
+      </c>
+      <c r="B52" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B53" s="10" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>90</v>
@@ -2514,51 +2529,51 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" s="10" t="s">
         <v>164</v>
       </c>
+      <c r="B54" s="20" t="n">
+        <v>1</v>
+      </c>
       <c r="C54" s="19" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B55" s="10" t="n">
-        <v>15</v>
+        <v>0.9</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B56" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="C56" s="19" t="s">
-        <v>90</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B57" s="10" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B58" s="10" t="n">
         <v>0</v>
@@ -2569,10 +2584,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B59" s="10" t="n">
-        <v>0.09</v>
+        <v>1</v>
       </c>
       <c r="C59" s="19" t="s">
         <v>90</v>
@@ -2580,7 +2595,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>0</v>
@@ -2591,10 +2606,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B61" s="10" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="C61" s="19" t="s">
         <v>90</v>
@@ -2602,7 +2617,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B62" s="10" t="n">
         <v>0</v>
@@ -2613,56 +2628,78 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B63" s="10" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B64" s="10" t="n">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B65" s="10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B66" s="10" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B67" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B68" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C67" s="19" t="s">
+      <c r="C69" s="19" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2690,7 +2727,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2698,18 +2735,18 @@
         <v>84</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -2745,12 +2782,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,133 +2796,133 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>195</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2906,17 +2943,17 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,66 +2963,66 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,28 +3030,28 @@
         <v>45</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>72</v>
@@ -3022,24 +3059,24 @@
     </row>
     <row r="15" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="24" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>43</v>
@@ -3056,7 +3093,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="24" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>43</v>
@@ -3073,58 +3110,58 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="24" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="24" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="24" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="24" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>43</v>
@@ -3141,70 +3178,70 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="24" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="24" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3226,41 +3263,41 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="24" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B29" s="26" t="s">
         <v>43</v>
@@ -3300,16 +3337,16 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="9" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="11.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="27" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3321,7 +3358,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -3344,10 +3381,10 @@
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3361,7 +3398,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3372,10 +3409,10 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
       <c r="C7" s="31" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -3395,16 +3432,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
@@ -3499,7 +3536,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="35" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(D14&gt;=1, "OK", "missing!")</f>
@@ -3565,7 +3602,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="35" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C16" s="36" t="str">
         <f aca="false">IF(D16&gt;=1, "OK", "missing!")</f>
@@ -3598,7 +3635,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="35" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C17" s="36" t="str">
         <f aca="false">IF(D17&gt;=1, "OK", "missing!")</f>
@@ -3895,7 +3932,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="35" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C26" s="36" t="str">
         <f aca="false">IF(D26&gt;=1, "OK", "missing!")</f>
@@ -4027,7 +4064,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="35" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C30" s="36" t="str">
         <f aca="false">IF(D30&gt;=1, "OK", "missing!")</f>
@@ -4720,7 +4757,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="35" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C51" s="36" t="str">
         <f aca="false">IF(D51&gt;=1, "OK", "missing!")</f>
@@ -5149,7 +5186,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="35" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C64" s="36" t="str">
         <f aca="false">IF(D64&gt;=1, "OK", "missing!")</f>
@@ -5182,7 +5219,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C65" s="36" t="str">
         <f aca="false">IF(D65&gt;=1, "OK", "missing!")</f>
@@ -5215,7 +5252,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="35" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C66" s="36" t="str">
         <f aca="false">IF(D66&gt;=1, "OK", "missing!")</f>
@@ -5248,7 +5285,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="35" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C67" s="36" t="str">
         <f aca="false">IF(D67&gt;=1, "OK", "missing!")</f>
@@ -5281,7 +5318,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="35" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C68" s="36" t="str">
         <f aca="false">IF(D68&gt;=1, "OK", "missing!")</f>
@@ -5314,7 +5351,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="35" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C69" s="36" t="str">
         <f aca="false">IF(D69&gt;=1, "OK", "missing!")</f>
@@ -5347,7 +5384,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="35" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C70" s="36" t="str">
         <f aca="false">IF(D70&gt;=1, "OK", "missing!")</f>
@@ -5380,7 +5417,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="35" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C71" s="36" t="str">
         <f aca="false">IF(D71&gt;=1, "OK", "missing!")</f>
@@ -5413,7 +5450,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C72" s="36" t="str">
         <f aca="false">IF(D72&gt;=1, "OK", "missing!")</f>
@@ -5446,7 +5483,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="35" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C73" s="36" t="str">
         <f aca="false">IF(D73&gt;=1, "OK", "missing!")</f>
@@ -5479,7 +5516,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C74" s="36" t="str">
         <f aca="false">IF(D74&gt;=1, "OK", "missing!")</f>
@@ -5512,7 +5549,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="35" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C75" s="36" t="str">
         <f aca="false">IF(D75&gt;=1, "OK", "missing!")</f>
@@ -5545,7 +5582,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="35" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C76" s="36" t="str">
         <f aca="false">IF(D76&gt;=1, "OK", "missing!")</f>
@@ -5578,7 +5615,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="35" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C77" s="36" t="str">
         <f aca="false">IF(D77&gt;=1, "OK", "missing!")</f>
@@ -5611,7 +5648,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="35" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C78" s="36" t="str">
         <f aca="false">IF(D78&gt;=1, "OK", "missing!")</f>
@@ -5644,7 +5681,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="35" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C79" s="36" t="str">
         <f aca="false">IF(D79&gt;=1, "OK", "missing!")</f>
@@ -5677,7 +5714,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="35" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C80" s="36" t="str">
         <f aca="false">IF(D80&gt;=1, "OK", "missing!")</f>
@@ -5710,7 +5747,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="35" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C81" s="36" t="str">
         <f aca="false">IF(D81&gt;=1, "OK", "missing!")</f>
@@ -5743,7 +5780,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="35" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C82" s="36" t="str">
         <f aca="false">IF(D82&gt;=1, "OK", "missing!")</f>
@@ -5776,7 +5813,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="35" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C83" s="36" t="str">
         <f aca="false">IF(D83&gt;=1, "OK", "missing!")</f>
@@ -5809,7 +5846,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="35" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C84" s="36" t="str">
         <f aca="false">IF(D84&gt;=1, "OK", "missing!")</f>
@@ -5842,7 +5879,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="35" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C85" s="36" t="str">
         <f aca="false">IF(D85&gt;=1, "OK", "missing!")</f>
@@ -5875,7 +5912,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="35" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C86" s="36" t="str">
         <f aca="false">IF(D86&gt;=1, "OK", "missing!")</f>
@@ -5908,7 +5945,7 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="35" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C87" s="36" t="str">
         <f aca="false">IF(D87&gt;=1, "OK", "missing!")</f>
@@ -5941,7 +5978,7 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="35" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C88" s="36" t="str">
         <f aca="false">IF(D88&gt;=1, "OK", "missing!")</f>
@@ -5974,7 +6011,7 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="35" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C89" s="36" t="str">
         <f aca="false">IF(D89&gt;=1, "OK", "missing!")</f>
@@ -6007,7 +6044,7 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="35" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C90" s="36" t="str">
         <f aca="false">IF(D90&gt;=1, "OK", "missing!")</f>
@@ -6040,7 +6077,7 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="35" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C91" s="36" t="str">
         <f aca="false">IF(D91&gt;=1, "OK", "missing!")</f>
@@ -6073,7 +6110,7 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="35" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C92" s="36" t="str">
         <f aca="false">IF(D92&gt;=1, "OK", "missing!")</f>
@@ -6106,7 +6143,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="35" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C93" s="36" t="str">
         <f aca="false">IF(D93&gt;=1, "OK", "missing!")</f>
@@ -6139,7 +6176,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="35" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C94" s="36" t="str">
         <f aca="false">IF(D94&gt;=1, "OK", "missing!")</f>
@@ -6172,7 +6209,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="35" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C95" s="36" t="str">
         <f aca="false">IF(D95&gt;=1, "OK", "missing!")</f>
@@ -6205,7 +6242,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="35" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C96" s="36" t="str">
         <f aca="false">IF(D96&gt;=1, "OK", "missing!")</f>
@@ -6238,7 +6275,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="35" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C97" s="36" t="str">
         <f aca="false">IF(D97&gt;=1, "OK", "missing!")</f>
@@ -6271,7 +6308,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="35" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C98" s="36" t="str">
         <f aca="false">IF(D98&gt;=1, "OK", "missing!")</f>
@@ -6304,7 +6341,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="35" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C99" s="36" t="str">
         <f aca="false">IF(D99&gt;=1, "OK", "missing!")</f>
@@ -6337,7 +6374,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="35" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C100" s="36" t="str">
         <f aca="false">IF(D100&gt;=1, "OK", "missing!")</f>
@@ -6370,7 +6407,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="35" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C101" s="36" t="str">
         <f aca="false">IF(D101&gt;=1, "OK", "missing!")</f>
@@ -6403,7 +6440,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="35" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C102" s="36" t="str">
         <f aca="false">IF(D102&gt;=1, "OK", "missing!")</f>
@@ -6436,7 +6473,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="35" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C103" s="36" t="str">
         <f aca="false">IF(D103&gt;=1, "OK", "missing!")</f>
@@ -6469,7 +6506,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="35" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C104" s="36" t="str">
         <f aca="false">IF(D104&gt;=1, "OK", "missing!")</f>
@@ -6502,7 +6539,7 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="35" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C105" s="36" t="str">
         <f aca="false">IF(D105&gt;=1, "OK", "missing!")</f>
@@ -6535,7 +6572,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="35" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C106" s="36" t="str">
         <f aca="false">IF(D106&gt;=1, "OK", "missing!")</f>
@@ -6568,7 +6605,7 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="35" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C107" s="36" t="str">
         <f aca="false">IF(D107&gt;=1, "OK", "missing!")</f>
@@ -6601,7 +6638,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="35" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C108" s="36" t="str">
         <f aca="false">IF(D108&gt;=1, "OK", "missing!")</f>
@@ -6634,7 +6671,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="35" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C109" s="36" t="str">
         <f aca="false">IF(D109&gt;=1, "OK", "missing!")</f>
@@ -6667,7 +6704,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="35" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C110" s="36" t="str">
         <f aca="false">IF(D110&gt;=1, "OK", "missing!")</f>
@@ -6700,7 +6737,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="35" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C111" s="36" t="str">
         <f aca="false">IF(D111&gt;=1, "OK", "missing!")</f>
@@ -6733,7 +6770,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="35" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C112" s="36" t="str">
         <f aca="false">IF(D112&gt;=1, "OK", "missing!")</f>
@@ -6766,7 +6803,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="35" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C113" s="36" t="str">
         <f aca="false">IF(D113&gt;=1, "OK", "missing!")</f>
@@ -6799,7 +6836,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="35" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C114" s="36" t="str">
         <f aca="false">IF(D114&gt;=1, "OK", "missing!")</f>
@@ -6832,7 +6869,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="35" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C115" s="36" t="str">
         <f aca="false">IF(D115&gt;=1, "OK", "missing!")</f>
@@ -6865,7 +6902,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="35" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C116" s="36" t="str">
         <f aca="false">IF(D116&gt;=1, "OK", "missing!")</f>
@@ -6898,7 +6935,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="35" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C117" s="36" t="str">
         <f aca="false">IF(D117&gt;=1, "OK", "missing!")</f>
@@ -6931,7 +6968,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="39" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C118" s="36" t="str">
         <f aca="false">IF(D118&gt;=1, "OK", "missing!")</f>
@@ -6952,7 +6989,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="39" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C119" s="36" t="str">
         <f aca="false">IF(D119&gt;=1, "OK", "missing!")</f>
@@ -6973,7 +7010,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="39" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C120" s="36" t="str">
         <f aca="false">IF(D120&gt;=1, "OK", "missing!")</f>
@@ -6994,7 +7031,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="39" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C121" s="36" t="str">
         <f aca="false">IF(D121&gt;=1, "OK", "missing!")</f>
@@ -7015,7 +7052,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="39" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C122" s="36" t="str">
         <f aca="false">IF(D122&gt;=1, "OK", "missing!")</f>
@@ -7036,7 +7073,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="39" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C123" s="36" t="str">
         <f aca="false">IF(D123&gt;=1, "OK", "missing!")</f>
@@ -7057,7 +7094,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="39" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C124" s="36" t="str">
         <f aca="false">IF(D124&gt;=1, "OK", "missing!")</f>
@@ -7078,7 +7115,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="39" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C125" s="36" t="str">
         <f aca="false">IF(D125&gt;=1, "OK", "missing!")</f>
@@ -7099,7 +7136,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="39" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C126" s="36" t="str">
         <f aca="false">IF(D126&gt;=1, "OK", "missing!")</f>
@@ -7153,7 +7190,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="39" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C128" s="36" t="str">
         <f aca="false">IF(D128&gt;=1, "OK", "missing!")</f>
@@ -7186,7 +7223,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="39" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C129" s="36" t="str">
         <f aca="false">IF(D129&gt;=1, "OK", "missing!")</f>
@@ -7219,7 +7256,7 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="39" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C130" s="36" t="str">
         <f aca="false">IF(D130&gt;=1, "OK", "missing!")</f>

</xml_diff>

<commit_message>
Changes in input template Changed some storage parameter names Blackout restore now working - no double entries Experiment/Blackout name with float Adjusted paths for windows
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="252">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -405,9 +405,6 @@
     <t xml:space="preserve">min_renewable_share</t>
   </si>
   <si>
-    <t xml:space="preserve">pcc_oversize_factor</t>
-  </si>
-  <si>
     <t xml:space="preserve">pcoupling_batch</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t xml:space="preserve">pcoupling_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcoupling_oversize_factor</t>
   </si>
   <si>
     <t xml:space="preserve">price_fuel</t>
@@ -480,12 +480,6 @@
     <t xml:space="preserve">kWh</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_capacity_max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_capacity_min</t>
-  </si>
-  <si>
     <t xml:space="preserve">storage_cost_investment</t>
   </si>
   <si>
@@ -504,10 +498,19 @@
     <t xml:space="preserve">storage_Crate_discharge</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_inflow_efficiency</t>
+    <t xml:space="preserve">storage_efficiency_charge</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_initial_soc</t>
+    <t xml:space="preserve">storage_efficiency_discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_loss_timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_soc_initial</t>
   </si>
   <si>
     <t xml:space="preserve">None</t>
@@ -516,13 +519,10 @@
     <t xml:space="preserve">None or factor</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_lifetime</t>
+    <t xml:space="preserve">storage_soc_max</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_loss_timestep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_outflow_efficiency</t>
+    <t xml:space="preserve">storage_soc_min</t>
   </si>
   <si>
     <t xml:space="preserve">tax</t>
@@ -705,22 +705,25 @@
     <t xml:space="preserve">pcc_feedin_fixed_capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">True or False or default</t>
+    <t xml:space="preserve">True or False</t>
   </si>
   <si>
     <t xml:space="preserve">max_shortage</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
+    <t xml:space="preserve">value, default (recommended)</t>
   </si>
   <si>
     <t xml:space="preserve">stability_constraint</t>
   </si>
   <si>
-    <t xml:space="preserve"> False or share_usage or share_backup</t>
+    <t xml:space="preserve"> False, share_usage,  share_backup, share_hybrid (recommended)</t>
   </si>
   <si>
     <t xml:space="preserve">renewable_constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True or False or default</t>
   </si>
   <si>
     <t xml:space="preserve">mg_hybrid_no_min</t>
@@ -1177,10 +1180,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.2959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,16 +1383,16 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1538,7 @@
         <v>44</v>
       </c>
       <c r="C16" s="18" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1809,16 +1812,16 @@
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G68" activeCellId="0" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.484693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -1885,7 +1888,7 @@
         <v>85</v>
       </c>
       <c r="B7" s="18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>86</v>
@@ -1907,7 +1910,7 @@
         <v>89</v>
       </c>
       <c r="B9" s="18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>90</v>
@@ -2174,13 +2177,10 @@
         <v>126</v>
       </c>
       <c r="B33" s="18" t="n">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,10 +2188,10 @@
         <v>127</v>
       </c>
       <c r="B34" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,10 +2221,10 @@
         <v>130</v>
       </c>
       <c r="B37" s="18" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2232,10 +2232,10 @@
         <v>131</v>
       </c>
       <c r="B38" s="18" t="n">
-        <v>0.95</v>
+        <v>20</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,10 +2243,13 @@
         <v>132</v>
       </c>
       <c r="B39" s="18" t="n">
-        <v>20</v>
+        <v>1.05</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,10 +2400,10 @@
         <v>151</v>
       </c>
       <c r="B53" s="18" t="n">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2408,43 +2411,43 @@
         <v>152</v>
       </c>
       <c r="B54" s="18" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B55" s="18" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B56" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>155</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="18" t="n">
-        <v>0</v>
+      <c r="B57" s="27" t="n">
+        <v>1</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,7 +2455,7 @@
         <v>157</v>
       </c>
       <c r="B58" s="18" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>88</v>
@@ -2462,7 +2465,7 @@
       <c r="A59" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="27" t="n">
+      <c r="B59" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="15" t="s">
@@ -2474,32 +2477,32 @@
         <v>159</v>
       </c>
       <c r="B60" s="18" t="n">
-        <v>0.9</v>
+        <v>15</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B61" s="18" t="s">
-        <v>161</v>
+      <c r="B61" s="18" t="n">
+        <v>0</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>162</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="B62" s="18" t="n">
-        <v>15</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,7 +2510,7 @@
         <v>164</v>
       </c>
       <c r="B63" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>88</v>
@@ -2518,7 +2521,7 @@
         <v>165</v>
       </c>
       <c r="B64" s="18" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>88</v>
@@ -2635,7 +2638,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="2">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -2658,17 +2660,17 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2846,12 +2848,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16271,7 +16273,7 @@
         <v>209</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>210</v>
@@ -16283,7 +16285,7 @@
         <v>212</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>213</v>
@@ -16323,17 +16325,17 @@
   </sheetPr>
   <dimension ref="1:30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="7.1530612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="20" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29725,7 +29727,7 @@
         <v>231</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -31780,21 +31782,21 @@
         <v>216</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E16" s="39" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>39</v>
@@ -31828,58 +31830,58 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C19" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="40" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="40" t="s">
-        <v>238</v>
-      </c>
       <c r="C20" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>39</v>
@@ -31896,70 +31898,70 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C23" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="D23" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>244</v>
-      </c>
       <c r="E23" s="40" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31984,16 +31986,16 @@
         <v>227</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32001,16 +32003,16 @@
         <v>229</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
pp.pprint(overall_results) only for most important parameters... sadly not sensitivity parameters
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="251">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currently faulty</t>
   </si>
   <si>
     <t xml:space="preserve">allow_shortage</t>
@@ -1180,10 +1177,10 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.9489795918367"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,16 +1380,16 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,13 +1518,10 @@
       <c r="C14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>41</v>
@@ -1535,15 +1529,15 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="18" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="19" t="n">
         <v>43101</v>
@@ -1551,21 +1545,21 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,15 +1573,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>39</v>
@@ -1595,18 +1589,18 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="D24" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="18" t="n">
         <v>0.03</v>
@@ -1624,19 +1618,19 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
       <c r="B28" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
       <c r="B29" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1638,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="22"/>
@@ -1652,7 +1646,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>39</v>
@@ -1660,18 +1654,18 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>41</v>
@@ -1679,7 +1673,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>39</v>
@@ -1687,7 +1681,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>41</v>
@@ -1695,7 +1689,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>39</v>
@@ -1703,7 +1697,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>41</v>
@@ -1721,7 +1715,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>39</v>
@@ -1729,7 +1723,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>39</v>
@@ -1737,7 +1731,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>39</v>
@@ -1754,7 +1748,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>41</v>
@@ -1762,7 +1756,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>41</v>
@@ -1770,7 +1764,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>39</v>
@@ -1778,7 +1772,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>39</v>
@@ -1812,22 +1806,21 @@
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G68" activeCellId="0" sqref="G68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.61224489795918"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -1843,10 +1836,10 @@
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>79</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1856,10 +1849,10 @@
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1874,767 +1867,767 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="18" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="18" t="n">
         <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="18" t="n">
         <v>8.8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="18" t="n">
         <v>650</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="18" t="n">
         <v>0.33</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="18" t="n">
         <v>1.2</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B28" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B35" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" s="18" t="n">
         <v>0.95</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="18" t="n">
         <v>1.05</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="18" t="n">
         <v>0.89</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B41" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B43" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B44" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" s="18" t="n">
         <v>1000</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B47" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B48" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B49" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B50" s="18" t="n">
         <v>0.1</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B51" s="18" t="n">
         <v>0.4</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B52" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B53" s="18" t="n">
         <v>600</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B54" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B57" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B58" s="18" t="n">
         <v>0.9</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B59" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B60" s="18" t="n">
         <v>15</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B61" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="C62" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B63" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B64" s="18" t="n">
         <v>0.2</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B65" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B66" s="18" t="n">
         <v>0.09</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B67" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B68" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B70" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B71" s="18" t="n">
         <v>1100</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B72" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B73" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B74" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2665,17 +2658,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -2691,10 +2684,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>177</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>178</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2704,10 +2697,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>79</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -2717,10 +2710,10 @@
     </row>
     <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -2730,10 +2723,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>180</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>181</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2743,10 +2736,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>183</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2756,10 +2749,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>185</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2775,21 +2768,21 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="32" t="n">
         <v>0</v>
@@ -2803,7 +2796,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="18" t="n">
         <v>10</v>
@@ -2848,17 +2841,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -4912,10 +4905,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>188</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -5942,10 +5935,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>189</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>190</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -6972,10 +6965,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>191</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>192</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -8002,10 +7995,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>193</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>194</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9032,10 +9025,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>195</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>196</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10062,10 +10055,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>197</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>198</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11092,10 +11085,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>199</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>200</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12122,10 +12115,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>201</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>202</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13152,10 +13145,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>203</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>204</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14182,10 +14175,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>205</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>206</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16238,57 +16231,57 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>210</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="G15" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>212</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>213</v>
       </c>
       <c r="I15" s="20" t="n">
         <v>0.6</v>
@@ -16325,17 +16318,17 @@
   </sheetPr>
   <dimension ref="1:30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="20" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18394,10 +18387,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>214</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>215</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -19424,10 +19417,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>216</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>217</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -20454,10 +20447,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>218</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>219</v>
       </c>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
@@ -21484,10 +21477,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>220</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>221</v>
       </c>
       <c r="C6" s="37"/>
       <c r="D6" s="37"/>
@@ -22514,10 +22507,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
@@ -23544,10 +23537,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
@@ -24574,10 +24567,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="37"/>
@@ -25604,10 +25597,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="37"/>
@@ -26634,10 +26627,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="37"/>
@@ -27664,10 +27657,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>227</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>228</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -28694,10 +28687,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>229</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>230</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
@@ -29724,10 +29717,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>231</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>232</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -31779,24 +31772,24 @@
     </row>
     <row r="16" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="D16" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="E16" s="39" t="s">
         <v>235</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>39</v>
@@ -31813,7 +31806,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" s="40" t="s">
         <v>39</v>
@@ -31830,58 +31823,58 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="40" t="s">
         <v>238</v>
       </c>
-      <c r="B19" s="40" t="s">
-        <v>239</v>
-      </c>
       <c r="C19" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>242</v>
-      </c>
       <c r="D21" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E21" s="40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B22" s="40" t="s">
         <v>39</v>
@@ -31898,75 +31891,75 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>244</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="C23" s="40" t="s">
         <v>245</v>
       </c>
-      <c r="C23" s="40" t="s">
-        <v>246</v>
-      </c>
       <c r="D23" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>245</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>242</v>
+        <v>161</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E26" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="40" t="s">
         <v>41</v>
@@ -31983,41 +31976,41 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E29" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B30" s="40" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Created min_renewable_share criterion Only one fuel source without summed max limited by min_renewable_share
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="251">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1171,16 +1171,15 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="A12:D13 A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="B15:B17 A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.3265306122449"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,16 +1379,15 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="1" sqref="A12:D13 C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="B15:B17 C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,7 +1557,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,15 +1805,15 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="A12:D13 B33"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="1" sqref="B15:B17 B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1023" min="4" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -2651,19 +2649,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12:D13"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2806,20 +2803,6 @@
       </c>
       <c r="D12" s="32" t="n">
         <v>0.025</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="C13" s="32" t="n">
-        <v>20</v>
-      </c>
-      <c r="D13" s="32" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2850,17 +2833,17 @@
   <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="A12:D13 B18"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="1" sqref="B15:B17 B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16333,16 +16316,16 @@
   <dimension ref="1:30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="A12:D13 C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="B15:B17 C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="6.47959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="20" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Comments for all experiments, even if no sensitivity necessary
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="261">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -150,10 +150,10 @@
     <t xml:space="preserve">restore_blackouts_if_existant</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
+    <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
-    <t xml:space="preserve">allow_shortage</t>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">evaluated_days</t>
@@ -648,10 +648,10 @@
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
-    <t xml:space="preserve">34_Araceli</t>
+    <t xml:space="preserve">17_Polo</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
+    <t xml:space="preserve">./inputs/timeseries/17_Polo.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand</t>
@@ -664,6 +664,30 @@
   </si>
   <si>
     <t xml:space="preserve">;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34_Araceli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53_Nabuctot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/53_Nabuctot.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121_Tandubanak.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/121_Tandubanak.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126_Pangutaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/126_Pangutaran.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -723,16 +747,22 @@
     <t xml:space="preserve">True or False or default</t>
   </si>
   <si>
-    <t xml:space="preserve">mg_hybrid_no_min</t>
+    <t xml:space="preserve">oem_offgrid</t>
   </si>
   <si>
-    <t xml:space="preserve">mg_hybrid</t>
+    <t xml:space="preserve">mg_grid_consumption</t>
   </si>
   <si>
-    <t xml:space="preserve">solar_battery_mg</t>
+    <t xml:space="preserve">mg_grid_inout</t>
   </si>
   <si>
-    <t xml:space="preserve">diesel_mg</t>
+    <t xml:space="preserve">oem_mg_grid_consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oem_mg_grid_inout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sole_national_grid</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -759,9 +789,6 @@
     <t xml:space="preserve">number_of_equal_generators</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
@@ -775,6 +802,9 @@
   </si>
   <si>
     <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2</t>
   </si>
   <si>
     <t xml:space="preserve">share_hybrid</t>
@@ -926,7 +956,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1059,6 +1089,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1170,17 +1208,17 @@
   </sheetPr>
   <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="49.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,7 +1403,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1380,16 +1418,16 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.10714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,15 +1554,15 @@
         <v>40</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,7 +1706,7 @@
         <v>64</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,7 +1722,7 @@
         <v>66</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,7 +1738,7 @@
         <v>68</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1789,7 @@
         <v>72</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1759,7 +1797,7 @@
         <v>73</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1829,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1806,16 +1844,17 @@
   </sheetPr>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="23" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,7 +1931,7 @@
         <v>86</v>
       </c>
       <c r="B8" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>87</v>
@@ -1903,7 +1942,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="18" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>89</v>
@@ -1914,7 +1953,7 @@
         <v>90</v>
       </c>
       <c r="B10" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>87</v>
@@ -2631,13 +2670,14 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="2">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2652,18 +2692,18 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="20" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,31 +2821,31 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="32" t="n">
+      <c r="A11" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="C11" s="32" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D11" s="32" t="n">
-        <v>0.025</v>
+      <c r="C11" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="18" t="n">
+      <c r="A12" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="24" t="n">
-        <v>20</v>
-      </c>
-      <c r="D12" s="32" t="n">
-        <v>5</v>
+      <c r="D12" s="20" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2860,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2833,20 +2873,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:15"/>
+  <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="17" min="3" style="20" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="20" width="6.88265306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="31.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="20" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="20" width="6.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16254,12 +16294,10 @@
       <c r="H14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="I14" s="24" t="s">
-        <v>132</v>
-      </c>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="33" t="s">
         <v>207</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -16268,23 +16306,124 @@
       <c r="C15" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="35" t="s">
         <v>161</v>
       </c>
       <c r="H15" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="I15" s="20" t="n">
-        <v>0.6</v>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -16303,7 +16442,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -16316,19 +16455,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:30"/>
+  <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="20" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="20" width="6.88265306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="20" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="20" width="6.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17360,7 +17499,7 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18387,16 +18526,16 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
@@ -19416,14 +19555,14 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20446,14 +20585,14 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21476,14 +21615,14 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22506,14 +22645,14 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23536,14 +23675,14 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -24566,14 +24705,14 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="A9" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -25596,14 +25735,14 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -26626,14 +26765,14 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="A11" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -27656,14 +27795,14 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -28686,14 +28825,14 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -29716,14 +29855,14 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -31770,258 +31909,348 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>234</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>235</v>
+    <row r="16" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="40" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>39</v>
+      <c r="A17" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="B18" s="40" t="s">
+      <c r="A18" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="F18" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="G18" s="42" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
-        <v>237</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>161</v>
+      <c r="A19" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>161</v>
+      <c r="A20" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="40" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="C21" s="42" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>238</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>241</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>241</v>
+      <c r="D21" s="42" t="s">
+        <v>240</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>41</v>
+      <c r="A22" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="42" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>245</v>
+      <c r="A23" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="B24" s="40" t="s">
+      <c r="A24" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>161</v>
+      <c r="C24" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B25" s="40" t="s">
+      <c r="A25" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="E25" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="F25" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="G25" s="42" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B26" s="40" t="s">
+      <c r="A26" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="42" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>41</v>
+      <c r="C27" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>249</v>
+      <c r="A28" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>258</v>
+      </c>
+      <c r="G28" s="42" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>250</v>
+      <c r="A29" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" s="40" t="s">
+      <c r="A30" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -32032,7 +32261,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Created busses and components needed for dc bus Added title_demand_ac/title_demand_dc to excel template
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="263">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -648,6 +648,12 @@
     <t xml:space="preserve">project_site_name</t>
   </si>
   <si>
+    <t xml:space="preserve">title_demand_ac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title_demand_dc</t>
+  </si>
+  <si>
     <t xml:space="preserve">17_Polo</t>
   </si>
   <si>
@@ -1418,7 +1424,7 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -2875,18 +2881,23 @@
   </sheetPr>
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="31.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="3" style="20" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="20" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="20" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="20" width="6.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2899,9 +2910,9 @@
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="0"/>
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
@@ -3925,9 +3936,9 @@
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -4952,12 +4963,12 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="23"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="15"/>
       <c r="G3" s="23"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="0"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -5982,12 +5993,12 @@
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="23"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="0"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="0"/>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
@@ -7012,12 +7023,12 @@
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="23"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="0"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="15"/>
       <c r="K5" s="0"/>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
@@ -8042,12 +8053,12 @@
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="0"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="0"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="15"/>
       <c r="K6" s="0"/>
       <c r="L6" s="0"/>
       <c r="M6" s="0"/>
@@ -9072,12 +9083,12 @@
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="0"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="0"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
@@ -10102,12 +10113,12 @@
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="0"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="0"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
@@ -11132,12 +11143,12 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="0"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="0"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="15"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
@@ -12162,12 +12173,12 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="0"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="0"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
@@ -13192,12 +13203,12 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="0"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="0"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="15"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
@@ -14222,12 +14233,12 @@
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="0"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="0"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
@@ -15251,9 +15262,9 @@
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
@@ -16280,150 +16291,168 @@
         <v>194</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="E14" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="G15" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="H15" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H15" s="20" t="s">
-        <v>212</v>
+      <c r="I15" s="20" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G16" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>212</v>
+      <c r="I16" s="20" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G17" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H17" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H17" s="20" t="s">
-        <v>212</v>
+      <c r="I17" s="20" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G18" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H18" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H18" s="20" t="s">
-        <v>212</v>
+      <c r="I18" s="20" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>161</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G19" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>212</v>
+      <c r="I19" s="20" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -18526,10 +18555,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -19556,10 +19585,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -20586,10 +20615,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -21616,10 +21645,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -22646,10 +22675,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -23676,10 +23705,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>230</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>228</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -24706,10 +24735,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -25736,10 +25765,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -26769,7 +26798,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -27796,10 +27825,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -28826,10 +28855,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -29856,10 +29885,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -31911,30 +31940,30 @@
     </row>
     <row r="16" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>42</v>
@@ -31957,7 +31986,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>39</v>
@@ -31980,76 +32009,76 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>42</v>
@@ -32072,53 +32101,53 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>161</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B25" s="42" t="s">
         <v>161</v>
@@ -32127,13 +32156,13 @@
         <v>161</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>161</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="G25" s="42" t="s">
         <v>161</v>
@@ -32141,7 +32170,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B26" s="42" t="s">
         <v>161</v>
@@ -32187,45 +32216,45 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G29" s="42" t="s">
         <v>39</v>
@@ -32233,7 +32262,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Created busses and components needed for dc bus Added title_demand_ac/title_demand_dc to excel template, preprocessing, sensitivity
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="265">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -288,7 +288,7 @@
     <t xml:space="preserve">blackout_duration_std_deviation</t>
   </si>
   <si>
-    <t xml:space="preserve">factor</t>
+    <t xml:space="preserve">fraction</t>
   </si>
   <si>
     <t xml:space="preserve">blackout_frequency</t>
@@ -306,7 +306,13 @@
     <t xml:space="preserve">kWh/l</t>
   </si>
   <si>
-    <t xml:space="preserve">demand_scaling_factor</t>
+    <t xml:space="preserve">demand_ac_scaling_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demand_dc_scaling_factor</t>
   </si>
   <si>
     <t xml:space="preserve">distribution_grid_cost_investment</t>
@@ -1848,10 +1854,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1984,18 +1990,18 @@
         <v>1</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>94</v>
-      </c>
-      <c r="B13" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2020,7 @@
         <v>98</v>
       </c>
       <c r="B15" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>99</v>
@@ -2025,7 +2031,7 @@
         <v>100</v>
       </c>
       <c r="B16" s="18" t="n">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>101</v>
@@ -2036,7 +2042,7 @@
         <v>102</v>
       </c>
       <c r="B17" s="18" t="n">
-        <v>650</v>
+        <v>0.5</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>103</v>
@@ -2047,7 +2053,7 @@
         <v>104</v>
       </c>
       <c r="B18" s="18" t="n">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>105</v>
@@ -2069,40 +2075,40 @@
         <v>108</v>
       </c>
       <c r="B20" s="18" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B21" s="18" t="n">
-        <v>20</v>
+        <v>0.33</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B22" s="18" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B23" s="18" t="n">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>87</v>
@@ -2110,16 +2116,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B24" s="18" t="n">
-        <v>1.2</v>
+        <v>0.15</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,9 +2130,12 @@
         <v>114</v>
       </c>
       <c r="B25" s="18" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2138,21 +2144,21 @@
         <v>116</v>
       </c>
       <c r="B26" s="18" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,37 +2177,37 @@
         <v>121</v>
       </c>
       <c r="B29" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>122</v>
-      </c>
-      <c r="B30" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B31" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B32" s="18" t="n">
         <v>0</v>
@@ -2212,21 +2218,21 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B33" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B34" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>103</v>
@@ -2234,7 +2240,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="18" t="n">
         <v>0</v>
@@ -2245,7 +2251,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="18" t="n">
         <v>0</v>
@@ -2256,49 +2262,49 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="18" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B38" s="18" t="n">
-        <v>20</v>
+        <v>0.95</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B39" s="18" t="n">
-        <v>1.05</v>
+        <v>20</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B40" s="18" t="n">
-        <v>0.89</v>
+        <v>1.05</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>133</v>
+        <v>94</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,15 +2312,15 @@
         <v>134</v>
       </c>
       <c r="B41" s="18" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" s="18" t="n">
         <v>0</v>
@@ -2325,10 +2331,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B43" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>99</v>
@@ -2336,13 +2342,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B44" s="18" t="n">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2356,7 @@
         <v>139</v>
       </c>
       <c r="B45" s="18" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>140</v>
@@ -2361,7 +2367,7 @@
         <v>141</v>
       </c>
       <c r="B46" s="18" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>142</v>
@@ -2375,62 +2381,62 @@
         <v>0</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B48" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B49" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B50" s="18" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B51" s="18" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B52" s="18" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,21 +2444,21 @@
         <v>150</v>
       </c>
       <c r="B53" s="18" t="n">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B54" s="18" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,25 +2469,25 @@
         <v>0</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B56" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B57" s="27" t="n">
+        <v>156</v>
+      </c>
+      <c r="B57" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C57" s="15" t="s">
@@ -2490,10 +2496,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B58" s="18" t="n">
-        <v>0.9</v>
+        <v>157</v>
+      </c>
+      <c r="B58" s="27" t="n">
+        <v>1</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>87</v>
@@ -2501,10 +2507,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B59" s="18" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>87</v>
@@ -2512,54 +2518,54 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B60" s="18" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B61" s="18" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B62" s="18" t="s">
         <v>161</v>
       </c>
+      <c r="B62" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="C62" s="15" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B63" s="18" t="n">
-        <v>1</v>
-      </c>
       <c r="C63" s="15" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B64" s="18" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>87</v>
@@ -2567,10 +2573,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B65" s="18" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>87</v>
@@ -2578,10 +2584,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B66" s="18" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>87</v>
@@ -2589,10 +2595,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B67" s="18" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>87</v>
@@ -2600,7 +2606,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B68" s="18" t="n">
         <v>0</v>
@@ -2611,7 +2617,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>0</v>
@@ -2622,21 +2628,21 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B70" s="18" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B71" s="18" t="n">
-        <v>1100</v>
+        <v>0.5</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>103</v>
@@ -2644,10 +2650,10 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B72" s="18" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>105</v>
@@ -2655,7 +2661,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B73" s="18" t="n">
         <v>0</v>
@@ -2666,17 +2672,27 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="18" t="n">
         <v>20</v>
       </c>
-      <c r="C74" s="15" t="s">
-        <v>99</v>
+      <c r="C75" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="2">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
@@ -2714,7 +2730,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -2730,10 +2746,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2759,7 +2775,7 @@
         <v>81</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -2769,10 +2785,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2782,10 +2798,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2795,10 +2811,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2817,13 +2833,13 @@
         <v>81</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2881,18 +2897,18 @@
   </sheetPr>
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="31.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="20" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="20" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.42"/>
@@ -2902,7 +2918,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -4956,10 +4972,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -5986,10 +6002,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -7016,10 +7032,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -8046,10 +8062,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9076,10 +9092,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10106,10 +10122,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11136,10 +11152,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12166,10 +12182,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13196,10 +13212,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14226,10 +14242,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16282,177 +16298,177 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="H16" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>216</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H18" s="35" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H19" s="35" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -18555,10 +18571,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -19585,10 +19601,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -20615,10 +20631,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -21645,10 +21661,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -22675,10 +22691,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -23705,10 +23721,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="38" t="s">
         <v>232</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>230</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -24735,10 +24751,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -25765,10 +25781,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -26798,7 +26814,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -27825,10 +27841,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -28855,10 +28871,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -29885,10 +29901,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -31940,30 +31956,30 @@
     </row>
     <row r="16" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>42</v>
@@ -31986,7 +32002,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>39</v>
@@ -32009,76 +32025,76 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>42</v>
@@ -32101,94 +32117,94 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32216,45 +32232,45 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G29" s="42" t="s">
         <v>39</v>
@@ -32262,7 +32278,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
NOT working interimstate of dc bus
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="277">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -556,6 +556,42 @@
   </si>
   <si>
     <t xml:space="preserve">wind_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_lifetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_efficiency</t>
   </si>
   <si>
     <t xml:space="preserve">Definition of sensitivity parameters</t>
@@ -1854,10 +1890,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2690,6 +2726,138 @@
       </c>
       <c r="C75" s="15" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B82" s="18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B84" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B86" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" s="10" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +2898,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -2746,10 +2914,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2775,7 +2943,7 @@
         <v>81</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -2785,10 +2953,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2798,10 +2966,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2811,10 +2979,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2833,13 +3001,13 @@
         <v>81</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,7 +3086,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -4972,10 +5140,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -6002,10 +6170,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -7032,10 +7200,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -8062,10 +8230,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9092,10 +9260,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10122,10 +10290,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11152,10 +11320,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12182,10 +12350,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13212,10 +13380,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14242,10 +14410,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16298,177 +16466,177 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>196</v>
-      </c>
       <c r="D14" s="0" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="33" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>163</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H15" s="35" t="s">
         <v>163</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>163</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>163</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>163</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H17" s="35" t="s">
         <v>163</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>163</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H18" s="35" t="s">
         <v>163</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>163</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>163</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="H19" s="35" t="s">
         <v>163</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -18571,10 +18739,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -19601,10 +19769,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -20631,10 +20799,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -21661,10 +21829,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -22691,10 +22859,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -23721,10 +23889,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -24751,10 +24919,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -25781,10 +25949,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -26814,7 +26982,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -27841,10 +28009,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -28871,10 +29039,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -29901,10 +30069,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -31956,30 +32124,30 @@
     </row>
     <row r="16" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>42</v>
@@ -32002,7 +32170,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>39</v>
@@ -32025,76 +32193,76 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="F19" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="F20" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="D21" s="42" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="F21" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="G21" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="40" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>42</v>
@@ -32117,53 +32285,53 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="40" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="B24" s="42" t="s">
         <v>163</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B25" s="42" t="s">
         <v>163</v>
@@ -32172,13 +32340,13 @@
         <v>163</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="E25" s="42" t="s">
         <v>163</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="G25" s="42" t="s">
         <v>163</v>
@@ -32186,7 +32354,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B26" s="42" t="s">
         <v>163</v>
@@ -32232,45 +32400,45 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="40" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="40" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="G29" s="42" t="s">
         <v>39</v>
@@ -32278,7 +32446,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Major updates! * Added DC bus including rectifier/inverter (testing needed -> Flows, calculated values) * Enabled demand AC + demand DC (testing needed -> Flows, calculated values) * PV charge only through battery can be enabled by not inluding a rectifier (testing needed -> Flows, calculated values) * New Constraint: Linearized forced charge when national grid available (test!) * New Constraint: Discharge of battery only when maingrid experiences blackout (test!) * New Constraint: Inverter from DC to AC bus only active when blackout occurs (test!) * New Constraint -> Shortage per timestep is in work
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="277">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -435,13 +435,13 @@
     <t xml:space="preserve">/l</t>
   </si>
   <si>
-    <t xml:space="preserve">project_cost_fix</t>
+    <t xml:space="preserve">project_cost_investment</t>
   </si>
   <si>
     <t xml:space="preserve">project_cost_opex</t>
   </si>
   <si>
-    <t xml:space="preserve">project_life</t>
+    <t xml:space="preserve">project_lifetime</t>
   </si>
   <si>
     <t xml:space="preserve">pv_batch</t>
@@ -469,6 +469,9 @@
   </si>
   <si>
     <t xml:space="preserve">shortage_max_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shortage_max_timestep</t>
   </si>
   <si>
     <t xml:space="preserve">shortage_penalty_costs</t>
@@ -696,10 +699,10 @@
     <t xml:space="preserve">title_demand_dc</t>
   </si>
   <si>
-    <t xml:space="preserve">17_Polo</t>
+    <t xml:space="preserve">34_Araceli</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/17_Polo.csv</t>
+    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand</t>
@@ -712,30 +715,6 @@
   </si>
   <si>
     <t xml:space="preserve">;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34_Araceli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/34_Araceli.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53_Nabuctot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/53_Nabuctot.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121_Tandubanak.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/121_Tandubanak.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">126_Pangutaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/126_Pangutaran.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -822,7 +801,25 @@
     <t xml:space="preserve">oem</t>
   </si>
   <si>
+    <t xml:space="preserve">capacity_wind_kW</t>
+  </si>
+  <si>
     <t xml:space="preserve">capacity_storage_kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">force_charge_from_maingrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discharge_only_when_blackout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_rectifier_ac_dc_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity_inverter_dc_ac_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enable_inverter_at_backout</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_genset_kW</t>
@@ -846,9 +843,6 @@
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">capacity_wind_kW</t>
-  </si>
-  <si>
     <t xml:space="preserve">default</t>
   </si>
   <si>
@@ -856,6 +850,12 @@
   </si>
   <si>
     <t xml:space="preserve">share_hybrid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evaluation_perspective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC_system</t>
   </si>
 </sst>
 </file>
@@ -919,7 +919,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,7 +959,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
@@ -1137,14 +1143,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1177,19 +1175,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -1467,7 +1473,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1770,7 +1776,7 @@
         <v>66</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,10 +1896,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2458,10 +2464,10 @@
         <v>148</v>
       </c>
       <c r="B51" s="18" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,10 +2475,10 @@
         <v>149</v>
       </c>
       <c r="B52" s="18" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,21 +2486,21 @@
         <v>150</v>
       </c>
       <c r="B53" s="18" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="B54" s="18" t="n">
-        <v>600</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,21 +2508,21 @@
         <v>153</v>
       </c>
       <c r="B55" s="18" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,17 +2530,17 @@
         <v>156</v>
       </c>
       <c r="B57" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B58" s="27" t="n">
+      <c r="B58" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -2545,8 +2551,8 @@
       <c r="A59" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B59" s="18" t="n">
-        <v>0.9</v>
+      <c r="B59" s="27" t="n">
+        <v>1</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>87</v>
@@ -2557,7 +2563,7 @@
         <v>159</v>
       </c>
       <c r="B60" s="18" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>87</v>
@@ -2568,10 +2574,10 @@
         <v>160</v>
       </c>
       <c r="B61" s="18" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,32 +2585,32 @@
         <v>161</v>
       </c>
       <c r="B62" s="18" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B63" s="18" t="s">
-        <v>163</v>
+      <c r="B63" s="18" t="n">
+        <v>0</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="B64" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,7 +2618,7 @@
         <v>166</v>
       </c>
       <c r="B65" s="18" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>87</v>
@@ -2623,7 +2629,7 @@
         <v>167</v>
       </c>
       <c r="B66" s="18" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>87</v>
@@ -2634,7 +2640,7 @@
         <v>168</v>
       </c>
       <c r="B67" s="18" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>87</v>
@@ -2645,7 +2651,7 @@
         <v>169</v>
       </c>
       <c r="B68" s="18" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>87</v>
@@ -2678,10 +2684,10 @@
         <v>172</v>
       </c>
       <c r="B71" s="18" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,10 +2695,10 @@
         <v>173</v>
       </c>
       <c r="B72" s="18" t="n">
-        <v>1100</v>
+        <v>0.5</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2700,10 +2706,10 @@
         <v>174</v>
       </c>
       <c r="B73" s="18" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,10 +2728,10 @@
         <v>176</v>
       </c>
       <c r="B75" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,10 +2739,10 @@
         <v>177</v>
       </c>
       <c r="B76" s="18" t="n">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,10 +2750,10 @@
         <v>178</v>
       </c>
       <c r="B77" s="18" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,10 +2761,10 @@
         <v>179</v>
       </c>
       <c r="B78" s="18" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,18 +2775,18 @@
         <v>0</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B80" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>101</v>
+      <c r="B80" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,21 +2794,21 @@
         <v>182</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>0.8</v>
+        <v>20</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B82" s="18" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>103</v>
+      <c r="B82" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2810,10 +2816,10 @@
         <v>184</v>
       </c>
       <c r="B83" s="18" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2821,10 +2827,10 @@
         <v>185</v>
       </c>
       <c r="B84" s="18" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,18 +2841,18 @@
         <v>0</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>101</v>
+      <c r="B86" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,9 +2860,20 @@
         <v>188</v>
       </c>
       <c r="B87" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C87" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B88" s="10" t="n">
         <v>0.98</v>
       </c>
-      <c r="C87" s="23" t="s">
+      <c r="C88" s="23" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2880,10 +2897,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2898,7 +2915,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -2914,10 +2931,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2943,7 +2960,7 @@
         <v>81</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -2953,10 +2970,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2966,10 +2983,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2979,10 +2996,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3001,41 +3018,13 @@
         <v>81</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="D11" s="20" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="20" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="20" t="n">
-        <v>1</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3063,10 +3052,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3086,7 +3075,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -5140,10 +5129,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -6170,10 +6159,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -7200,10 +7189,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -8230,10 +8219,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9260,10 +9249,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10290,10 +10279,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11320,10 +11309,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12350,10 +12339,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13380,10 +13369,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14410,10 +14399,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16466,177 +16455,61 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33" t="s">
-        <v>223</v>
+      <c r="A15" s="20" t="s">
+        <v>224</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="E15" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="H15" s="35" t="s">
-        <v>163</v>
+      <c r="G15" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>164</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
         <v>229</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>225</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>226</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -16668,10 +16541,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ30"/>
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17712,7 +17585,7 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18739,16 +18612,16 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
@@ -19768,14 +19641,14 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>240</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
+      <c r="A4" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20798,14 +20671,14 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
+      <c r="A5" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21828,14 +21701,14 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="A6" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22858,14 +22731,14 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="A7" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23888,14 +23761,14 @@
       <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="A8" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -24918,14 +24791,14 @@
       <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
+      <c r="A9" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -25948,14 +25821,14 @@
       <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
+      <c r="A10" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -26978,14 +26851,14 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -28008,14 +27881,14 @@
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
+      <c r="A12" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -29038,14 +28911,14 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="A13" s="36" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -30068,14 +29941,14 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="A14" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -32123,352 +31996,552 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="120.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="s">
-        <v>239</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>256</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>257</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>258</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>259</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>260</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>261</v>
+      <c r="A16" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
-        <v>262</v>
-      </c>
-      <c r="B17" s="42" t="s">
+      <c r="A17" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="40" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="40" t="s">
-        <v>241</v>
-      </c>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="40" t="s">
-        <v>263</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="C19" s="42" t="s">
+      <c r="A19" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="D19" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>264</v>
+      <c r="B19" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="F20" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>264</v>
+      <c r="A20" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="G21" s="42" t="s">
-        <v>267</v>
+      <c r="A21" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="42" t="s">
+      <c r="A22" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="D22" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="F22" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="42" t="s">
+      <c r="H22" s="40" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>270</v>
+      <c r="A23" s="41" t="s">
+        <v>261</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>267</v>
+      <c r="A24" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="40" t="s">
-        <v>272</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="42" t="s">
-        <v>267</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="F25" s="42" t="s">
-        <v>264</v>
-      </c>
-      <c r="G25" s="42" t="s">
-        <v>163</v>
+      <c r="A25" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="40" t="s">
-        <v>273</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="F26" s="42" t="s">
-        <v>163</v>
-      </c>
-      <c r="G26" s="42" t="s">
-        <v>163</v>
+      <c r="A26" s="41" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="42" t="s">
-        <v>42</v>
+      <c r="A27" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="C28" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="F28" s="42" t="s">
-        <v>274</v>
-      </c>
-      <c r="G28" s="42" t="s">
-        <v>275</v>
+      <c r="A28" s="41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="40" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="C29" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>39</v>
+      <c r="A29" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="B30" s="42" t="s">
+      <c r="A30" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="H30" s="40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="E34" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="F34" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="G34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="H34" s="40" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="C35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="D35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="E35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="42" t="s">
+      <c r="F35" s="40" t="s">
         <v>39</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>

</xml_diff>

<commit_message>
Merged versions 4.4 + 10.4 Working on constraints
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="285">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -375,6 +375,24 @@
     <t xml:space="preserve">(only used if estimated through case definition “peak demand”)</t>
   </si>
   <si>
+    <t xml:space="preserve">inverter_dc_ac_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inverter_dc_ac_lifetime</t>
+  </si>
+  <si>
     <t xml:space="preserve">maingrid_distance</t>
   </si>
   <si>
@@ -468,6 +486,24 @@
     <t xml:space="preserve">pv_lifetime</t>
   </si>
   <si>
+    <t xml:space="preserve">rectifier_ac_dc_batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_cost_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rectifier_ac_dc_lifetime</t>
+  </si>
+  <si>
     <t xml:space="preserve">shortage_max_allowed</t>
   </si>
   <si>
@@ -559,42 +595,6 @@
   </si>
   <si>
     <t xml:space="preserve">wind_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rectifier_ac_dc_efficiency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_batch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_cost_opex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_cost_var</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_lifetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inverter_dc_ac_efficiency</t>
   </si>
   <si>
     <t xml:space="preserve">Definition of sensitivity parameters</t>
@@ -864,16 +864,13 @@
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">0.5</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">default</t>
   </si>
   <si>
     <t xml:space="preserve">0.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">share_hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">evaluation_perspective</t>
@@ -1037,7 +1034,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1166,10 +1163,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1212,12 +1205,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1500,7 +1493,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1768,7 +1761,7 @@
         <v>61</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,8 +1918,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B78" activeCellId="0" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2023,7 +2016,7 @@
         <v>88</v>
       </c>
       <c r="B9" s="18" t="n">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>89</v>
@@ -2215,109 +2208,109 @@
         <v>116</v>
       </c>
       <c r="B26" s="18" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="18" t="n">
-        <v>0.15</v>
+        <v>200</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B29" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B30" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="B30" s="10" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>109</v>
+        <v>121</v>
+      </c>
+      <c r="B31" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B32" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B33" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B34" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B35" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,10 +2318,10 @@
         <v>129</v>
       </c>
       <c r="B36" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2347,7 +2340,7 @@
         <v>131</v>
       </c>
       <c r="B38" s="18" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>87</v>
@@ -2358,10 +2351,10 @@
         <v>132</v>
       </c>
       <c r="B39" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,13 +2362,10 @@
         <v>133</v>
       </c>
       <c r="B40" s="18" t="n">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,142 +2373,145 @@
         <v>134</v>
       </c>
       <c r="B41" s="18" t="n">
-        <v>0.89</v>
+        <v>0</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B42" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B43" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B44" s="18" t="n">
-        <v>20</v>
+        <v>0.95</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B45" s="18" t="n">
-        <v>0.5</v>
+        <v>20</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" s="18" t="n">
-        <v>1000</v>
+        <v>1.05</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>142</v>
+        <v>94</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B47" s="18" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B48" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B49" s="18" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B50" s="18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B51" s="18" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B52" s="18" t="n">
-        <v>0.1</v>
+        <v>1000</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>150</v>
-      </c>
-      <c r="B53" s="18" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,106 +2519,106 @@
         <v>151</v>
       </c>
       <c r="B54" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B55" s="18" t="n">
-        <v>600</v>
+        <v>20</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" s="18" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B57" s="18" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B58" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B59" s="27" t="n">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="B59" s="18" t="n">
+        <v>0</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="18" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C60" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B60" s="10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B61" s="18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>87</v>
+        <v>158</v>
+      </c>
+      <c r="B61" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B62" s="18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B63" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>87</v>
@@ -2633,21 +2626,21 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="B64" s="18" t="n">
+        <v>0.2</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>165</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B65" s="18" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>87</v>
@@ -2655,54 +2648,54 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B66" s="18" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B67" s="18" t="n">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B68" s="18" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B70" s="18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>87</v>
@@ -2710,10 +2703,10 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B71" s="18" t="n">
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="B71" s="27" t="n">
+        <v>1</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>87</v>
@@ -2721,57 +2714,57 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B72" s="18" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B73" s="18" t="n">
-        <v>1100</v>
+        <v>1</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B74" s="18" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B75" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C76" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="B76" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,10 +2772,10 @@
         <v>178</v>
       </c>
       <c r="B77" s="18" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2790,10 +2783,10 @@
         <v>179</v>
       </c>
       <c r="B78" s="18" t="n">
-        <v>1000</v>
+        <v>0.2</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2804,7 +2797,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,31 +2805,31 @@
         <v>181</v>
       </c>
       <c r="B80" s="18" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B81" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>101</v>
+      <c r="B81" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="B82" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C82" s="0" t="s">
+      <c r="B82" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2845,10 +2838,10 @@
         <v>184</v>
       </c>
       <c r="B83" s="18" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2856,10 +2849,10 @@
         <v>185</v>
       </c>
       <c r="B84" s="18" t="n">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,10 +2860,10 @@
         <v>186</v>
       </c>
       <c r="B85" s="18" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2881,29 +2874,29 @@
         <v>0</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="C87" s="23" t="s">
-        <v>101</v>
+      <c r="B87" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B88" s="10" t="n">
-        <v>0.98</v>
-      </c>
-      <c r="C88" s="23" t="s">
-        <v>87</v>
+      <c r="B88" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3081,10 +3074,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ20"/>
+  <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16510,7 +16503,6 @@
       <c r="I14" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
@@ -16520,13 +16512,13 @@
         <v>225</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>226</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>227</v>
@@ -16534,8 +16526,8 @@
       <c r="G15" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H15" s="33" t="s">
-        <v>164</v>
+      <c r="H15" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>229</v>
@@ -16549,10 +16541,10 @@
         <v>231</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>226</v>
@@ -16563,8 +16555,8 @@
       <c r="G16" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H16" s="33" t="s">
-        <v>164</v>
+      <c r="H16" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>229</v>
@@ -16578,13 +16570,13 @@
         <v>233</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>226</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>227</v>
@@ -16592,8 +16584,8 @@
       <c r="G17" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H17" s="33" t="s">
-        <v>164</v>
+      <c r="H17" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>229</v>
@@ -16607,10 +16599,10 @@
         <v>235</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>226</v>
@@ -16621,8 +16613,8 @@
       <c r="G18" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H18" s="33" t="s">
-        <v>164</v>
+      <c r="H18" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>229</v>
@@ -16636,13 +16628,13 @@
         <v>237</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>226</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>227</v>
@@ -16650,15 +16642,12 @@
       <c r="G19" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H19" s="33" t="s">
-        <v>164</v>
+      <c r="H19" s="32" t="s">
+        <v>176</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="33"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -16691,8 +16680,8 @@
   </sheetPr>
   <dimension ref="A1:AMF36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17728,7 +17717,7 @@
       <c r="AMF1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18758,7 +18747,7 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="35"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -19776,14 +19765,14 @@
       <c r="AMF3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20802,14 +20791,14 @@
       <c r="AMF4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21828,14 +21817,14 @@
       <c r="AMF5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22854,14 +22843,14 @@
       <c r="AMF6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23880,14 +23869,14 @@
       <c r="AMF7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>247</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -24906,14 +24895,14 @@
       <c r="AMF8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -25932,14 +25921,14 @@
       <c r="AMF9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>245</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -26958,14 +26947,14 @@
       <c r="AMF10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -27984,14 +27973,14 @@
       <c r="AMF11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>251</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -29010,14 +28999,14 @@
       <c r="AMF12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -30036,14 +30025,14 @@
       <c r="AMF13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -32083,423 +32072,423 @@
       <c r="AMF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="38" t="s">
         <v>259</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="38" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="40" t="s">
+      <c r="C17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="B19" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="B19" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="39" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="B20" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>164</v>
+      <c r="B20" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C21" s="40" t="s">
+      <c r="B21" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="39" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="40" t="s">
+      <c r="E23" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="B24" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C24" s="40" t="s">
+      <c r="B24" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="E24" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>164</v>
+      <c r="D24" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="B25" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="40" t="s">
+      <c r="B25" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="39" t="s">
         <v>264</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="39" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="B27" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>164</v>
+      <c r="B27" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="39" t="s">
         <v>275</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="39" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="39" t="s">
         <v>277</v>
       </c>
-      <c r="F30" s="40" t="s">
-        <v>164</v>
+      <c r="F30" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B31" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="F31" s="40" t="s">
-        <v>164</v>
+      <c r="B31" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="39" t="s">
         <v>279</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="39" t="s">
         <v>280</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F33" s="39" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="E34" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="F34" s="40" t="s">
-        <v>282</v>
+      <c r="C34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="B35" s="40" t="s">
+      <c r="B35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="B36" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="C36" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="F36" s="41" t="s">
         <v>284</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>284</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>284</v>
-      </c>
-      <c r="F36" s="42" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New yearly approximated timeseries appropriate sdg leicester testfile
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="291">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -150,6 +150,9 @@
     <t xml:space="preserve">restore_blackouts_if_existant</t>
   </si>
   <si>
+    <t xml:space="preserve">include_shortage_penalty_costs_in_lcoe</t>
+  </si>
+  <si>
     <t xml:space="preserve">allow_shortage</t>
   </si>
   <si>
@@ -204,7 +207,7 @@
     <t xml:space="preserve">output_file</t>
   </si>
   <si>
-    <t xml:space="preserve">results</t>
+    <t xml:space="preserve">results_ac</t>
   </si>
   <si>
     <t xml:space="preserve">Output – files</t>
@@ -699,10 +702,10 @@
     <t xml:space="preserve">title_demand_dc</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2_AC</t>
+    <t xml:space="preserve">Tier4_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T2_ac_week.csv</t>
+    <t xml:space="preserve">./inputs/timeseries/T4_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">power</t>
@@ -720,34 +723,40 @@
     <t xml:space="preserve">,</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/T2_dc_week.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tier4_AC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_ac_week.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier4_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_dc_week.csv</t>
+    <t xml:space="preserve">./inputs/timeseries/T4_ac_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Tier4_AC_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_ac_dc_week.csv</t>
+    <t xml:space="preserve">./inputs/timeseries/T4_ac_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand AC</t>
   </si>
   <si>
     <t xml:space="preserve">Demand DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier2_DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/T2_dc_year.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier2_AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/T2_ac_year.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier2_AC_DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries/T2_ac_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -849,7 +858,7 @@
     <t xml:space="preserve">capacity_inverter_dc_ac_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">enable_inverter_at_backout</t>
+    <t xml:space="preserve">enable_inverter_only_at_backout</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_genset_kW</t>
@@ -1043,7 +1052,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1172,6 +1181,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1214,12 +1227,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1499,10 +1512,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1645,151 +1658,151 @@
         <v>41</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="18" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="19" t="n">
-        <v>43101</v>
+      <c r="C17" s="18" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>47</v>
+      <c r="C18" s="19" t="n">
+        <v>43101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="20"/>
+      <c r="B20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="C21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>54</v>
+      <c r="C24" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="C25" s="18" t="n">
-        <v>0.03</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="20"/>
+      <c r="B26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="18" t="n">
+        <v>0.03</v>
+      </c>
     </row>
-    <row r="27" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="21"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
-      <c r="B28" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="C28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
       <c r="B29" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="21"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="C31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="A32" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>42</v>
-      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="22"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>62</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1810,7 @@
         <v>65</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,7 +1818,7 @@
         <v>66</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,7 +1826,7 @@
         <v>67</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,26 +1834,26 @@
         <v>68</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="21"/>
+      <c r="B39" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="11"/>
       <c r="C40" s="21"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="A41" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
@@ -1859,36 +1872,36 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="21"/>
+      <c r="B44" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="20"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="21"/>
     </row>
     <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>42</v>
-      </c>
+      <c r="A46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="20"/>
     </row>
     <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>73</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>74</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,11 +1909,18 @@
         <v>75</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="7">
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
@@ -1927,8 +1947,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B78" activeCellId="0" sqref="B78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1942,7 +1962,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -1958,10 +1978,10 @@
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1971,10 +1991,10 @@
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -1989,923 +2009,923 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B7" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" s="18" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" s="18" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B10" s="18" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B11" s="18" t="n">
-        <v>8.8</v>
+        <v>9.8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="18" t="n">
         <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B13" s="18" t="n">
         <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B14" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="18" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B17" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B18" s="18" t="n">
         <v>650</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B20" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B21" s="18" t="n">
         <v>0.33</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B22" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B24" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B25" s="18" t="n">
         <v>1.2</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B26" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B27" s="18" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B28" s="18" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B29" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B30" s="10" t="n">
         <v>0.98</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B32" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B33" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B34" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B36" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B37" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B38" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B39" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B40" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B41" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B42" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B43" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B44" s="18" t="n">
         <v>0.95</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B45" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B46" s="18" t="n">
         <v>1.05</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B47" s="18" t="n">
-        <v>0.89</v>
+        <v>0.76</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B48" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B49" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B50" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B51" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B52" s="18" t="n">
-        <v>1000</v>
+        <v>650</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B53" s="18" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B54" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B55" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B56" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B57" s="18" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B58" s="18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B59" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>0.8</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B61" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B62" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B63" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B64" s="18" t="n">
         <v>0.2</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B65" s="18" t="n">
         <v>0.4</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B66" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B67" s="18" t="n">
-        <v>600</v>
+        <v>230</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B68" s="18" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B70" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B71" s="27" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B72" s="18" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B73" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B74" s="18" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B75" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B77" s="18" t="n">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B78" s="18" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B79" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B80" s="18" t="n">
         <v>0.09</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B81" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B82" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B83" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B84" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B85" s="18" t="n">
         <v>1100</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B86" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B87" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B88" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2946,7 +2966,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="15"/>
@@ -2962,10 +2982,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -2975,10 +2995,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -2988,10 +3008,10 @@
     </row>
     <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31"/>
@@ -3001,10 +3021,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3014,10 +3034,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="30" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3027,10 +3047,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="30" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3046,16 +3066,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3083,10 +3103,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ19"/>
+  <dimension ref="A1:AMJ20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3106,7 +3126,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -5160,10 +5180,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
@@ -6190,10 +6210,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -7220,10 +7240,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -8250,10 +8270,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9280,10 +9300,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10310,10 +10330,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11340,10 +11360,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12370,10 +12390,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13400,10 +13420,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14430,10 +14450,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16486,176 +16506,247 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>219</v>
+        <v>220</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="H15" s="32" t="s">
         <v>229</v>
       </c>
+      <c r="H15" s="33" t="s">
+        <v>230</v>
+      </c>
       <c r="I15" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="J15" s="20" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="K15" s="20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>230</v>
+      <c r="J16" s="20" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="K16" s="20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>176</v>
+        <v>237</v>
       </c>
       <c r="F17" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H17" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="J17" s="20" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="K17" s="20" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="E18" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="G18" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="H18" s="33" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="H18" s="32" t="s">
-        <v>229</v>
-      </c>
       <c r="I18" s="20" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="J18" s="20" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="K18" s="20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="J19" s="20" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="K19" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="G19" s="20" t="s">
+      <c r="F20" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="G20" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="H20" s="33" t="s">
         <v>230</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="J20" s="20" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="K20" s="20" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -16688,13 +16779,13 @@
   </sheetPr>
   <dimension ref="A1:AMF36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="20" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="5" style="20" width="6.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
@@ -17725,7 +17816,7 @@
       <c r="AMF1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18748,14 +18839,14 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
@@ -19773,14 +19864,14 @@
       <c r="AMF3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="A4" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20799,14 +20890,14 @@
       <c r="AMF4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>246</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
+      <c r="A5" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21825,14 +21916,14 @@
       <c r="AMF5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
+      <c r="A6" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22851,14 +22942,14 @@
       <c r="AMF6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="A7" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23877,14 +23968,14 @@
       <c r="AMF7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
+      <c r="A8" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -24903,14 +24994,14 @@
       <c r="AMF8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -25929,14 +26020,14 @@
       <c r="AMF9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="A10" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -26955,14 +27046,14 @@
       <c r="AMF10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>253</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="A11" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -27981,14 +28072,14 @@
       <c r="AMF11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
+      <c r="A12" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -29007,14 +29098,14 @@
       <c r="AMF12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>257</v>
-      </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
+      <c r="A13" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -30033,14 +30124,14 @@
       <c r="AMF13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>259</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
+      <c r="A14" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -32080,423 +32171,423 @@
       <c r="AMF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>260</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>262</v>
-      </c>
-      <c r="E16" s="38" t="s">
+      <c r="A16" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="39" t="s">
         <v>263</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>264</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>39</v>
+      <c r="A17" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
-        <v>266</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>267</v>
+      <c r="A19" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
-        <v>268</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>176</v>
+      <c r="A20" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>267</v>
+      <c r="A21" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="39" t="s">
+      <c r="C22" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B23" s="39" t="s">
+      <c r="A23" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="39" t="s">
+      <c r="D23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="E23" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37" t="s">
-        <v>272</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="F24" s="39" t="s">
-        <v>176</v>
+      <c r="A24" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="E24" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="F24" s="40" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>267</v>
+      <c r="A25" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="E25" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B26" s="39" t="s">
+      <c r="A26" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="B26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="39" t="s">
+      <c r="C26" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27" s="39" t="s">
-        <v>176</v>
+      <c r="A27" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="39" t="s">
-        <v>42</v>
+      <c r="A28" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="F29" s="39" t="s">
-        <v>278</v>
+      <c r="A29" s="41" t="s">
+        <v>280</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="B30" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="F30" s="39" t="s">
-        <v>176</v>
+      <c r="A30" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="F30" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="B31" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="F31" s="39" t="s">
-        <v>176</v>
+      <c r="A31" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="39" t="s">
+      <c r="A32" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="39" t="s">
-        <v>42</v>
+      <c r="B32" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="E33" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="F33" s="39" t="s">
-        <v>284</v>
+      <c r="A33" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="E33" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="B34" s="39" t="s">
+      <c r="A34" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="39" t="s">
+      <c r="C34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="37" t="s">
-        <v>258</v>
-      </c>
-      <c r="B35" s="39" t="s">
+      <c r="A35" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="39" t="s">
+      <c r="F35" s="40" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="E36" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>287</v>
+      <c r="A36" s="38" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included input_folder_timeseries, so that copied input timeseries can be named after the original file name Included an estimation of simulation time left
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="295">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t xml:space="preserve">cmdline_option_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_folder_timeseries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./inputs/timeseries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for timeseries</t>
   </si>
   <si>
     <t xml:space="preserve">output_folder</t>
@@ -705,7 +714,7 @@
     <t xml:space="preserve">Tier4_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_dc_year.csv</t>
+    <t xml:space="preserve">T4_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">power</t>
@@ -726,13 +735,13 @@
     <t xml:space="preserve">Tier4_AC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_ac_year.csv</t>
+    <t xml:space="preserve">T4_ac_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Tier4_AC_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T4_ac_dc_year.csv</t>
+    <t xml:space="preserve">T4_ac_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Demand AC</t>
@@ -744,19 +753,19 @@
     <t xml:space="preserve">Tier2_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T2_dc_year.csv</t>
+    <t xml:space="preserve">T2_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Tier2_AC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T2_ac_year.csv</t>
+    <t xml:space="preserve">T2_ac_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Tier2_AC_DC</t>
   </si>
   <si>
-    <t xml:space="preserve">./inputs/timeseries/T2_ac_dc_year.csv</t>
+    <t xml:space="preserve">T2_ac_dc_year.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -1055,7 +1064,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1141,6 +1150,10 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1230,12 +1243,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1515,10 +1528,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1760,115 +1773,119 @@
       </c>
       <c r="C28" s="21"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
       <c r="B29" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="22" t="s">
         <v>58</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
       <c r="B30" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="18" t="s">
         <v>60</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="21"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="22"/>
-      <c r="G32" s="22"/>
+      <c r="C32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="A33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="21"/>
+      <c r="B40" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="11"/>
       <c r="C41" s="21"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="A42" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="21"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>39</v>
@@ -1876,40 +1893,40 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="21"/>
+      <c r="B45" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="20"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="21"/>
     </row>
     <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="A47" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>43</v>
@@ -1917,9 +1934,17 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C50" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1950,7 +1975,7 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
     </sheetView>
   </sheetViews>
@@ -1958,33 +1983,33 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="24"/>
+        <v>80</v>
+      </c>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11"/>
-      <c r="B2" s="24"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1994,10 +2019,10 @@
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
@@ -2007,928 +2032,928 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B7" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B8" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B9" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B10" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B11" s="18" t="n">
         <v>9.8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B12" s="18" t="n">
         <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>95</v>
+      <c r="C12" s="24" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B13" s="18" t="n">
         <f aca="false">1/1000</f>
         <v>0.001</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>95</v>
+      <c r="C13" s="24" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B14" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B15" s="18" t="n">
         <v>10</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B16" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B17" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B18" s="18" t="n">
         <v>650</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B19" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B20" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B21" s="18" t="n">
         <v>0.33</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B22" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B23" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B24" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B25" s="18" t="n">
         <v>1.2</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B26" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B27" s="18" t="n">
         <v>400</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B28" s="18" t="n">
         <v>50</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B29" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B30" s="10" t="n">
         <v>0.98</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>88</v>
+      <c r="C30" s="24" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>102</v>
+      <c r="C31" s="24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B32" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B33" s="18" t="n">
         <v>0.15</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B34" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B35" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B36" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B37" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B38" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B39" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B40" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B41" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B42" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B43" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B44" s="18" t="n">
         <v>0.95</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B45" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B46" s="18" t="n">
         <v>1.05</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B47" s="18" t="n">
         <v>0.76</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B48" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B49" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B50" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B51" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B52" s="18" t="n">
         <v>650</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B53" s="18" t="n">
         <v>8</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B54" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B55" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B56" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B57" s="18" t="n">
         <v>150</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B58" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B59" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B60" s="10" t="n">
         <v>0.8</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B61" s="10" t="n">
         <v>15</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B62" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B63" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B64" s="18" t="n">
         <v>0.2</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B65" s="18" t="n">
         <v>0.4</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B66" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B67" s="18" t="n">
         <v>230</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B68" s="18" t="n">
         <v>15</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B69" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B70" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="B71" s="27" t="n">
+        <v>174</v>
+      </c>
+      <c r="B71" s="28" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B72" s="18" t="n">
         <v>0.8</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B73" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B74" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B75" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B77" s="18" t="n">
         <v>0.95</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B78" s="18" t="n">
         <v>0.3</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B79" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B80" s="18" t="n">
         <v>0.09</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B81" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B82" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B83" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B84" s="18" t="n">
         <v>0.5</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B85" s="18" t="n">
         <v>1100</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B86" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B87" s="18" t="n">
         <v>0</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B88" s="18" t="n">
         <v>20</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2969,65 +2994,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="24"/>
+        <v>194</v>
+      </c>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11"/>
-      <c r="B2" s="24"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="A3" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="A4" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
+      <c r="A5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
-        <v>195</v>
+      <c r="A6" s="31" t="s">
+        <v>198</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3036,11 +3061,11 @@
       <c r="G6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
-        <v>197</v>
+      <c r="A7" s="31" t="s">
+        <v>200</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3049,11 +3074,11 @@
       <c r="G7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="30" t="s">
-        <v>199</v>
+      <c r="A8" s="31" t="s">
+        <v>202</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3069,16 +3094,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3106,10 +3131,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ20"/>
+  <dimension ref="A1:AMI20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3124,12 +3149,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="21" style="20" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -4153,7 +4179,6 @@
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -5179,21 +5204,20 @@
       <c r="AMG2" s="0"/>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
       <c r="I3" s="10"/>
       <c r="J3" s="15"/>
       <c r="K3" s="0"/>
@@ -6209,21 +6233,20 @@
       <c r="AMG3" s="0"/>
       <c r="AMH3" s="0"/>
       <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="A4" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="10"/>
       <c r="J4" s="15"/>
       <c r="K4" s="0"/>
@@ -7239,21 +7262,20 @@
       <c r="AMG4" s="0"/>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="A5" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="10"/>
       <c r="J5" s="15"/>
       <c r="K5" s="0"/>
@@ -8269,14 +8291,13 @@
       <c r="AMG5" s="0"/>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9299,14 +9320,13 @@
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10329,14 +10349,13 @@
       <c r="AMG7" s="0"/>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11359,14 +11378,13 @@
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12389,14 +12407,13 @@
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13419,14 +13436,13 @@
       <c r="AMG10" s="0"/>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14449,14 +14465,13 @@
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -15479,7 +15494,6 @@
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0"/>
@@ -16505,70 +16519,69 @@
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="J14" s="32" t="s">
-        <v>125</v>
+      <c r="J14" s="33" t="s">
+        <v>128</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>233</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J15" s="20" t="n">
         <v>0.079</v>
@@ -16579,31 +16592,31 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="H16" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>227</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>230</v>
-      </c>
       <c r="I16" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>0.079</v>
@@ -16614,66 +16627,66 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="I17" s="20" t="s">
         <v>234</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>236</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>231</v>
       </c>
       <c r="J17" s="20" t="n">
         <v>0.079</v>
       </c>
       <c r="K17" s="20" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>233</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>0.032</v>
@@ -16684,31 +16697,31 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>233</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J19" s="20" t="n">
         <v>0.032</v>
@@ -16719,37 +16732,37 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H20" s="33" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>233</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J20" s="20" t="n">
         <v>0.032</v>
       </c>
       <c r="K20" s="20" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -17820,7 +17833,7 @@
       <c r="AMG1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="34"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18843,16 +18856,16 @@
       <c r="AMG2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="A3" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
@@ -19870,14 +19883,14 @@
       <c r="AMG3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="A4" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20897,14 +20910,14 @@
       <c r="AMG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
+      <c r="A5" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21924,14 +21937,14 @@
       <c r="AMG5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="37" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22951,14 +22964,14 @@
       <c r="AMG6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="A7" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23978,14 +23991,14 @@
       <c r="AMG7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -25005,14 +25018,14 @@
       <c r="AMG8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -26032,14 +26045,14 @@
       <c r="AMG9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -27059,14 +27072,14 @@
       <c r="AMG10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -28086,14 +28099,14 @@
       <c r="AMG11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="A12" s="37" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -29113,14 +29126,14 @@
       <c r="AMG12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="A13" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -30140,14 +30153,14 @@
       <c r="AMG13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
+      <c r="A14" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -32189,486 +32202,486 @@
       <c r="AMG15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
-        <v>246</v>
-      </c>
-      <c r="B16" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>265</v>
-      </c>
-      <c r="E16" s="39" t="s">
+      <c r="A16" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B16" s="40" t="s">
         <v>266</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="C16" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="D16" s="40" t="s">
         <v>268</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="38" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="40" t="s">
+      <c r="A17" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="B18" s="40" t="s">
+      <c r="A18" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
-        <v>270</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G19" s="40" t="s">
-        <v>271</v>
+      <c r="A19" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38" t="s">
-        <v>272</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="G20" s="40" t="s">
-        <v>177</v>
+      <c r="A20" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
-        <v>273</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>271</v>
+      <c r="A21" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="B22" s="40" t="s">
+      <c r="A22" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="B23" s="40" t="s">
+      <c r="A23" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="B23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="38" t="s">
-        <v>276</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>271</v>
+      <c r="A24" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="F25" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G25" s="40" t="s">
-        <v>271</v>
+      <c r="A25" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B26" s="40" t="s">
+      <c r="A26" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="B26" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F27" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="G27" s="40" t="s">
-        <v>177</v>
+      <c r="A27" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41" t="s">
-        <v>280</v>
-      </c>
-      <c r="B28" s="40" t="s">
+      <c r="A28" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="40" t="s">
+      <c r="G28" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41" t="s">
-        <v>281</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="E29" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="F29" s="40" t="s">
-        <v>282</v>
-      </c>
-      <c r="G29" s="40" t="s">
-        <v>282</v>
+      <c r="A29" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38" t="s">
-        <v>283</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="D30" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="F30" s="40" t="s">
-        <v>284</v>
-      </c>
-      <c r="G30" s="40" t="s">
-        <v>177</v>
+      <c r="A30" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="B31" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="D31" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="E31" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F31" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" s="40" t="s">
-        <v>177</v>
+      <c r="A31" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>286</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="D33" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="E33" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="F33" s="40" t="s">
-        <v>287</v>
-      </c>
-      <c r="G33" s="40" t="s">
-        <v>288</v>
+      <c r="A33" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="F33" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>259</v>
-      </c>
-      <c r="B34" s="40" t="s">
+      <c r="A34" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="B34" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="40" t="s">
+      <c r="G34" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38" t="s">
-        <v>261</v>
-      </c>
-      <c r="B35" s="40" t="s">
+      <c r="A35" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="40" t="s">
+      <c r="G35" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="38" t="s">
-        <v>289</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="F36" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="G36" s="42" t="s">
-        <v>291</v>
+      <c r="A36" s="39" t="s">
+        <v>292</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" s="43" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included input_folder_timeseries, so that copied input timeseries can be named after the original file name Included an estimation of simulation time left Execution of simulation tool via command line - multiple inputs possible
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -144,19 +144,19 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
-    <t xml:space="preserve">False</t>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">restore_blackouts_if_existant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">include_shortage_penalty_costs_in_lcoe</t>
   </si>
   <si>
     <t xml:space="preserve">allow_shortage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">evaluated_days</t>
@@ -1530,8 +1530,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1666,23 +1666,23 @@
         <v>40</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1717,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1742,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1819,7 @@
         <v>65</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1827,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>67</v>
@@ -1838,7 +1838,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1846,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1854,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1862,7 @@
         <v>71</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1870,7 @@
         <v>72</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1888,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,7 +1896,7 @@
         <v>74</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,7 +1904,7 @@
         <v>75</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1921,7 @@
         <v>76</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1929,7 +1929,7 @@
         <v>77</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,7 +1937,7 @@
         <v>78</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1945,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -16795,8 +16795,8 @@
   </sheetPr>
   <dimension ref="A1:AMG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27073,7 +27073,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="37" t="s">
         <v>259</v>
@@ -32232,7 +32232,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>39</v>
@@ -32252,22 +32252,22 @@
         <v>251</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32344,22 +32344,22 @@
         <v>277</v>
       </c>
       <c r="B22" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>43</v>
-      </c>
       <c r="D22" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32367,22 +32367,22 @@
         <v>278</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G23" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32436,22 +32436,22 @@
         <v>281</v>
       </c>
       <c r="B26" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G26" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32482,22 +32482,22 @@
         <v>283</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G28" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32571,25 +32571,25 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G32" s="41" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32620,22 +32620,22 @@
         <v>262</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G34" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32643,22 +32643,22 @@
         <v>264</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G35" s="41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
including storage power optimization
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="296">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -534,7 +534,10 @@
     <t xml:space="preserve">kWh</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_cost_investment</t>
+    <t xml:space="preserve">storage_capacity_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_power_cost_investment</t>
   </si>
   <si>
     <t xml:space="preserve">storage_cost_opex</t>
@@ -1243,12 +1246,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1973,10 +1976,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2730,21 +2733,21 @@
         <v>170</v>
       </c>
       <c r="B68" s="18" t="n">
-        <v>15</v>
+        <v>230</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="18" t="n">
+        <v>15</v>
+      </c>
+      <c r="C69" s="15" t="s">
         <v>172</v>
-      </c>
-      <c r="B69" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,17 +2755,17 @@
         <v>173</v>
       </c>
       <c r="B70" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B71" s="28" t="n">
+      <c r="B71" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C71" s="15" t="s">
@@ -2773,8 +2776,8 @@
       <c r="A72" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B72" s="18" t="n">
-        <v>0.8</v>
+      <c r="B72" s="28" t="n">
+        <v>1</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>91</v>
@@ -2785,7 +2788,7 @@
         <v>176</v>
       </c>
       <c r="B73" s="18" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>91</v>
@@ -2796,10 +2799,10 @@
         <v>177</v>
       </c>
       <c r="B74" s="18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,32 +2810,32 @@
         <v>178</v>
       </c>
       <c r="B75" s="18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B76" s="18" t="s">
-        <v>180</v>
+      <c r="B76" s="18" t="n">
+        <v>0</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" s="15" t="s">
         <v>182</v>
-      </c>
-      <c r="B77" s="18" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2840,7 +2843,7 @@
         <v>183</v>
       </c>
       <c r="B78" s="18" t="n">
-        <v>0.3</v>
+        <v>0.95</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>91</v>
@@ -2851,7 +2854,7 @@
         <v>184</v>
       </c>
       <c r="B79" s="18" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C79" s="15" t="s">
         <v>91</v>
@@ -2862,7 +2865,7 @@
         <v>185</v>
       </c>
       <c r="B80" s="18" t="n">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>91</v>
@@ -2873,7 +2876,7 @@
         <v>186</v>
       </c>
       <c r="B81" s="18" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>91</v>
@@ -2906,10 +2909,10 @@
         <v>189</v>
       </c>
       <c r="B84" s="18" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,10 +2920,10 @@
         <v>190</v>
       </c>
       <c r="B85" s="18" t="n">
-        <v>1100</v>
+        <v>0.5</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2928,10 +2931,10 @@
         <v>191</v>
       </c>
       <c r="B86" s="18" t="n">
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2942,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2950,9 +2953,20 @@
         <v>193</v>
       </c>
       <c r="B88" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B89" s="18" t="n">
         <v>20</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C89" s="15" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2994,7 +3008,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="15"/>
@@ -3010,10 +3024,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3039,7 +3053,7 @@
         <v>85</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -3049,10 +3063,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3062,10 +3076,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3075,10 +3089,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3097,13 +3111,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3155,7 +3169,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -5207,10 +5221,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6236,10 +6250,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7265,10 +7279,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8294,10 +8308,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9323,10 +9337,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10352,10 +10366,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11381,10 +11395,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12410,10 +12424,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13439,10 +13453,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14468,10 +14482,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16522,31 +16536,31 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J14" s="33" t="s">
         <v>128</v>
@@ -16557,31 +16571,31 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J15" s="20" t="n">
         <v>0.079</v>
@@ -16592,31 +16606,31 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>234</v>
       </c>
       <c r="J16" s="20" t="n">
         <v>0.079</v>
@@ -16627,31 +16641,31 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J17" s="20" t="n">
         <v>0.079</v>
@@ -16662,31 +16676,31 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H18" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J18" s="20" t="n">
         <v>0.032</v>
@@ -16697,31 +16711,31 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H19" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J19" s="20" t="n">
         <v>0.032</v>
@@ -16732,31 +16746,31 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J20" s="20" t="n">
         <v>0.032</v>
@@ -16795,7 +16809,7 @@
   </sheetPr>
   <dimension ref="A1:AMG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
@@ -18857,10 +18871,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -19884,10 +19898,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -20911,10 +20925,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="37" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -21938,10 +21952,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -22965,10 +22979,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>255</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>254</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
@@ -23992,10 +24006,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -25019,10 +25033,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -26046,10 +26060,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -27076,7 +27090,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -28100,10 +28114,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -29127,10 +29141,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -30154,10 +30168,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="37" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
@@ -32203,30 +32217,30 @@
     </row>
     <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>39</v>
@@ -32249,7 +32263,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B18" s="41" t="s">
         <v>41</v>
@@ -32272,76 +32286,76 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G21" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="42" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>41</v>
@@ -32364,7 +32378,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="42" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>41</v>
@@ -32387,53 +32401,53 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G24" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G25" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="42" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>41</v>
@@ -32456,30 +32470,30 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G27" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="42" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>39</v>
@@ -32502,71 +32516,71 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="42" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G29" s="41" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G31" s="41" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32594,30 +32608,30 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G33" s="41" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B34" s="41" t="s">
         <v>41</v>
@@ -32640,7 +32654,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B35" s="41" t="s">
         <v>41</v>
@@ -32663,25 +32677,25 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F36" s="43" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G36" s="43" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrated power_capacity optimization errors if title_xy wrong stability_constraint corrected for power multiple simulations
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="283">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -144,19 +144,19 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">include_shortage_penalty_costs_in_lcoe</t>
   </si>
   <si>
     <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">evaluated_days</t>
@@ -216,7 +216,7 @@
     <t xml:space="preserve">output_file</t>
   </si>
   <si>
-    <t xml:space="preserve">results_ac</t>
+    <t xml:space="preserve">results</t>
   </si>
   <si>
     <t xml:space="preserve">Output – files</t>
@@ -528,22 +528,25 @@
     <t xml:space="preserve">stability_limit</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_batch</t>
+    <t xml:space="preserve">storage_batch_capacity</t>
   </si>
   <si>
     <t xml:space="preserve">kWh</t>
   </si>
   <si>
+    <t xml:space="preserve">storage_batch_power</t>
+  </si>
+  <si>
     <t xml:space="preserve">storage_capacity_cost_investment</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_power_cost_investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">storage_cost_opex</t>
+    <t xml:space="preserve">storage_capacity_cost_opex</t>
   </si>
   <si>
     <t xml:space="preserve">/kWh/a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_capacity_lifetime</t>
   </si>
   <si>
     <t xml:space="preserve">storage_cost_var</t>
@@ -561,10 +564,16 @@
     <t xml:space="preserve">storage_efficiency_discharge</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_lifetime</t>
+    <t xml:space="preserve">storage_loss_timestep</t>
   </si>
   <si>
-    <t xml:space="preserve">storage_loss_timestep</t>
+    <t xml:space="preserve">storage_power_cost_investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_power_cost_opex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_power_lifetime</t>
   </si>
   <si>
     <t xml:space="preserve">storage_soc_initial</t>
@@ -714,13 +723,13 @@
     <t xml:space="preserve">title_demand_dc</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier4_DC</t>
+    <t xml:space="preserve">Profile_01</t>
   </si>
   <si>
-    <t xml:space="preserve">T4_dc_year.csv</t>
+    <t xml:space="preserve">intermediate_tier2.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">power</t>
+    <t xml:space="preserve">profile_1</t>
   </si>
   <si>
     <t xml:space="preserve">SolarGen</t>
@@ -729,46 +738,7 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">GridAvailability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier4_AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T4_ac_year.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier4_AC_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T4_ac_dc_year.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier2_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T2_dc_year.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier2_AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T2_ac_year.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier2_AC_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T2_ac_dc_year.csv</t>
+    <t xml:space="preserve">;</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -828,22 +798,16 @@
     <t xml:space="preserve">True or False or default</t>
   </si>
   <si>
-    <t xml:space="preserve">sole_maingrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_battery_forced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_battery_foresight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_shs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parallel_shs</t>
+    <t xml:space="preserve">mg</t>
   </si>
   <si>
     <t xml:space="preserve">offgrid_shs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_grid_cons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_grid_cons_prod</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -897,13 +861,10 @@
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">0.02</t>
+    <t xml:space="preserve">share_hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">evaluation_perspective</t>
@@ -1533,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,23 +1630,23 @@
         <v>40</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,7 +1654,7 @@
         <v>44</v>
       </c>
       <c r="C17" s="18" t="n">
-        <v>365</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1681,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1706,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,7 +1783,7 @@
         <v>65</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,7 +1791,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>67</v>
@@ -1841,7 +1802,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,7 +1810,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1857,7 +1818,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,7 +1826,7 @@
         <v>71</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,7 +1834,7 @@
         <v>72</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,7 +1852,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,7 +1860,7 @@
         <v>74</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1907,7 +1868,7 @@
         <v>75</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +1885,7 @@
         <v>76</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1932,7 +1893,7 @@
         <v>77</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,7 +1901,7 @@
         <v>78</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,7 +1909,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1976,10 +1937,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2121,8 +2082,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="18" t="n">
-        <f aca="false">1/1000</f>
-        <v>0.001</v>
+        <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>98</v>
@@ -2144,7 +2104,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>103</v>
@@ -2155,7 +2115,7 @@
         <v>104</v>
       </c>
       <c r="B16" s="18" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>105</v>
@@ -2177,7 +2137,7 @@
         <v>108</v>
       </c>
       <c r="B18" s="18" t="n">
-        <v>650</v>
+        <v>820</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>109</v>
@@ -2221,7 +2181,7 @@
         <v>115</v>
       </c>
       <c r="B22" s="18" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>105</v>
@@ -2243,7 +2203,7 @@
         <v>117</v>
       </c>
       <c r="B24" s="18" t="n">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>91</v>
@@ -2279,7 +2239,7 @@
         <v>121</v>
       </c>
       <c r="B27" s="18" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>109</v>
@@ -2290,7 +2250,7 @@
         <v>122</v>
       </c>
       <c r="B28" s="18" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>111</v>
@@ -2312,7 +2272,7 @@
         <v>124</v>
       </c>
       <c r="B30" s="10" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>91</v>
@@ -2345,7 +2305,7 @@
         <v>128</v>
       </c>
       <c r="B33" s="18" t="n">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>113</v>
@@ -2378,7 +2338,7 @@
         <v>133</v>
       </c>
       <c r="B36" s="18" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>132</v>
@@ -2433,7 +2393,7 @@
         <v>138</v>
       </c>
       <c r="B41" s="18" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>109</v>
@@ -2466,7 +2426,7 @@
         <v>141</v>
       </c>
       <c r="B44" s="18" t="n">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>91</v>
@@ -2502,7 +2462,7 @@
         <v>144</v>
       </c>
       <c r="B47" s="18" t="n">
-        <v>0.76</v>
+        <v>0.63</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>145</v>
@@ -2513,7 +2473,7 @@
         <v>146</v>
       </c>
       <c r="B48" s="18" t="n">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>101</v>
@@ -2557,7 +2517,7 @@
         <v>151</v>
       </c>
       <c r="B52" s="18" t="n">
-        <v>650</v>
+        <v>1250</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>152</v>
@@ -2568,7 +2528,7 @@
         <v>153</v>
       </c>
       <c r="B53" s="18" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>154</v>
@@ -2590,7 +2550,7 @@
         <v>156</v>
       </c>
       <c r="B55" s="18" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>105</v>
@@ -2612,7 +2572,7 @@
         <v>158</v>
       </c>
       <c r="B57" s="18" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>109</v>
@@ -2623,7 +2583,7 @@
         <v>159</v>
       </c>
       <c r="B58" s="18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>111</v>
@@ -2645,7 +2605,7 @@
         <v>161</v>
       </c>
       <c r="B60" s="10" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>91</v>
@@ -2722,10 +2682,10 @@
         <v>169</v>
       </c>
       <c r="B67" s="18" t="n">
-        <v>230</v>
+        <v>1</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2733,10 +2693,10 @@
         <v>170</v>
       </c>
       <c r="B68" s="18" t="n">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2744,7 +2704,7 @@
         <v>171</v>
       </c>
       <c r="B69" s="18" t="n">
-        <v>15</v>
+        <v>6.75</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>172</v>
@@ -2755,7 +2715,7 @@
         <v>173</v>
       </c>
       <c r="B70" s="18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>105</v>
@@ -2766,17 +2726,17 @@
         <v>174</v>
       </c>
       <c r="B71" s="18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B72" s="28" t="n">
+      <c r="B72" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C72" s="15" t="s">
@@ -2787,8 +2747,8 @@
       <c r="A73" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B73" s="18" t="n">
-        <v>0.8</v>
+      <c r="B73" s="28" t="n">
+        <v>0.5</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>91</v>
@@ -2799,7 +2759,7 @@
         <v>177</v>
       </c>
       <c r="B74" s="18" t="n">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>91</v>
@@ -2810,10 +2770,10 @@
         <v>178</v>
       </c>
       <c r="B75" s="18" t="n">
-        <v>5</v>
+        <v>0.97</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,44 +2791,44 @@
       <c r="A77" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B77" s="18" t="s">
-        <v>181</v>
+      <c r="B77" s="18" t="n">
+        <v>500</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>182</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B78" s="18" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B79" s="18" t="n">
-        <v>0.3</v>
+        <v>5</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C80" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="B80" s="18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2876,7 +2836,7 @@
         <v>186</v>
       </c>
       <c r="B81" s="18" t="n">
-        <v>0.09</v>
+        <v>1</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>91</v>
@@ -2887,7 +2847,7 @@
         <v>187</v>
       </c>
       <c r="B82" s="18" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>91</v>
@@ -2909,7 +2869,7 @@
         <v>189</v>
       </c>
       <c r="B84" s="18" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>91</v>
@@ -2920,10 +2880,10 @@
         <v>190</v>
       </c>
       <c r="B85" s="18" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2931,10 +2891,10 @@
         <v>191</v>
       </c>
       <c r="B86" s="18" t="n">
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,7 +2905,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2953,10 +2913,10 @@
         <v>193</v>
       </c>
       <c r="B88" s="18" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,9 +2924,42 @@
         <v>194</v>
       </c>
       <c r="B89" s="18" t="n">
+        <v>1100</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B90" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B91" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B92" s="18" t="n">
         <v>20</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C92" s="15" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2990,10 +2983,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3008,7 +3001,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="15"/>
@@ -3024,10 +3017,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -3053,7 +3046,7 @@
         <v>85</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -3063,10 +3056,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -3076,10 +3069,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3089,10 +3082,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3111,13 +3104,27 @@
         <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -3145,10 +3152,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI20"/>
+  <dimension ref="A1:AMI18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3169,7 +3176,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -5221,10 +5228,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6250,10 +6257,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7279,10 +7286,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8308,10 +8315,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9337,10 +9344,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10366,10 +10373,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11395,10 +11402,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12424,10 +12431,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13453,10 +13460,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14482,10 +14489,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16536,249 +16543,65 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="J14" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>100</v>
-      </c>
+      <c r="J14" s="33"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>231</v>
+        <v>184</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>234</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J15" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K15" s="20" t="n">
-        <v>0</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J16" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K16" s="20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J17" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K17" s="20" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J18" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K18" s="20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J19" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K19" s="20" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="J20" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K20" s="20" t="n">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B3:D3"/>
@@ -16809,8 +16632,8 @@
   </sheetPr>
   <dimension ref="A1:AMG36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18871,10 +18694,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -19898,10 +19721,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="37" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
@@ -20925,10 +20748,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="37" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -21952,10 +21775,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="37" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
@@ -22979,10 +22802,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="38"/>
@@ -24006,10 +23829,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="38"/>
@@ -25033,10 +24856,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="37" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -26060,10 +25883,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
@@ -27087,10 +26910,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="38"/>
@@ -28114,10 +27937,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -29141,10 +28964,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -30168,10 +29991,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="37" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
@@ -32215,38 +32038,36 @@
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="85.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="39" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>272</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="AMD16" s="0"/>
+      <c r="AME16" s="0"/>
+      <c r="AMF16" s="0"/>
+      <c r="AMG16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="39" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>39</v>
@@ -32254,203 +32075,185 @@
       <c r="E17" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>39</v>
-      </c>
+      <c r="AMD17" s="0"/>
+      <c r="AME17" s="0"/>
+      <c r="AMF17" s="0"/>
+      <c r="AMG17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>41</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AMD18" s="0"/>
+      <c r="AME18" s="0"/>
+      <c r="AMF18" s="0"/>
+      <c r="AMG18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="39" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="F19" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>275</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AMD19" s="0"/>
+      <c r="AME19" s="0"/>
+      <c r="AMF19" s="0"/>
+      <c r="AMG19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="39" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>181</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="AMD20" s="0"/>
+      <c r="AME20" s="0"/>
+      <c r="AMF20" s="0"/>
+      <c r="AMG20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="39" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D21" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>275</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
+      <c r="AMF21" s="0"/>
+      <c r="AMG21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="42" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>41</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AMD22" s="0"/>
+      <c r="AME22" s="0"/>
+      <c r="AMF22" s="0"/>
+      <c r="AMG22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="42" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>41</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AMD23" s="0"/>
+      <c r="AME23" s="0"/>
+      <c r="AMF23" s="0"/>
+      <c r="AMG23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="39" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>275</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AMD24" s="0"/>
+      <c r="AME24" s="0"/>
+      <c r="AMF24" s="0"/>
+      <c r="AMG24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="39" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D25" s="41" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>275</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AMD25" s="0"/>
+      <c r="AME25" s="0"/>
+      <c r="AMF25" s="0"/>
+      <c r="AMG25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="42" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="41" t="s">
         <v>39</v>
@@ -32461,39 +32264,35 @@
       <c r="E26" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="AMD26" s="0"/>
+      <c r="AME26" s="0"/>
+      <c r="AMF26" s="0"/>
+      <c r="AMG26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="39" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>181</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="AMD27" s="0"/>
+      <c r="AME27" s="0"/>
+      <c r="AMF27" s="0"/>
+      <c r="AMG27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="42" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B28" s="41" t="s">
         <v>39</v>
@@ -32507,196 +32306,178 @@
       <c r="E28" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="41" t="s">
-        <v>39</v>
-      </c>
+      <c r="AMD28" s="0"/>
+      <c r="AME28" s="0"/>
+      <c r="AMF28" s="0"/>
+      <c r="AMG28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="42" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="G29" s="41" t="s">
-        <v>286</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="AMD29" s="0"/>
+      <c r="AME29" s="0"/>
+      <c r="AMF29" s="0"/>
+      <c r="AMG29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="39" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>288</v>
+        <v>184</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>288</v>
+        <v>184</v>
       </c>
       <c r="D30" s="41" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>288</v>
-      </c>
-      <c r="F30" s="41" t="s">
-        <v>288</v>
-      </c>
-      <c r="G30" s="41" t="s">
-        <v>181</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="AMD30" s="0"/>
+      <c r="AME30" s="0"/>
+      <c r="AMF30" s="0"/>
+      <c r="AMG30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="F31" s="41" t="s">
-        <v>181</v>
-      </c>
-      <c r="G31" s="41" t="s">
-        <v>181</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="AMD31" s="0"/>
+      <c r="AME31" s="0"/>
+      <c r="AMF31" s="0"/>
+      <c r="AMG31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="41" t="s">
-        <v>39</v>
-      </c>
       <c r="C32" s="41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="41" t="s">
-        <v>39</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="AMD32" s="0"/>
+      <c r="AME32" s="0"/>
+      <c r="AMF32" s="0"/>
+      <c r="AMG32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="39" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="F33" s="41" t="s">
-        <v>291</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>292</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="AMD33" s="0"/>
+      <c r="AME33" s="0"/>
+      <c r="AMF33" s="0"/>
+      <c r="AMG33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="39" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B34" s="41" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>41</v>
+        <v>279</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G34" s="41" t="s">
-        <v>41</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="AMD34" s="0"/>
+      <c r="AME34" s="0"/>
+      <c r="AMF34" s="0"/>
+      <c r="AMG34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="39" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B35" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="41" t="s">
-        <v>41</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AMD35" s="0"/>
+      <c r="AME35" s="0"/>
+      <c r="AMF35" s="0"/>
+      <c r="AMG35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="39" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>294</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>294</v>
-      </c>
-      <c r="G36" s="43" t="s">
-        <v>295</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="AMD36" s="0"/>
+      <c r="AME36" s="0"/>
+      <c r="AMF36" s="0"/>
+      <c r="AMG36" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
working renewable constraint removed issues with case_definitions and unnamed columns added error and sys.exit when no cases analysed added error and sys.exit when optimizing minimal loaded generator
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="286">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -144,19 +144,19 @@
     <t xml:space="preserve">restore_oemof_if_existant</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
+    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">restore_blackouts_if_existant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
   </si>
   <si>
     <t xml:space="preserve">include_shortage_penalty_costs_in_lcoe</t>
   </si>
   <si>
     <t xml:space="preserve">allow_shortage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
   </si>
   <si>
     <t xml:space="preserve">evaluated_days</t>
@@ -711,13 +711,13 @@
     <t xml:space="preserve">title_demand_dc</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier4_DC</t>
+    <t xml:space="preserve">loc_1</t>
   </si>
   <si>
-    <t xml:space="preserve">T4_dc_year.csv</t>
+    <t xml:space="preserve">nesp_4108.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">power</t>
+    <t xml:space="preserve">Demand</t>
   </si>
   <si>
     <t xml:space="preserve">SolarGen</t>
@@ -726,46 +726,43 @@
     <t xml:space="preserve">Wind</t>
   </si>
   <si>
-    <t xml:space="preserve">GridAvailability</t>
+    <t xml:space="preserve">;</t>
   </si>
   <si>
-    <t xml:space="preserve">,</t>
+    <t xml:space="preserve">loc_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier4_AC</t>
+    <t xml:space="preserve">nesp_3513.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">T4_ac_year.csv</t>
+    <t xml:space="preserve">loc_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier4_AC_DC</t>
+    <t xml:space="preserve">nesp_3536.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">T4_ac_dc_year.csv</t>
+    <t xml:space="preserve">loc_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Demand AC</t>
+    <t xml:space="preserve">nesp_3724.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Demand DC</t>
+    <t xml:space="preserve">loc_5</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2_DC</t>
+    <t xml:space="preserve">nesp_4100.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">T2_dc_year.csv</t>
+    <t xml:space="preserve">loc_6</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2_AC</t>
+    <t xml:space="preserve">nesp_4655.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">T2_ac_year.csv</t>
+    <t xml:space="preserve">loc_7</t>
   </si>
   <si>
-    <t xml:space="preserve">Tier2_AC_DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T2_ac_dc_year.csv</t>
+    <t xml:space="preserve">nesp_4696.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Adding cases</t>
@@ -825,22 +822,7 @@
     <t xml:space="preserve">True or False or default</t>
   </si>
   <si>
-    <t xml:space="preserve">sole_maingrid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_battery_forced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_battery_foresight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backup_shs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parallel_shs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">offgrid_shs</t>
+    <t xml:space="preserve">mg</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -882,34 +864,25 @@
     <t xml:space="preserve">number_of_equal_generators</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
   </si>
   <si>
-    <t xml:space="preserve">peak_demand</t>
-  </si>
-  <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">0.02</t>
+    <t xml:space="preserve">share_hybrid</t>
   </si>
   <si>
     <t xml:space="preserve">evaluation_perspective</t>
   </si>
   <si>
     <t xml:space="preserve">AC_system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC_system</t>
   </si>
 </sst>
 </file>
@@ -1201,6 +1174,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1221,11 +1198,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1233,13 +1210,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1530,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1666,23 +1639,23 @@
         <v>40</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,7 +1663,7 @@
         <v>44</v>
       </c>
       <c r="C17" s="18" t="n">
-        <v>365</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1690,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1715,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1792,7 @@
         <v>65</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1800,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>67</v>
@@ -1838,7 +1811,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1819,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,7 +1827,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1835,7 @@
         <v>71</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1843,7 @@
         <v>72</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1861,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,7 +1869,7 @@
         <v>74</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,7 +1877,7 @@
         <v>75</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1894,7 @@
         <v>76</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1929,7 +1902,7 @@
         <v>77</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1937,7 +1910,7 @@
         <v>78</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1945,7 +1918,7 @@
         <v>79</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1975,8 +1948,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D78" activeCellId="0" sqref="D78"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2976,10 +2949,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3104,6 +3077,20 @@
       </c>
       <c r="D10" s="0" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -3131,10 +3118,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMI20"/>
+  <dimension ref="A1:AMI21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16548,12 +16535,8 @@
       <c r="I14" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="J14" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>100</v>
-      </c>
+      <c r="J14" s="33"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
@@ -16565,7 +16548,7 @@
       <c r="C15" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="34" t="s">
         <v>230</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -16577,30 +16560,24 @@
       <c r="G15" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I15" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J15" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K15" s="20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>235</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>236</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="34" t="s">
         <v>230</v>
       </c>
       <c r="E16" s="20" t="s">
@@ -16612,34 +16589,28 @@
       <c r="G16" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J16" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K16" s="20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>237</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>238</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>239</v>
+      <c r="D17" s="34" t="s">
+        <v>230</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>231</v>
@@ -16647,30 +16618,24 @@
       <c r="G17" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J17" s="20" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="K17" s="20" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="34" t="s">
         <v>230</v>
       </c>
       <c r="E18" s="20" t="s">
@@ -16682,30 +16647,24 @@
       <c r="G18" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J18" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K18" s="20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="34" t="s">
         <v>230</v>
       </c>
       <c r="E19" s="20" t="s">
@@ -16717,34 +16676,28 @@
       <c r="G19" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I19" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J19" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K19" s="20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>239</v>
+      <c r="D20" s="34" t="s">
+        <v>230</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="F20" s="20" t="s">
         <v>231</v>
@@ -16752,17 +16705,40 @@
       <c r="G20" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="I20" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="J20" s="20" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="K20" s="20" t="n">
-        <v>30</v>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -16793,10 +16769,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMG36"/>
+  <dimension ref="A1:AMG37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17833,7 +17809,7 @@
       <c r="AMG1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
@@ -18857,15 +18833,15 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>247</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>248</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
@@ -19883,14 +19859,14 @@
       <c r="AMG3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>249</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
@@ -20910,14 +20886,14 @@
       <c r="AMG4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -21937,14 +21913,14 @@
       <c r="AMG5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
@@ -22964,14 +22940,14 @@
       <c r="AMG6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
@@ -23991,14 +23967,14 @@
       <c r="AMG7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="A8" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
@@ -25018,14 +24994,14 @@
       <c r="AMG8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="A9" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
@@ -26045,14 +26021,14 @@
       <c r="AMG9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="A10" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
@@ -27072,14 +27048,14 @@
       <c r="AMG10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
+      <c r="A11" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
@@ -28099,14 +28075,14 @@
       <c r="AMG11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="G12" s="0"/>
@@ -29126,14 +29102,14 @@
       <c r="AMG12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
@@ -30153,14 +30129,14 @@
       <c r="AMG13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>264</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
@@ -32201,488 +32177,285 @@
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="110.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="s">
-        <v>249</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="F16" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>271</v>
-      </c>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="AMC16" s="0"/>
+      <c r="AMD16" s="0"/>
+      <c r="AME16" s="0"/>
+      <c r="AMF16" s="0"/>
+      <c r="AMG16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="s">
-        <v>272</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>39</v>
-      </c>
+      <c r="A17" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC17" s="0"/>
+      <c r="AMD17" s="0"/>
+      <c r="AME17" s="0"/>
+      <c r="AMF17" s="0"/>
+      <c r="AMG17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="s">
-        <v>251</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="A18" s="40" t="s">
+        <v>250</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="AMC18" s="0"/>
+      <c r="AMD18" s="0"/>
+      <c r="AME18" s="0"/>
+      <c r="AMF18" s="0"/>
+      <c r="AMG18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="F19" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="G19" s="41" t="s">
-        <v>274</v>
-      </c>
+      <c r="A19" s="40" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC19" s="0"/>
+      <c r="AMD19" s="0"/>
+      <c r="AME19" s="0"/>
+      <c r="AMF19" s="0"/>
+      <c r="AMG19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
-        <v>275</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>180</v>
-      </c>
+      <c r="A20" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC20" s="0"/>
+      <c r="AMD20" s="0"/>
+      <c r="AME20" s="0"/>
+      <c r="AMF20" s="0"/>
+      <c r="AMG20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="F21" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="G21" s="41" t="s">
-        <v>274</v>
-      </c>
+      <c r="A21" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC21" s="0"/>
+      <c r="AMD21" s="0"/>
+      <c r="AME21" s="0"/>
+      <c r="AMF21" s="0"/>
+      <c r="AMG21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="s">
-        <v>277</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="41" t="s">
+      <c r="A22" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="AMC22" s="0"/>
+      <c r="AMD22" s="0"/>
+      <c r="AME22" s="0"/>
+      <c r="AMF22" s="0"/>
+      <c r="AMG22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="A23" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="AMC23" s="0"/>
+      <c r="AMD23" s="0"/>
+      <c r="AME23" s="0"/>
+      <c r="AMF23" s="0"/>
+      <c r="AMG23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="D24" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="G24" s="41" t="s">
-        <v>274</v>
-      </c>
+      <c r="A24" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC24" s="0"/>
+      <c r="AMD24" s="0"/>
+      <c r="AME24" s="0"/>
+      <c r="AMF24" s="0"/>
+      <c r="AMG24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C25" s="41" t="s">
+      <c r="A25" s="40" t="s">
         <v>274</v>
       </c>
-      <c r="D25" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>274</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>274</v>
-      </c>
+      <c r="B25" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC25" s="0"/>
+      <c r="AMD25" s="0"/>
+      <c r="AME25" s="0"/>
+      <c r="AMF25" s="0"/>
+      <c r="AMG25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42" t="s">
-        <v>281</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="41" t="s">
+      <c r="A26" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="B26" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="AMC26" s="0"/>
+      <c r="AMD26" s="0"/>
+      <c r="AME26" s="0"/>
+      <c r="AMF26" s="0"/>
+      <c r="AMG26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="E27" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>180</v>
-      </c>
+      <c r="A27" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="AMC27" s="0"/>
+      <c r="AMD27" s="0"/>
+      <c r="AME27" s="0"/>
+      <c r="AMF27" s="0"/>
+      <c r="AMG27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42" t="s">
-        <v>283</v>
-      </c>
-      <c r="B28" s="41" t="s">
+      <c r="A28" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="B28" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="41" t="s">
-        <v>39</v>
-      </c>
+      <c r="AMC28" s="0"/>
+      <c r="AMD28" s="0"/>
+      <c r="AME28" s="0"/>
+      <c r="AMF28" s="0"/>
+      <c r="AMG28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42" t="s">
-        <v>284</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="E29" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="G29" s="41" t="s">
-        <v>285</v>
-      </c>
+      <c r="A29" s="43" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="AMC29" s="0"/>
+      <c r="AMD29" s="0"/>
+      <c r="AME29" s="0"/>
+      <c r="AMF29" s="0"/>
+      <c r="AMG29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39" t="s">
-        <v>286</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="D30" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="E30" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="F30" s="41" t="s">
-        <v>287</v>
-      </c>
-      <c r="G30" s="41" t="s">
+      <c r="A30" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="B30" s="42" t="s">
         <v>180</v>
       </c>
+      <c r="AMC30" s="0"/>
+      <c r="AMD30" s="0"/>
+      <c r="AME30" s="0"/>
+      <c r="AMF30" s="0"/>
+      <c r="AMG30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39" t="s">
-        <v>288</v>
-      </c>
-      <c r="B31" s="41" t="s">
+      <c r="A31" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B31" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="D31" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="41" t="s">
-        <v>180</v>
-      </c>
-      <c r="G31" s="41" t="s">
-        <v>180</v>
-      </c>
+      <c r="AMC31" s="0"/>
+      <c r="AMD31" s="0"/>
+      <c r="AME31" s="0"/>
+      <c r="AMF31" s="0"/>
+      <c r="AMG31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="41" t="s">
-        <v>39</v>
-      </c>
+      <c r="AMC32" s="0"/>
+      <c r="AMD32" s="0"/>
+      <c r="AME32" s="0"/>
+      <c r="AMF32" s="0"/>
+      <c r="AMG32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>289</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>290</v>
-      </c>
-      <c r="D33" s="41" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>290</v>
-      </c>
-      <c r="F33" s="41" t="s">
-        <v>290</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>291</v>
-      </c>
+      <c r="A33" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="AMC33" s="0"/>
+      <c r="AMD33" s="0"/>
+      <c r="AME33" s="0"/>
+      <c r="AMF33" s="0"/>
+      <c r="AMG33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G34" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="A34" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="AMC34" s="0"/>
+      <c r="AMD34" s="0"/>
+      <c r="AME34" s="0"/>
+      <c r="AMF34" s="0"/>
+      <c r="AMG34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39" t="s">
-        <v>264</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="G35" s="41" t="s">
-        <v>41</v>
-      </c>
+      <c r="A35" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="AMC35" s="0"/>
+      <c r="AMD35" s="0"/>
+      <c r="AME35" s="0"/>
+      <c r="AMF35" s="0"/>
+      <c r="AMG35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
-        <v>292</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="D36" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="E36" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="G36" s="43" t="s">
-        <v>294</v>
-      </c>
+      <c r="A36" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="AMC36" s="0"/>
+      <c r="AMD36" s="0"/>
+      <c r="AME36" s="0"/>
+      <c r="AMF36" s="0"/>
+      <c r="AMG36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMC37" s="0"/>
+      <c r="AMD37" s="0"/>
+      <c r="AME37" s="0"/>
+      <c r="AMF37" s="0"/>
+      <c r="AMG37" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
readme.md new release (minor)
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="274">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -729,42 +729,6 @@
     <t xml:space="preserve">;</t>
   </si>
   <si>
-    <t xml:space="preserve">loc_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_3513.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_3536.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_3724.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_4100.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_4655.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc_7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nesp_4696.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adding cases</t>
   </si>
   <si>
@@ -1294,7 +1258,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A16:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1504,7 +1468,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="A16:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1948,8 +1912,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="A16:I22 B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2952,7 +2916,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="A16:I22 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3120,8 +3084,8 @@
   </sheetPr>
   <dimension ref="A1:AMI21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16568,178 +16532,28 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D16" s="34"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D17" s="34"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D18" s="34"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D19" s="34"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D20" s="34"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>180</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="D21" s="34"/>
+      <c r="H21" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -16772,7 +16586,7 @@
   <dimension ref="A1:AMG37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="A16:I22 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18833,10 +18647,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -19860,10 +19674,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -20887,10 +20701,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -21914,10 +21728,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -22941,10 +22755,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -23968,10 +23782,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -24995,10 +24809,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -26022,10 +25836,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -27052,7 +26866,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -28076,10 +27890,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -29103,10 +28917,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -30130,10 +29944,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -32179,10 +31993,10 @@
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
@@ -32192,7 +32006,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>43</v>
@@ -32205,7 +32019,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>39</v>
@@ -32218,10 +32032,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC19" s="0"/>
       <c r="AMD19" s="0"/>
@@ -32231,10 +32045,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC20" s="0"/>
       <c r="AMD20" s="0"/>
@@ -32244,10 +32058,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
@@ -32257,7 +32071,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="43" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B22" s="42" t="s">
         <v>39</v>
@@ -32270,7 +32084,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="43" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="B23" s="42" t="s">
         <v>39</v>
@@ -32283,10 +32097,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC24" s="0"/>
       <c r="AMD24" s="0"/>
@@ -32296,10 +32110,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC25" s="0"/>
       <c r="AMD25" s="0"/>
@@ -32309,7 +32123,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="43" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B26" s="42" t="s">
         <v>39</v>
@@ -32322,10 +32136,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AMC27" s="0"/>
       <c r="AMD27" s="0"/>
@@ -32335,7 +32149,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="43" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B28" s="42" t="s">
         <v>39</v>
@@ -32348,10 +32162,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="43" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="AMC29" s="0"/>
       <c r="AMD29" s="0"/>
@@ -32361,7 +32175,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>180</v>
@@ -32374,7 +32188,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>180</v>
@@ -32400,10 +32214,10 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="40" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="AMC33" s="0"/>
       <c r="AMD33" s="0"/>
@@ -32413,10 +32227,10 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="AMC34" s="0"/>
       <c r="AMD34" s="0"/>
@@ -32426,7 +32240,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>43</v>
@@ -32439,10 +32253,10 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="AMC36" s="0"/>
       <c r="AMD36" s="0"/>

</xml_diff>

<commit_message>
Include test for missing input data (especially by version switch) and add generic values
</commit_message>
<xml_diff>
--- a/inputs/input_template_excel.xlsx
+++ b/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="276">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -606,9 +606,6 @@
     <t xml:space="preserve">wind_cost_var</t>
   </si>
   <si>
-    <t xml:space="preserve">wind_lifetime</t>
-  </si>
-  <si>
     <t xml:space="preserve">Definition of sensitivity parameters</t>
   </si>
   <si>
@@ -786,7 +783,13 @@
     <t xml:space="preserve">True or False or default</t>
   </si>
   <si>
-    <t xml:space="preserve">mg</t>
+    <t xml:space="preserve">mg_on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_res_charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg_off</t>
   </si>
   <si>
     <t xml:space="preserve">perform_simulation</t>
@@ -832,6 +835,9 @@
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_consumption_kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peak_demand</t>
   </si>
   <si>
     <t xml:space="preserve">capacity_pcc_feedin_kW</t>
@@ -1258,7 +1264,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A16:I22"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="A88:C88 A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1467,8 +1473,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="A16:I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="A88:C88 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1912,8 +1918,8 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="1" sqref="A16:I22 B52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A88" activeCellId="0" sqref="A88:C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1988,7 +1994,7 @@
         <v>88</v>
       </c>
       <c r="B7" s="18" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>89</v>
@@ -1999,7 +2005,7 @@
         <v>90</v>
       </c>
       <c r="B8" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>91</v>
@@ -2010,7 +2016,7 @@
         <v>92</v>
       </c>
       <c r="B9" s="18" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>93</v>
@@ -2021,7 +2027,7 @@
         <v>94</v>
       </c>
       <c r="B10" s="18" t="n">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>91</v>
@@ -2883,15 +2889,8 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B88" s="18" t="n">
-        <v>20</v>
-      </c>
-      <c r="C88" s="15" t="s">
-        <v>105</v>
-      </c>
+      <c r="B88" s="18"/>
+      <c r="C88" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2913,10 +2912,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="A16:I22 D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="1" sqref="A88:C88 E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2931,7 +2930,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="15"/>
@@ -2947,10 +2946,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>195</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>196</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -2976,7 +2975,7 @@
         <v>85</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -2986,10 +2985,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2999,10 +2998,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -3012,10 +3011,10 @@
     </row>
     <row r="8" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>202</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>203</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -3034,27 +3033,13 @@
         <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20" t="n">
-        <v>0.1</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3084,8 +3069,8 @@
   </sheetPr>
   <dimension ref="A1:AMI21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16:I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="A88:C88 A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3106,7 +3091,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
@@ -5158,10 +5143,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>205</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>206</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -6187,10 +6172,10 @@
     </row>
     <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>207</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>208</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -7216,10 +7201,10 @@
     </row>
     <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>209</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>210</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -8245,10 +8230,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>211</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>212</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -9274,10 +9259,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>214</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -10303,10 +10288,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>215</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>216</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -11332,10 +11317,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>218</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -12361,10 +12346,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>220</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -13390,10 +13375,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>221</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>222</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -14419,10 +14404,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>223</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>224</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -16473,62 +16458,62 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>227</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J14" s="33"/>
       <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>229</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>180</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>180</v>
       </c>
       <c r="F15" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>231</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>232</v>
       </c>
       <c r="H15" s="35" t="s">
         <v>180</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16586,7 +16571,7 @@
   <dimension ref="A1:AMG37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="1" sqref="A16:I22 B30"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="A88:C88 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18647,10 +18632,10 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>234</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>235</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -19674,10 +19659,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="38" t="s">
         <v>236</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>237</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -20701,10 +20686,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="38" t="s">
         <v>238</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>239</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -21728,10 +21713,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="38" t="s">
         <v>240</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>241</v>
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
@@ -22755,10 +22740,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
@@ -23782,10 +23767,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
@@ -24809,10 +24794,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
@@ -25836,10 +25821,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -26866,7 +26851,7 @@
         <v>42</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
@@ -27890,10 +27875,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="38" t="s">
         <v>247</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>248</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -28917,10 +28902,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="B13" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>250</v>
       </c>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -29944,10 +29929,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>251</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>252</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -31991,12 +31976,18 @@
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="67.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B16" s="41" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>253</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>254</v>
       </c>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
@@ -32006,9 +31997,15 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="40" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B17" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="42" t="s">
         <v>43</v>
       </c>
       <c r="AMC17" s="0"/>
@@ -32019,9 +32016,15 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B18" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="42" t="s">
         <v>39</v>
       </c>
       <c r="AMC18" s="0"/>
@@ -32032,10 +32035,16 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="40" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>257</v>
       </c>
       <c r="AMC19" s="0"/>
       <c r="AMD19" s="0"/>
@@ -32045,10 +32054,16 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="40" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>256</v>
+        <v>180</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="AMC20" s="0"/>
       <c r="AMD20" s="0"/>
@@ -32058,10 +32073,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>257</v>
       </c>
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
@@ -32071,9 +32092,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="43" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B22" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="42" t="s">
         <v>39</v>
       </c>
       <c r="AMC22" s="0"/>
@@ -32084,9 +32111,15 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="43" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B23" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="42" t="s">
         <v>39</v>
       </c>
       <c r="AMC23" s="0"/>
@@ -32097,10 +32130,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="40" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>256</v>
+        <v>180</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>180</v>
       </c>
       <c r="AMC24" s="0"/>
       <c r="AMD24" s="0"/>
@@ -32110,10 +32149,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="40" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>257</v>
       </c>
       <c r="AMC25" s="0"/>
       <c r="AMD25" s="0"/>
@@ -32123,9 +32168,15 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="43" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B26" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="42" t="s">
         <v>39</v>
       </c>
       <c r="AMC26" s="0"/>
@@ -32136,10 +32187,16 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="40" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>257</v>
       </c>
       <c r="AMC27" s="0"/>
       <c r="AMD27" s="0"/>
@@ -32149,9 +32206,15 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="43" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B28" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="42" t="s">
         <v>39</v>
       </c>
       <c r="AMC28" s="0"/>
@@ -32162,10 +32225,16 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="43" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>268</v>
       </c>
       <c r="AMC29" s="0"/>
       <c r="AMD29" s="0"/>
@@ -32175,9 +32244,15 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B30" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>180</v>
       </c>
       <c r="AMC30" s="0"/>
@@ -32188,9 +32263,15 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="40" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B31" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D31" s="42" t="s">
         <v>180</v>
       </c>
       <c r="AMC31" s="0"/>
@@ -32206,6 +32287,12 @@
       <c r="B32" s="42" t="s">
         <v>43</v>
       </c>
+      <c r="C32" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>43</v>
+      </c>
       <c r="AMC32" s="0"/>
       <c r="AMD32" s="0"/>
       <c r="AME32" s="0"/>
@@ -32214,10 +32301,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>270</v>
+        <v>272</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="D33" s="42" t="s">
+        <v>272</v>
       </c>
       <c r="AMC33" s="0"/>
       <c r="AMD33" s="0"/>
@@ -32227,10 +32320,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>271</v>
+        <v>273</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>273</v>
       </c>
       <c r="AMC34" s="0"/>
       <c r="AMD34" s="0"/>
@@ -32240,10 +32339,16 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="AMC35" s="0"/>
       <c r="AMD35" s="0"/>
@@ -32253,10 +32358,16 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="40" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>273</v>
+        <v>275</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>275</v>
       </c>
       <c r="AMC36" s="0"/>
       <c r="AMD36" s="0"/>

</xml_diff>